<commit_message>
first consistent model for a single tier
</commit_message>
<xml_diff>
--- a/model/RunControl.xlsx
+++ b/model/RunControl.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4623D4A5-6E14-445E-885C-09EAE3A956A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9034216E-8251-485F-8062-D9D73437E7CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="524" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params_sim" sheetId="22" r:id="rId1"/>
@@ -14,6 +14,8 @@
     <sheet name="params_byTier" sheetId="19" r:id="rId4"/>
     <sheet name="returns" sheetId="2" r:id="rId5"/>
     <sheet name="targetVals_2018" sheetId="20" r:id="rId6"/>
+    <sheet name="targeVals_raw" sheetId="23" r:id="rId7"/>
+    <sheet name="shares" sheetId="24" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,10 +38,9 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
-    <author>tc={A81602AF-0C15-4BB8-A273-D046D350C354}</author>
   </authors>
   <commentList>
-    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{CDE40F89-78CF-4C3B-B38C-D04825AF5F6F}">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{CDE40F89-78CF-4C3B-B38C-D04825AF5F6F}">
       <text>
         <r>
           <rPr>
@@ -63,15 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K4" authorId="1" shapeId="0" xr:uid="{A81602AF-0C15-4BB8-A273-D046D350C354}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Check AV assumption</t>
-      </text>
-    </comment>
-    <comment ref="V4" authorId="0" shapeId="0" xr:uid="{568404F5-400A-46EF-8AA1-93D4C44E460E}">
+    <comment ref="N4" authorId="0" shapeId="0" xr:uid="{568404F5-400A-46EF-8AA1-93D4C44E460E}">
       <text>
         <r>
           <rPr>
@@ -96,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG4" authorId="0" shapeId="0" xr:uid="{148CF5FB-6519-420B-97E2-DCE9E3F8AE4C}">
+    <comment ref="X4" authorId="0" shapeId="0" xr:uid="{148CF5FB-6519-420B-97E2-DCE9E3F8AE4C}">
       <text>
         <r>
           <rPr>
@@ -159,10 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="203">
-  <si>
-    <t>runname</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="219">
   <si>
     <t>nsim</t>
   </si>
@@ -275,9 +265,6 @@
     <t>cd</t>
   </si>
   <si>
-    <t>cola</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
@@ -305,18 +292,6 @@
     <t>min_retAge</t>
   </si>
   <si>
-    <t>fasyears</t>
-  </si>
-  <si>
-    <t>benefit parameters</t>
-  </si>
-  <si>
-    <t>age_vben</t>
-  </si>
-  <si>
-    <t>v.year</t>
-  </si>
-  <si>
     <t>Return Assumptions</t>
   </si>
   <si>
@@ -356,9 +331,6 @@
     <t>init_AA_type</t>
   </si>
   <si>
-    <t>workforce</t>
-  </si>
-  <si>
     <t>estInitTerm</t>
   </si>
   <si>
@@ -368,9 +340,6 @@
     <t>startingSalgrowth</t>
   </si>
   <si>
-    <t>no_entrants</t>
-  </si>
-  <si>
     <t>2017-2018</t>
   </si>
   <si>
@@ -425,12 +394,6 @@
     <t>Tiers</t>
   </si>
   <si>
-    <t>tier_Mode</t>
-  </si>
-  <si>
-    <t>singleTier_select</t>
-  </si>
-  <si>
     <t>PVFB_disbRet</t>
   </si>
   <si>
@@ -443,42 +406,9 @@
     <t>simple</t>
   </si>
   <si>
-    <t>nt6</t>
-  </si>
-  <si>
     <t>singleTier</t>
   </si>
   <si>
-    <t>sal_dist</t>
-  </si>
-  <si>
-    <t>Dev_singleTier</t>
-  </si>
-  <si>
-    <t>multiTier</t>
-  </si>
-  <si>
-    <t>NMR</t>
-  </si>
-  <si>
-    <t>Cost Method</t>
-  </si>
-  <si>
-    <t>cost_method</t>
-  </si>
-  <si>
-    <t>EAN</t>
-  </si>
-  <si>
-    <t>Dev_multiTier_AGG</t>
-  </si>
-  <si>
-    <t>Dev_multiTier_EAN</t>
-  </si>
-  <si>
-    <t>AGG</t>
-  </si>
-  <si>
     <t>Source: NYSERS_targets.xlsx Sheet "Analysis_targets_byTier"</t>
   </si>
   <si>
@@ -768,13 +698,124 @@
   </si>
   <si>
     <t>tier_include</t>
+  </si>
+  <si>
+    <t>Dev</t>
+  </si>
+  <si>
+    <t>valuation</t>
+  </si>
+  <si>
+    <t>run_val</t>
+  </si>
+  <si>
+    <t>sim_name</t>
+  </si>
+  <si>
+    <t>Values on June 30, 2018</t>
+  </si>
+  <si>
+    <t>misc</t>
+  </si>
+  <si>
+    <t>inds</t>
+  </si>
+  <si>
+    <t>misc+inds</t>
+  </si>
+  <si>
+    <t>Members</t>
+  </si>
+  <si>
+    <t>Funded status</t>
+  </si>
+  <si>
+    <t>Employer contribution</t>
+  </si>
+  <si>
+    <t>Active Members</t>
+  </si>
+  <si>
+    <t>Transfers from State Miscellaneous</t>
+  </si>
+  <si>
+    <t>Vested Terminations2</t>
+  </si>
+  <si>
+    <t>Receiving Payments</t>
+  </si>
+  <si>
+    <t>Present Value of Benefits</t>
+  </si>
+  <si>
+    <t>Accrued Liability</t>
+  </si>
+  <si>
+    <t>Market Value of Assets</t>
+  </si>
+  <si>
+    <t>Unfunded Liability/(Surplus)</t>
+  </si>
+  <si>
+    <t>Funded Status</t>
+  </si>
+  <si>
+    <t>Covered Payroll in Fiscal Year Ending on Valuation Date</t>
+  </si>
+  <si>
+    <t>Projected Payroll for Contribution Rate</t>
+  </si>
+  <si>
+    <t>Total Normal Cost</t>
+  </si>
+  <si>
+    <t>Employee Contribution</t>
+  </si>
+  <si>
+    <t>Employer Normal Costs</t>
+  </si>
+  <si>
+    <t>Amortization of Unfunded Liability</t>
+  </si>
+  <si>
+    <t>Contribution required (% proj payroll)</t>
+  </si>
+  <si>
+    <t>Contribution required (% current payroll)</t>
+  </si>
+  <si>
+    <t>misc t1</t>
+  </si>
+  <si>
+    <t>misc t2</t>
+  </si>
+  <si>
+    <t>inds t1</t>
+  </si>
+  <si>
+    <t>inds t2</t>
+  </si>
+  <si>
+    <t>actives</t>
+  </si>
+  <si>
+    <t>retirees</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>discount rate</t>
+  </si>
+  <si>
+    <t>seed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
@@ -782,8 +823,9 @@
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
     <numFmt numFmtId="170" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="172" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -846,8 +888,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -857,12 +924,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -908,14 +969,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1018,6 +1073,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1031,7 +1095,7 @@
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1050,23 +1114,19 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1087,6 +1147,31 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1489,23 +1574,15 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="K4" dT="2020-02-17T21:37:27.59" personId="{00000000-0000-0000-0000-000000000000}" id="{A81602AF-0C15-4BB8-A273-D046D350C354}">
-    <text>Check AV assumption</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D014B46A-D012-4D18-AEAB-1D829080B2CE}">
-  <dimension ref="A1:AS7"/>
+  <dimension ref="A1:AJ5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="I26" sqref="I26"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1513,663 +1590,320 @@
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" customWidth="1"/>
-    <col min="10" max="12" width="14.140625" customWidth="1"/>
-    <col min="13" max="14" width="19.7109375" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.85546875" customWidth="1"/>
-    <col min="18" max="18" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.7109375" customWidth="1"/>
-    <col min="24" max="24" width="14" customWidth="1"/>
-    <col min="25" max="25" width="13.42578125" customWidth="1"/>
-    <col min="26" max="26" width="12.5703125" customWidth="1"/>
-    <col min="27" max="27" width="14.85546875" customWidth="1"/>
-    <col min="32" max="32" width="12" customWidth="1"/>
-    <col min="33" max="33" width="13.7109375" customWidth="1"/>
-    <col min="34" max="34" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="7.85546875" customWidth="1"/>
-    <col min="38" max="38" width="12.7109375" customWidth="1"/>
-    <col min="39" max="39" width="16.5703125" customWidth="1"/>
-    <col min="40" max="40" width="12" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="18" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.28515625" customWidth="1"/>
-    <col min="44" max="44" width="11.42578125" customWidth="1"/>
-    <col min="45" max="45" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" customWidth="1"/>
+    <col min="23" max="23" width="12" customWidth="1"/>
+    <col min="24" max="24" width="13.7109375" customWidth="1"/>
+    <col min="25" max="25" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="7.85546875" customWidth="1"/>
+    <col min="29" max="29" width="12.7109375" customWidth="1"/>
+    <col min="30" max="30" width="16.5703125" customWidth="1"/>
+    <col min="31" max="31" width="12" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.28515625" customWidth="1"/>
+    <col min="35" max="35" width="11.42578125" customWidth="1"/>
+    <col min="36" max="36" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="AH1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="AH2" s="26">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="Y1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="Y2" s="24">
         <f>179995000/184504000</f>
         <v>0.97556150544161646</v>
       </c>
-      <c r="AI2" s="26">
+      <c r="Z2" s="24">
         <f>175430000/184504000</f>
         <v>0.95081949442830505</v>
       </c>
     </row>
-    <row r="3" spans="1:45" s="23" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>49</v>
-      </c>
+    <row r="3" spans="1:36" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="F3" s="19"/>
+      <c r="G3" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
       <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="17" t="s">
-        <v>55</v>
-      </c>
+      <c r="K3" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
       <c r="N3" s="17"/>
-      <c r="O3" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="19" t="s">
-        <v>57</v>
-      </c>
+      <c r="O3" s="17"/>
+      <c r="P3" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
       <c r="T3" s="19"/>
       <c r="U3" s="19"/>
       <c r="V3" s="19"/>
-      <c r="W3" s="19"/>
-      <c r="X3" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y3" s="20"/>
-      <c r="Z3" s="21" t="s">
+      <c r="W3" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="X3" s="15"/>
+      <c r="Y3" s="15"/>
+      <c r="Z3" s="15"/>
+      <c r="AA3" s="15"/>
+      <c r="AB3" s="15"/>
+      <c r="AC3" s="15"/>
+      <c r="AD3" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE3" s="20"/>
+      <c r="AF3" s="20"/>
+      <c r="AG3" s="20"/>
+      <c r="AH3" s="20"/>
+      <c r="AI3" s="20"/>
+      <c r="AJ3" s="20"/>
+    </row>
+    <row r="4" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="AA3" s="21"/>
-      <c r="AB3" s="21"/>
-      <c r="AC3" s="21"/>
-      <c r="AD3" s="21"/>
-      <c r="AE3" s="21"/>
-      <c r="AF3" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG3" s="17"/>
-      <c r="AH3" s="17"/>
-      <c r="AI3" s="17"/>
-      <c r="AJ3" s="17"/>
-      <c r="AK3" s="17"/>
-      <c r="AL3" s="17"/>
-      <c r="AM3" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="AN3" s="22"/>
-      <c r="AO3" s="22"/>
-      <c r="AP3" s="22"/>
-      <c r="AQ3" s="22"/>
-      <c r="AR3" s="22"/>
-      <c r="AS3" s="22"/>
-    </row>
-    <row r="4" spans="1:45" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="H4" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>51</v>
-      </c>
       <c r="M4" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="N4" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="O4" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="P4" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="R4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="S4" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="T4" s="10" t="s">
+      <c r="O4" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="W4" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="X4" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="U4" s="10" t="s">
+      <c r="Y4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC4" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD4" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="V4" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="W4" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="X4" s="14" t="s">
+      <c r="AE4" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="Y4" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE4" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF4" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG4" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="AH4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK4" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="AL4" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="AM4" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="AN4" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="AO4" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AP4" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="AQ4" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="AR4" s="13" t="s">
+      <c r="AH4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="AS4" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>182</v>
       </c>
       <c r="C5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>99</v>
-      </c>
-      <c r="F5" t="s">
-        <v>95</v>
+        <v>175</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>94</v>
+        <v>36</v>
       </c>
       <c r="H5" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
       <c r="I5">
+        <v>20</v>
+      </c>
+      <c r="J5">
+        <v>2.75E-2</v>
+      </c>
+      <c r="K5">
+        <v>5</v>
+      </c>
+      <c r="L5">
+        <v>999</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5" t="s">
+        <v>55</v>
+      </c>
+      <c r="O5" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>20</v>
+      </c>
+      <c r="R5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S5">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="T5" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="U5" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="V5" s="57">
+        <v>123</v>
+      </c>
+      <c r="W5" t="s">
+        <v>31</v>
+      </c>
+      <c r="X5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y5" s="24">
+        <v>0.6976</v>
+      </c>
+      <c r="Z5" s="24">
+        <v>0.6976</v>
+      </c>
+      <c r="AC5" s="44">
+        <v>0</v>
+      </c>
+      <c r="AD5" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE5" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5" t="s">
         <v>3</v>
       </c>
-      <c r="J5">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="K5">
-        <v>55</v>
-      </c>
-      <c r="L5">
-        <v>5</v>
-      </c>
-      <c r="M5" t="s">
-        <v>86</v>
-      </c>
-      <c r="N5">
-        <v>0.03</v>
-      </c>
-      <c r="O5" t="s">
-        <v>37</v>
-      </c>
-      <c r="P5" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q5">
-        <v>15</v>
-      </c>
-      <c r="R5">
-        <v>0.03</v>
-      </c>
-      <c r="S5">
-        <v>5</v>
-      </c>
-      <c r="T5">
-        <v>999</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5" t="s">
-        <v>61</v>
-      </c>
-      <c r="W5" t="b">
-        <v>0</v>
-      </c>
-      <c r="X5">
-        <v>0.01</v>
-      </c>
-      <c r="Y5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>93</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB5">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="AC5">
-        <v>7.7200000000000005E-2</v>
-      </c>
-      <c r="AD5" s="3">
-        <v>0.12</v>
-      </c>
-      <c r="AE5" s="5">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH5" s="26">
-        <v>0.99462395886975496</v>
-      </c>
-      <c r="AI5" s="26">
-        <v>0.96988052819607695</v>
-      </c>
-      <c r="AL5" s="48">
-        <v>3517847922</v>
-      </c>
-      <c r="AM5" t="b">
+      <c r="AI5" t="b">
         <v>1</v>
       </c>
-      <c r="AN5" t="b">
+      <c r="AJ5" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="AO5" t="b">
-        <v>1</v>
-      </c>
-      <c r="AP5">
-        <v>0</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>4</v>
-      </c>
-      <c r="AR5" t="b">
-        <v>1</v>
-      </c>
-      <c r="AS5" s="24" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G6" t="s">
-        <v>94</v>
-      </c>
-      <c r="H6" t="s">
-        <v>102</v>
-      </c>
-      <c r="I6">
-        <v>3</v>
-      </c>
-      <c r="J6">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="K6">
-        <v>55</v>
-      </c>
-      <c r="L6">
-        <v>5</v>
-      </c>
-      <c r="M6" t="s">
-        <v>86</v>
-      </c>
-      <c r="N6">
-        <v>0.03</v>
-      </c>
-      <c r="O6" t="s">
-        <v>37</v>
-      </c>
-      <c r="P6" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q6">
-        <v>15</v>
-      </c>
-      <c r="R6">
-        <v>0.03</v>
-      </c>
-      <c r="S6">
-        <v>5</v>
-      </c>
-      <c r="T6">
-        <v>999</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6" t="s">
-        <v>61</v>
-      </c>
-      <c r="W6" t="b">
-        <v>0</v>
-      </c>
-      <c r="X6">
-        <v>0.01</v>
-      </c>
-      <c r="Y6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>93</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB6">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="AC6">
-        <v>7.7200000000000005E-2</v>
-      </c>
-      <c r="AD6" s="3">
-        <v>0.12</v>
-      </c>
-      <c r="AE6" s="5">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH6" s="26">
-        <v>0.99462395886975508</v>
-      </c>
-      <c r="AI6" s="26">
-        <v>0.96988052819607673</v>
-      </c>
-      <c r="AL6" s="48">
-        <v>3517847922</v>
-      </c>
-      <c r="AM6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AO6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AP6">
-        <v>0</v>
-      </c>
-      <c r="AQ6" t="s">
-        <v>4</v>
-      </c>
-      <c r="AR6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AS6" s="24" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F7" t="s">
-        <v>98</v>
-      </c>
-      <c r="G7" t="s">
-        <v>94</v>
-      </c>
-      <c r="H7" t="s">
-        <v>105</v>
-      </c>
-      <c r="I7">
-        <v>3</v>
-      </c>
-      <c r="J7">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="K7">
-        <v>55</v>
-      </c>
-      <c r="L7">
-        <v>5</v>
-      </c>
-      <c r="M7" t="s">
-        <v>86</v>
-      </c>
-      <c r="N7">
-        <v>0.03</v>
-      </c>
-      <c r="O7" t="s">
-        <v>37</v>
-      </c>
-      <c r="P7" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q7">
-        <v>15</v>
-      </c>
-      <c r="R7">
-        <v>0.03</v>
-      </c>
-      <c r="S7">
-        <v>5</v>
-      </c>
-      <c r="T7">
-        <v>999</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-      <c r="V7" t="s">
-        <v>61</v>
-      </c>
-      <c r="W7" t="b">
-        <v>0</v>
-      </c>
-      <c r="X7">
-        <v>0.01</v>
-      </c>
-      <c r="Y7" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>93</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB7">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="AC7">
-        <v>7.7200000000000005E-2</v>
-      </c>
-      <c r="AD7" s="3">
-        <v>0.12</v>
-      </c>
-      <c r="AE7" s="5">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH7" s="26">
-        <v>0.99462395886975508</v>
-      </c>
-      <c r="AI7" s="26">
-        <v>0.96988052819607673</v>
-      </c>
-      <c r="AL7" s="48">
-        <v>3517847922</v>
-      </c>
-      <c r="AM7" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN7" t="b">
-        <v>1</v>
-      </c>
-      <c r="AO7" t="b">
-        <v>1</v>
-      </c>
-      <c r="AP7">
-        <v>0</v>
-      </c>
-      <c r="AQ7" t="s">
-        <v>4</v>
-      </c>
-      <c r="AR7" t="b">
-        <v>1</v>
-      </c>
-      <c r="AS7" s="24" t="b">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN5:AO7 C5:C7" xr:uid="{1240F49A-5091-456D-B77A-0673AD56E758}">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE5:AF5 C5" xr:uid="{1240F49A-5091-456D-B77A-0673AD56E758}">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z5:Z7" xr:uid="{8909875A-86FC-4594-BBAF-A364A5851F3C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P5" xr:uid="{8909875A-86FC-4594-BBAF-A364A5851F3C}">
       <formula1>"simple, internal"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F7" xr:uid="{74315FAD-C45A-4DC3-BA52-2C9420B1E53C}">
-      <formula1>"singleTier,multiTier"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E7" xr:uid="{FE99E520-5245-4606-89B9-5B3E4C28457B}">
-      <formula1>"flat,NMR"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D7" xr:uid="{EC327A6A-3FD9-4228-86E6-BF4DFCBDFAEB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5" xr:uid="{EC327A6A-3FD9-4228-86E6-BF4DFCBDFAEB}">
       <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H7" xr:uid="{D412AB2C-441D-4DD0-A524-39422CB58EC7}">
-      <formula1>"EAN,AGG"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2180,13 +1914,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62142380-6405-410A-A4D9-17F48F5CE536}">
-  <dimension ref="A3:I5"/>
+  <dimension ref="A3:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2201,67 +1935,73 @@
     <col min="8" max="9" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" s="23" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="20" t="s">
-        <v>198</v>
-      </c>
-      <c r="I3" s="20"/>
-    </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="19"/>
+      <c r="F3" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="I3" s="18"/>
+      <c r="J3" s="21" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="E5" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="F5" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G5">
         <v>2.75E-2</v>
@@ -2271,6 +2011,9 @@
       </c>
       <c r="I5" t="b">
         <v>1</v>
+      </c>
+      <c r="J5">
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2293,7 +2036,7 @@
   <dimension ref="A3:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2305,34 +2048,34 @@
   <sheetData>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="I3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2406,30 +2149,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="4">
         <v>0.128</v>
@@ -2449,12 +2192,12 @@
         <v>0.128</v>
       </c>
       <c r="G2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="4">
         <v>0.02</v>
@@ -2473,12 +2216,12 @@
         <v>0.02</v>
       </c>
       <c r="G3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="4">
         <v>7.7200000000000005E-2</v>
@@ -2498,12 +2241,12 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B5" s="4">
         <v>0.128</v>
@@ -2523,12 +2266,12 @@
         <v>0.128</v>
       </c>
       <c r="G5" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B6" s="4">
         <v>0.02</v>
@@ -2547,12 +2290,12 @@
         <v>0.02</v>
       </c>
       <c r="G6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B7" s="4">
         <v>5.7200000000000001E-2</v>
@@ -2572,12 +2315,12 @@
         <v>0.05</v>
       </c>
       <c r="G7" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B8" s="4">
         <v>7.22E-2</v>
@@ -2597,12 +2340,12 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="G8" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B9" s="4">
         <v>7.7200000000000005E-2</v>
@@ -2622,12 +2365,12 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G9" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B10" s="4">
         <v>0.128</v>
@@ -2647,12 +2390,12 @@
         <v>0.128</v>
       </c>
       <c r="G10" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B11" s="4">
         <v>0.02</v>
@@ -2671,12 +2414,12 @@
         <v>0.02</v>
       </c>
       <c r="G11" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B12" s="4">
         <v>5.7200000000000001E-2</v>
@@ -2696,12 +2439,12 @@
         <v>0.05</v>
       </c>
       <c r="G12" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B13" s="4">
         <v>7.22E-2</v>
@@ -2721,12 +2464,12 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="G13" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B14" s="4">
         <v>0.128</v>
@@ -2746,12 +2489,12 @@
         <v>0.128</v>
       </c>
       <c r="G14" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B15" s="4">
         <v>0.02</v>
@@ -2770,12 +2513,12 @@
         <v>0.02</v>
       </c>
       <c r="G15" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B16" s="4">
         <v>-0.24</v>
@@ -2795,12 +2538,12 @@
         <v>-0.24</v>
       </c>
       <c r="G16" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B17" s="4">
         <v>0.12</v>
@@ -2820,12 +2563,12 @@
         <v>0.12</v>
       </c>
       <c r="G17" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B18" s="4">
         <v>0.13</v>
@@ -2845,12 +2588,12 @@
         <v>0.13</v>
       </c>
       <c r="G18" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B19" s="4">
         <v>0.11</v>
@@ -2870,12 +2613,12 @@
         <v>0.11</v>
       </c>
       <c r="G19" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B20" s="4">
         <v>0.05</v>
@@ -2895,12 +2638,12 @@
         <v>0.05</v>
       </c>
       <c r="G20" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B21" s="4">
         <v>0.128</v>
@@ -2920,12 +2663,12 @@
         <v>0.128</v>
       </c>
       <c r="G21" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B22" s="4">
         <v>0.02</v>
@@ -2944,12 +2687,12 @@
         <v>0.02</v>
       </c>
       <c r="G22" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B23" s="4">
         <v>-0.24</v>
@@ -2969,12 +2712,12 @@
         <v>-0.24</v>
       </c>
       <c r="G23" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B24" s="4">
         <v>0.12</v>
@@ -2994,12 +2737,12 @@
         <v>0.12</v>
       </c>
       <c r="G24" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B25" s="4">
         <v>0.13</v>
@@ -3019,12 +2762,12 @@
         <v>0.13</v>
       </c>
       <c r="G25" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B26" s="4">
         <v>0.11</v>
@@ -3044,12 +2787,12 @@
         <v>0.11</v>
       </c>
       <c r="G26" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B27" s="4">
         <v>7.0000000000000007E-2</v>
@@ -3069,7 +2812,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G27" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -3082,830 +2825,830 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE0D02CC-7CA6-4318-9258-0FC7F2A32ECB}">
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" style="39" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" style="35" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" customWidth="1"/>
     <col min="5" max="5" width="40.28515625" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" customWidth="1"/>
     <col min="9" max="9" width="44.85546875" customWidth="1"/>
-    <col min="10" max="12" width="21.42578125" style="29" customWidth="1"/>
+    <col min="10" max="12" width="21.42578125" style="25" customWidth="1"/>
     <col min="13" max="13" width="43.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
-        <v>184</v>
+      <c r="A1" s="42" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="K3" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="L3" s="33" t="s">
-        <v>123</v>
-      </c>
-      <c r="M3" s="34"/>
+        <v>85</v>
+      </c>
+      <c r="I3" s="28"/>
+      <c r="J3" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="K3" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="L3" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="M3" s="30"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="36"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="32"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>186</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>107</v>
+        <v>165</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>86</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I5" s="35" t="s">
-        <v>124</v>
-      </c>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="36"/>
+        <v>81</v>
+      </c>
+      <c r="I5" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="32"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C6" s="39">
+        <v>87</v>
+      </c>
+      <c r="C6" s="35">
         <f>L6</f>
         <v>95305185749</v>
       </c>
       <c r="D6" t="s">
-        <v>183</v>
-      </c>
-      <c r="I6" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="J6" s="30">
+        <v>162</v>
+      </c>
+      <c r="I6" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="J6" s="26">
         <v>85983851018</v>
       </c>
-      <c r="K6" s="30">
+      <c r="K6" s="26">
         <v>9321334731</v>
       </c>
-      <c r="L6" s="30">
+      <c r="L6" s="26">
         <v>95305185749</v>
       </c>
-      <c r="M6" s="36" t="s">
-        <v>126</v>
+      <c r="M6" s="32" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>142</v>
-      </c>
-      <c r="C7" s="39">
+        <v>121</v>
+      </c>
+      <c r="C7" s="35">
         <f>L7</f>
         <v>2563817075</v>
       </c>
       <c r="D7" t="s">
-        <v>183</v>
-      </c>
-      <c r="I7" s="35" t="s">
-        <v>141</v>
-      </c>
-      <c r="J7" s="30">
+        <v>162</v>
+      </c>
+      <c r="I7" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="J7" s="26">
         <v>2216327709</v>
       </c>
-      <c r="K7" s="30">
+      <c r="K7" s="26">
         <v>347489366</v>
       </c>
-      <c r="L7" s="30">
+      <c r="L7" s="26">
         <v>2563817075</v>
       </c>
-      <c r="M7" s="36"/>
+      <c r="M7" s="32"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C8" s="39">
+        <v>88</v>
+      </c>
+      <c r="C8" s="35">
         <f>L8</f>
         <v>1698710276</v>
       </c>
       <c r="D8" t="s">
-        <v>183</v>
-      </c>
-      <c r="I8" s="35" t="s">
-        <v>127</v>
-      </c>
-      <c r="J8" s="30">
+        <v>162</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="J8" s="26">
         <v>1279308588</v>
       </c>
-      <c r="K8" s="30">
+      <c r="K8" s="26">
         <v>419401688</v>
       </c>
-      <c r="L8" s="30">
+      <c r="L8" s="26">
         <v>1698710276</v>
       </c>
-      <c r="M8" s="36"/>
+      <c r="M8" s="32"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>110</v>
-      </c>
-      <c r="C9" s="39">
+        <v>89</v>
+      </c>
+      <c r="C9" s="35">
         <f>L9</f>
         <v>1066831555</v>
       </c>
       <c r="D9" t="s">
-        <v>183</v>
-      </c>
-      <c r="I9" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="J9" s="30">
+        <v>162</v>
+      </c>
+      <c r="I9" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="J9" s="26">
         <v>810506954</v>
       </c>
-      <c r="K9" s="30">
+      <c r="K9" s="26">
         <v>256324601</v>
       </c>
-      <c r="L9" s="30">
+      <c r="L9" s="26">
         <v>1066831555</v>
       </c>
-      <c r="M9" s="36"/>
+      <c r="M9" s="32"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C10" s="39">
+        <v>90</v>
+      </c>
+      <c r="C10" s="35">
         <f>SUM(C6:C9)</f>
         <v>100634544655</v>
       </c>
-      <c r="I10" s="35" t="s">
-        <v>140</v>
-      </c>
-      <c r="J10" s="30">
+      <c r="I10" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="J10" s="26">
         <v>3466904030</v>
       </c>
-      <c r="K10" s="30">
+      <c r="K10" s="26">
         <v>50943892</v>
       </c>
-      <c r="L10" s="30">
+      <c r="L10" s="26">
         <v>3517847922</v>
       </c>
-      <c r="M10" s="36" t="s">
-        <v>129</v>
+      <c r="M10" s="32" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I11" s="35" t="s">
-        <v>123</v>
-      </c>
-      <c r="J11" s="30">
+      <c r="I11" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="J11" s="26">
         <v>93756898299</v>
       </c>
-      <c r="K11" s="30">
+      <c r="K11" s="26">
         <v>10395494278</v>
       </c>
-      <c r="L11" s="30">
+      <c r="L11" s="26">
         <v>104152392577</v>
       </c>
-      <c r="M11" s="36"/>
+      <c r="M11" s="32"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>143</v>
-      </c>
-      <c r="C12" s="39">
+        <v>122</v>
+      </c>
+      <c r="C12" s="35">
         <f>L10</f>
         <v>3517847922</v>
       </c>
       <c r="D12" t="s">
-        <v>183</v>
-      </c>
-      <c r="I12" s="35"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="36"/>
+        <v>162</v>
+      </c>
+      <c r="I12" s="31"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="32"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>92</v>
-      </c>
-      <c r="C13" s="39">
+        <v>82</v>
+      </c>
+      <c r="C13" s="35">
         <f>L16</f>
         <v>102667818285.175</v>
       </c>
       <c r="D13" t="s">
-        <v>183</v>
-      </c>
-      <c r="I13" s="35"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="36"/>
+        <v>162</v>
+      </c>
+      <c r="I13" s="31"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="32"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C14" s="39">
+        <v>80</v>
+      </c>
+      <c r="C14" s="35">
         <f>L17</f>
         <v>4837750599.8249998</v>
       </c>
       <c r="D14" t="s">
-        <v>183</v>
-      </c>
-      <c r="I14" s="35"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="36"/>
+        <v>162</v>
+      </c>
+      <c r="I14" s="31"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="32"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>112</v>
-      </c>
-      <c r="C15" s="39">
+        <v>91</v>
+      </c>
+      <c r="C15" s="35">
         <f>SUM(C12:C14)</f>
         <v>111023416807</v>
       </c>
-      <c r="I15" s="35" t="s">
-        <v>131</v>
-      </c>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="36" t="s">
-        <v>132</v>
+      <c r="I15" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="32" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I16" s="35" t="s">
-        <v>130</v>
-      </c>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30">
+      <c r="I16" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26">
         <v>102667818285.175</v>
       </c>
-      <c r="M16" s="36">
+      <c r="M16" s="32">
         <v>0.95499999999999996</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>113</v>
-      </c>
-      <c r="C17" s="39">
+        <v>92</v>
+      </c>
+      <c r="C17" s="35">
         <f>SUM(C10,C15)</f>
         <v>211657961462</v>
       </c>
-      <c r="I17" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30">
+      <c r="I17" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26">
         <v>4837750599.8249998</v>
       </c>
-      <c r="M17" s="36">
+      <c r="M17" s="32">
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="I18" s="35" t="s">
-        <v>123</v>
-      </c>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30">
+      <c r="I18" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26">
         <v>107505568885</v>
       </c>
-      <c r="M18" s="36"/>
+      <c r="M18" s="32"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>114</v>
-      </c>
-      <c r="C19" s="39">
+        <v>93</v>
+      </c>
+      <c r="C19" s="35">
         <f>L23-L10</f>
         <v>73480303118</v>
       </c>
       <c r="D19" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="E19" t="s">
-        <v>157</v>
-      </c>
-      <c r="I19" s="35"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="30"/>
-      <c r="L19" s="30"/>
-      <c r="M19" s="36"/>
+        <v>136</v>
+      </c>
+      <c r="I19" s="31"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="32"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>115</v>
-      </c>
-      <c r="C20" s="39">
+        <v>94</v>
+      </c>
+      <c r="C20" s="35">
         <f>L22+L10</f>
         <v>111023416807</v>
       </c>
       <c r="D20" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="E20" t="s">
-        <v>156</v>
-      </c>
-      <c r="I20" s="35"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="30"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="36"/>
+        <v>135</v>
+      </c>
+      <c r="I20" s="31"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="32"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>116</v>
-      </c>
-      <c r="C21" s="39">
+        <v>95</v>
+      </c>
+      <c r="C21" s="35">
         <f>SUM(C19:C20)</f>
         <v>184503719925</v>
       </c>
-      <c r="I21" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="36"/>
+      <c r="I21" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="32"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="I22" s="35" t="s">
-        <v>135</v>
-      </c>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="30">
+      <c r="I22" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26">
         <v>107505568885</v>
       </c>
-      <c r="M22" s="36" t="s">
-        <v>136</v>
+      <c r="M22" s="32" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>171</v>
-      </c>
-      <c r="C23" s="39">
+        <v>150</v>
+      </c>
+      <c r="C23" s="35">
         <f>180173145483 - (175607890480 -175429944726)</f>
         <v>179995199729</v>
       </c>
       <c r="D23" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="E23" t="s">
-        <v>166</v>
-      </c>
-      <c r="I23" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="J23" s="30"/>
-      <c r="K23" s="30"/>
-      <c r="L23" s="30">
+        <v>145</v>
+      </c>
+      <c r="I23" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26">
         <v>76998151040</v>
       </c>
-      <c r="M23" s="36"/>
+      <c r="M23" s="32"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>172</v>
-      </c>
-      <c r="C24" s="39">
+        <v>151</v>
+      </c>
+      <c r="C24" s="35">
         <v>175429944726</v>
       </c>
       <c r="D24" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="E24" t="s">
-        <v>166</v>
-      </c>
-      <c r="I24" s="35" t="s">
-        <v>138</v>
-      </c>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30">
+        <v>145</v>
+      </c>
+      <c r="I24" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26">
         <v>177945754</v>
       </c>
-      <c r="M24" s="36" t="s">
-        <v>158</v>
+      <c r="M24" s="32" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>176</v>
-      </c>
-      <c r="C25" s="39">
+        <v>155</v>
+      </c>
+      <c r="C25" s="35">
         <f>C23+C29</f>
         <v>183511820338</v>
       </c>
       <c r="D25" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="E25" t="s">
-        <v>179</v>
-      </c>
-      <c r="I25" s="35" t="s">
-        <v>139</v>
-      </c>
-      <c r="J25" s="30"/>
-      <c r="K25" s="30"/>
-      <c r="L25" s="30">
+        <v>158</v>
+      </c>
+      <c r="I25" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26">
         <v>184681665679</v>
       </c>
-      <c r="M25" s="36"/>
+      <c r="M25" s="32"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>177</v>
-      </c>
-      <c r="C26" s="39">
+        <v>156</v>
+      </c>
+      <c r="C26" s="35">
         <f>C24+C29</f>
         <v>178946565335</v>
       </c>
       <c r="D26" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="E26" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>181</v>
-      </c>
-      <c r="C27" s="42">
+        <v>160</v>
+      </c>
+      <c r="C27" s="38">
         <f>100*C25/C21</f>
         <v>99.4623958869755</v>
       </c>
       <c r="D27" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>182</v>
-      </c>
-      <c r="C28" s="42">
+        <v>161</v>
+      </c>
+      <c r="C28" s="38">
         <f>100*C26/C21</f>
         <v>96.988052819607674</v>
       </c>
       <c r="D28" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>165</v>
-      </c>
-      <c r="C29" s="39">
+        <v>144</v>
+      </c>
+      <c r="C29" s="35">
         <v>3516620609</v>
       </c>
       <c r="D29" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="E29" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>147</v>
-      </c>
-      <c r="C31" s="39">
+        <v>126</v>
+      </c>
+      <c r="C31" s="35">
         <v>203234206945</v>
       </c>
       <c r="D31" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="E31" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>148</v>
-      </c>
-      <c r="C32" s="39">
+        <v>127</v>
+      </c>
+      <c r="C32" s="35">
         <f>63288468 +507929211+3665994265</f>
         <v>4237211944</v>
       </c>
       <c r="D32" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="E32" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>170</v>
-      </c>
-      <c r="C34" s="45">
+        <v>149</v>
+      </c>
+      <c r="C34" s="41">
         <f>100*(C17-C24-C32-C29)/C31</f>
         <v>14.010527366933751</v>
       </c>
       <c r="D34" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="E34" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>169</v>
-      </c>
-      <c r="C35" s="45">
+        <v>148</v>
+      </c>
+      <c r="C35" s="41">
         <f>100*(C17-C24-C32-C29)*1.058002/C31</f>
         <v>14.823165975270644</v>
       </c>
       <c r="D35" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="E35" t="s">
-        <v>174</v>
-      </c>
-      <c r="I35" s="35"/>
-      <c r="J35" s="30"/>
-      <c r="K35" s="30"/>
-      <c r="L35" s="30"/>
-      <c r="M35" s="36"/>
+        <v>153</v>
+      </c>
+      <c r="I35" s="31"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="26"/>
+      <c r="L35" s="26"/>
+      <c r="M35" s="32"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="I36" s="37"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="31"/>
-      <c r="L36" s="31"/>
-      <c r="M36" s="38"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="27"/>
+      <c r="L36" s="27"/>
+      <c r="M36" s="34"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>168</v>
-      </c>
-      <c r="C37" s="41">
+        <v>147</v>
+      </c>
+      <c r="C37" s="37">
         <v>3949872663.98</v>
       </c>
       <c r="D37" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="E37" t="s">
-        <v>146</v>
-      </c>
-      <c r="F37" s="44">
+        <v>125</v>
+      </c>
+      <c r="F37" s="40">
         <f>C37/C41</f>
         <v>0.15207803906004272</v>
       </c>
-      <c r="I37" s="43"/>
-      <c r="J37" s="30"/>
-      <c r="K37" s="30"/>
-      <c r="L37" s="30"/>
-      <c r="M37" s="43"/>
+      <c r="I37" s="39"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="26"/>
+      <c r="L37" s="26"/>
+      <c r="M37" s="39"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>167</v>
-      </c>
-      <c r="C38" s="41">
+        <v>146</v>
+      </c>
+      <c r="C38" s="37">
         <v>318439464.75999999</v>
       </c>
       <c r="D38" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="E38" t="s">
-        <v>146</v>
-      </c>
-      <c r="F38" s="44">
+        <v>125</v>
+      </c>
+      <c r="F38" s="40">
         <f>C38/C41</f>
         <v>1.2260559638201943E-2</v>
       </c>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>187</v>
-      </c>
-      <c r="C39" s="39">
+        <v>166</v>
+      </c>
+      <c r="C39" s="35">
         <v>10303277133</v>
       </c>
       <c r="D39" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="E39" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>161</v>
-      </c>
-      <c r="C41" s="39">
+        <v>140</v>
+      </c>
+      <c r="C41" s="35">
         <v>25972669613.529999</v>
       </c>
       <c r="D41" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="E41" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="F41" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>188</v>
-      </c>
-      <c r="C43" s="41">
+        <v>167</v>
+      </c>
+      <c r="C43" s="37">
         <f>3007993.383*1000</f>
         <v>3007993383</v>
       </c>
       <c r="D43" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="E43" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="I44" s="35"/>
-      <c r="J44" s="30"/>
-      <c r="K44" s="30"/>
-      <c r="L44" s="30"/>
-      <c r="M44" s="36"/>
+      <c r="I44" s="31"/>
+      <c r="J44" s="26"/>
+      <c r="K44" s="26"/>
+      <c r="L44" s="26"/>
+      <c r="M44" s="32"/>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>117</v>
-      </c>
-      <c r="C45" s="39">
+        <v>96</v>
+      </c>
+      <c r="C45" s="35">
         <f>J6</f>
         <v>85983851018</v>
       </c>
       <c r="D45" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>145</v>
-      </c>
-      <c r="C46" s="39">
+        <v>124</v>
+      </c>
+      <c r="C46" s="35">
         <f>J7</f>
         <v>2216327709</v>
       </c>
       <c r="D46" t="s">
-        <v>183</v>
-      </c>
-      <c r="G46" s="25"/>
+        <v>162</v>
+      </c>
+      <c r="G46" s="23"/>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>118</v>
-      </c>
-      <c r="C47" s="39">
+        <v>97</v>
+      </c>
+      <c r="C47" s="35">
         <f>J8</f>
         <v>1279308588</v>
       </c>
       <c r="D47" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>119</v>
-      </c>
-      <c r="C48" s="39">
+        <v>98</v>
+      </c>
+      <c r="C48" s="35">
         <f>J9</f>
         <v>810506954</v>
       </c>
       <c r="D48" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>120</v>
-      </c>
-      <c r="C49" s="39">
+        <v>99</v>
+      </c>
+      <c r="C49" s="35">
         <f>SUM(C45:C48)</f>
         <v>90289994269</v>
       </c>
       <c r="D49" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>191</v>
-      </c>
-      <c r="C51" s="39">
+        <v>170</v>
+      </c>
+      <c r="C51" s="35">
         <f>K6</f>
         <v>9321334731</v>
       </c>
       <c r="D51" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>192</v>
-      </c>
-      <c r="C52" s="39">
+        <v>171</v>
+      </c>
+      <c r="C52" s="35">
         <f>K7</f>
         <v>347489366</v>
       </c>
       <c r="D52" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>193</v>
-      </c>
-      <c r="C53" s="39">
+        <v>172</v>
+      </c>
+      <c r="C53" s="35">
         <f>K8</f>
         <v>419401688</v>
       </c>
       <c r="D53" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>194</v>
-      </c>
-      <c r="C54" s="39">
+        <v>173</v>
+      </c>
+      <c r="C54" s="35">
         <f>K9</f>
         <v>256324601</v>
       </c>
       <c r="D54" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>195</v>
-      </c>
-      <c r="C55" s="39">
+        <v>174</v>
+      </c>
+      <c r="C55" s="35">
         <f>SUM(C51:C54)</f>
         <v>10344550386</v>
       </c>
       <c r="D55" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>163</v>
-      </c>
-      <c r="C57" s="39">
+        <v>142</v>
+      </c>
+      <c r="C57" s="35">
         <f>118654145.1+145569699.42+18999932198.97+1476318991.92</f>
         <v>20740475035.410004</v>
       </c>
       <c r="D57" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>164</v>
-      </c>
-      <c r="C58" s="39">
+        <v>143</v>
+      </c>
+      <c r="C58" s="35">
         <v>5232194578.1199999</v>
       </c>
       <c r="D58" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -3916,4 +3659,518 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD963C7-C30C-4F41-9ED1-A3A9BFD95FFA}">
+  <dimension ref="A1:D39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.5703125" style="45" customWidth="1"/>
+    <col min="2" max="2" width="20" style="46" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="46" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="46" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="45"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="45" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" s="47" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>188</v>
+      </c>
+      <c r="D3" s="47" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="48" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="45" t="s">
+        <v>193</v>
+      </c>
+      <c r="B5" s="46">
+        <v>174402</v>
+      </c>
+      <c r="C5" s="46">
+        <v>11811</v>
+      </c>
+      <c r="D5" s="46">
+        <f>SUM(B5:C5)</f>
+        <v>186213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="45" t="s">
+        <v>194</v>
+      </c>
+      <c r="B6" s="46">
+        <v>37586</v>
+      </c>
+      <c r="C6" s="46">
+        <v>8909</v>
+      </c>
+      <c r="D6" s="46">
+        <f t="shared" ref="D6:D25" si="0">SUM(B6:C6)</f>
+        <v>46495</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="45" t="s">
+        <v>195</v>
+      </c>
+      <c r="B7" s="46">
+        <v>61005</v>
+      </c>
+      <c r="C7" s="46">
+        <v>3566</v>
+      </c>
+      <c r="D7" s="46">
+        <f t="shared" si="0"/>
+        <v>64571</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="45" t="s">
+        <v>196</v>
+      </c>
+      <c r="B8" s="46">
+        <v>195158</v>
+      </c>
+      <c r="C8" s="46">
+        <v>14642</v>
+      </c>
+      <c r="D8" s="46">
+        <f t="shared" si="0"/>
+        <v>209800</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="46">
+        <v>468151</v>
+      </c>
+      <c r="C9" s="46">
+        <v>38928</v>
+      </c>
+      <c r="D9" s="46">
+        <f t="shared" si="0"/>
+        <v>507079</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="49" t="s">
+        <v>202</v>
+      </c>
+      <c r="B11" s="46">
+        <v>12251583453</v>
+      </c>
+      <c r="C11" s="46">
+        <v>699252899</v>
+      </c>
+      <c r="D11" s="46">
+        <f t="shared" si="0"/>
+        <v>12950836352</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="49" t="s">
+        <v>203</v>
+      </c>
+      <c r="B12" s="46">
+        <v>12934685803</v>
+      </c>
+      <c r="C12" s="46">
+        <v>738240618</v>
+      </c>
+      <c r="D12" s="46">
+        <f t="shared" si="0"/>
+        <v>13672926421</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="49"/>
+      <c r="B13" s="50"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="48" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="49" t="s">
+        <v>197</v>
+      </c>
+      <c r="B15" s="46">
+        <v>132446673597</v>
+      </c>
+      <c r="C15" s="46">
+        <v>5746905539</v>
+      </c>
+      <c r="D15" s="46">
+        <f t="shared" si="0"/>
+        <v>138193579136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="49" t="s">
+        <v>198</v>
+      </c>
+      <c r="B16" s="46">
+        <v>115469058970</v>
+      </c>
+      <c r="C16" s="46">
+        <v>4670036601</v>
+      </c>
+      <c r="D16" s="46">
+        <f t="shared" si="0"/>
+        <v>120139095571</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="49" t="s">
+        <v>199</v>
+      </c>
+      <c r="B17" s="46">
+        <v>80223069956</v>
+      </c>
+      <c r="C17" s="46">
+        <v>3589902866</v>
+      </c>
+      <c r="D17" s="46">
+        <f t="shared" si="0"/>
+        <v>83812972822</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="49" t="s">
+        <v>200</v>
+      </c>
+      <c r="B18" s="46">
+        <v>35245989014</v>
+      </c>
+      <c r="C18" s="46">
+        <v>1080133735</v>
+      </c>
+      <c r="D18" s="46">
+        <f t="shared" si="0"/>
+        <v>36326122749</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="49" t="s">
+        <v>201</v>
+      </c>
+      <c r="B19" s="51">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="C19" s="51">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="D19" s="55">
+        <f>D17/D16</f>
+        <v>0.69763279325228544</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="49"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="48" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="49" t="s">
+        <v>204</v>
+      </c>
+      <c r="B22" s="46">
+        <v>2174670866</v>
+      </c>
+      <c r="C22" s="46">
+        <v>134810119</v>
+      </c>
+      <c r="D22" s="46">
+        <f t="shared" si="0"/>
+        <v>2309480985</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="B23" s="46">
+        <v>893164372</v>
+      </c>
+      <c r="C23" s="46">
+        <v>58830395</v>
+      </c>
+      <c r="D23" s="46">
+        <f t="shared" si="0"/>
+        <v>951994767</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="49" t="s">
+        <v>206</v>
+      </c>
+      <c r="B24" s="46">
+        <v>1281506494</v>
+      </c>
+      <c r="C24" s="46">
+        <v>75979724</v>
+      </c>
+      <c r="D24" s="46">
+        <f t="shared" si="0"/>
+        <v>1357486218</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="49" t="s">
+        <v>207</v>
+      </c>
+      <c r="B25" s="46">
+        <v>2725165218</v>
+      </c>
+      <c r="C25" s="46">
+        <v>77744321</v>
+      </c>
+      <c r="D25" s="46">
+        <f t="shared" si="0"/>
+        <v>2802909539</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A27" s="52" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="49" t="s">
+        <v>204</v>
+      </c>
+      <c r="B28" s="53">
+        <v>0.16813</v>
+      </c>
+      <c r="C28" s="56">
+        <v>0.18260999999999999</v>
+      </c>
+      <c r="D28" s="55">
+        <f>D22/$D$12</f>
+        <v>0.16890904798938361</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="B29" s="53">
+        <v>6.905E-2</v>
+      </c>
+      <c r="C29" s="56">
+        <v>7.9689999999999997E-2</v>
+      </c>
+      <c r="D29" s="55">
+        <f t="shared" ref="D29:D32" si="1">D23/$D$12</f>
+        <v>6.9626262709777217E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="49" t="s">
+        <v>206</v>
+      </c>
+      <c r="B30" s="53">
+        <v>9.9080000000000001E-2</v>
+      </c>
+      <c r="C30" s="56">
+        <v>0.10292</v>
+      </c>
+      <c r="D30" s="55">
+        <f t="shared" si="1"/>
+        <v>9.9282785279606378E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="49" t="s">
+        <v>207</v>
+      </c>
+      <c r="B31" s="53">
+        <v>0.21068999999999999</v>
+      </c>
+      <c r="C31" s="56">
+        <v>0.10531</v>
+      </c>
+      <c r="D31" s="55">
+        <f t="shared" si="1"/>
+        <v>0.20499704691565238</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="54">
+        <v>0.30976999999999999</v>
+      </c>
+      <c r="C32" s="56">
+        <v>0.20823</v>
+      </c>
+      <c r="D32" s="55">
+        <f>SUM(D24:D25)/D12</f>
+        <v>0.30427983219525878</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A34" s="52" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="49" t="s">
+        <v>204</v>
+      </c>
+      <c r="B35" s="55">
+        <f>B22/B$11</f>
+        <v>0.17750120825953289</v>
+      </c>
+      <c r="C35" s="55">
+        <f>C22/C$11</f>
+        <v>0.19279164833323059</v>
+      </c>
+      <c r="D35" s="55">
+        <f>D22/D$11</f>
+        <v>0.1783267830917612</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="B36" s="55">
+        <f t="shared" ref="B36:C38" si="2">B23/B$11</f>
+        <v>7.2901953892441071E-2</v>
+      </c>
+      <c r="C36" s="55">
+        <f t="shared" si="2"/>
+        <v>8.4133215728005153E-2</v>
+      </c>
+      <c r="D36" s="55">
+        <f t="shared" ref="D36" si="3">D23/D$11</f>
+        <v>7.3508362018101112E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="49" t="s">
+        <v>206</v>
+      </c>
+      <c r="B37" s="55">
+        <f t="shared" si="2"/>
+        <v>0.1045992543670918</v>
+      </c>
+      <c r="C37" s="55">
+        <f t="shared" si="2"/>
+        <v>0.10865843260522542</v>
+      </c>
+      <c r="D37" s="55">
+        <f t="shared" ref="D37" si="4">D24/D$11</f>
+        <v>0.10481842107366009</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="49" t="s">
+        <v>207</v>
+      </c>
+      <c r="B38" s="55">
+        <f t="shared" si="2"/>
+        <v>0.222433714666711</v>
+      </c>
+      <c r="C38" s="55">
+        <f t="shared" si="2"/>
+        <v>0.11118197881078788</v>
+      </c>
+      <c r="D38" s="55">
+        <f t="shared" ref="D38" si="5">D25/D$11</f>
+        <v>0.21642691350718413</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="B39" s="55">
+        <f>SUM(B24:B25)/B$11</f>
+        <v>0.3270329690338028</v>
+      </c>
+      <c r="C39" s="55">
+        <f t="shared" ref="C39:D39" si="6">SUM(C24:C25)/C$11</f>
+        <v>0.21984041141601332</v>
+      </c>
+      <c r="D39" s="55">
+        <f t="shared" si="6"/>
+        <v>0.3212453345808442</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3E00125-AE25-4C2C-BBE6-6A6AFF0CBB38}">
+  <dimension ref="A3:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add alternative policy options
</commit_message>
<xml_diff>
--- a/model/RunControl.xlsx
+++ b/model/RunControl.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FF59E6-B4C8-45BB-A97D-49A59646FF83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CE3A56-FA9E-4214-9F66-65C4ACEC9ACB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="targetVals_2018" sheetId="20" r:id="rId6"/>
     <sheet name="targeVals_raw" sheetId="23" r:id="rId7"/>
     <sheet name="shares" sheetId="24" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="25" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -121,6 +122,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
+    <author>tc={193EA9F6-E97A-4C0F-8458-C4A79EA80C2A}</author>
   </authors>
   <commentList>
     <comment ref="D4" authorId="0" shapeId="0" xr:uid="{03C2B8DE-A041-40C7-A6E1-06D6FD91B561}">
@@ -147,12 +149,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="E4" authorId="1" shapeId="0" xr:uid="{193EA9F6-E97A-4C0F-8458-C4A79EA80C2A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    comma separated tier names</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="258">
   <si>
     <t>nsim</t>
   </si>
@@ -844,15 +854,6 @@
     <t>AL_defrRet_pctALservRet</t>
   </si>
   <si>
-    <t>sim_2tiers_baseline</t>
-  </si>
-  <si>
-    <t>sim_2tiers_cola_fast</t>
-  </si>
-  <si>
-    <t>sim_2tiers_cola_slow</t>
-  </si>
-  <si>
     <t>Special settings</t>
   </si>
   <si>
@@ -862,9 +863,6 @@
     <t>sim_name_baseline</t>
   </si>
   <si>
-    <t>use_baseline_MA</t>
-  </si>
-  <si>
     <t>lower cola assumption</t>
   </si>
   <si>
@@ -880,22 +878,64 @@
     <t>Keep high contributions</t>
   </si>
   <si>
-    <t>combine the two "fast" runs</t>
-  </si>
-  <si>
-    <t>combine the two "slow" runs</t>
-  </si>
-  <si>
-    <t>sim_2tiers_bf1_fast</t>
-  </si>
-  <si>
-    <t>sim_2tiers_bf1_slow</t>
-  </si>
-  <si>
-    <t>sim_2tiers_bf1&amp;cola_fast</t>
-  </si>
-  <si>
-    <t>sim_2tiers_bf1&amp;cola_slow</t>
+    <t>twoTiers_baseline</t>
+  </si>
+  <si>
+    <t>use_baselineMA</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>COLA</t>
+  </si>
+  <si>
+    <t>cola_assumed_override</t>
+  </si>
+  <si>
+    <t>COLA rsuspension</t>
+  </si>
+  <si>
+    <t>twoTiers_bf2</t>
+  </si>
+  <si>
+    <t>twoTiers_bf1</t>
+  </si>
+  <si>
+    <t>twoTiers_bf2_cola1</t>
+  </si>
+  <si>
+    <t>twoTiers_bf1_cola1</t>
+  </si>
+  <si>
+    <t>twoTiers_bf2_cola1p5</t>
+  </si>
+  <si>
+    <t>twoTiers_bf1_cola1p5</t>
+  </si>
+  <si>
+    <t>twoTiers_bf1_lowERC</t>
+  </si>
+  <si>
+    <t>twoTiers_bf1_highERC</t>
+  </si>
+  <si>
+    <t>twoTiers_cola_lowERC</t>
+  </si>
+  <si>
+    <t>twoTiers_cola_highERC</t>
+  </si>
+  <si>
+    <t>twoTiers_bf1&amp;cola_lowERC</t>
+  </si>
+  <si>
+    <t>twoTiers_bf1&amp;cola_highERC</t>
+  </si>
+  <si>
+    <t>combine the two "lowERC" runs</t>
+  </si>
+  <si>
+    <t>combine the two "highERC" runs</t>
   </si>
 </sst>
 </file>
@@ -1395,6 +1435,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1690,24 +1734,32 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E4" dT="2020-06-24T14:51:37.17" personId="{00000000-0000-0000-0000-000000000000}" id="{193EA9F6-E97A-4C0F-8458-C4A79EA80C2A}">
+    <text>comma separated tier names</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D014B46A-D012-4D18-AEAB-1D829080B2CE}">
-  <dimension ref="A2:AP21"/>
+  <dimension ref="A2:AP20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H26" sqref="H26"/>
+      <selection pane="bottomRight" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
     <col min="3" max="3" width="8.140625" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" customWidth="1"/>
     <col min="8" max="8" width="17.42578125" customWidth="1"/>
@@ -1754,7 +1806,7 @@
       </c>
       <c r="F3" s="19"/>
       <c r="G3" s="63" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H3" s="63"/>
       <c r="I3" s="63"/>
@@ -1824,13 +1876,13 @@
         <v>171</v>
       </c>
       <c r="G4" s="64" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="H4" s="64" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="I4" s="64" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J4" s="58" t="s">
         <v>221</v>
@@ -1949,7 +2001,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>230</v>
+        <v>169</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -1964,7 +2016,7 @@
         <v>0.02</v>
       </c>
       <c r="L5">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="M5" t="s">
         <v>36</v>
@@ -2068,7 +2120,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
@@ -2083,7 +2135,7 @@
         <v>0.02</v>
       </c>
       <c r="L6">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="M6" t="s">
         <v>36</v>
@@ -2187,7 +2239,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
@@ -2202,7 +2254,7 @@
         <v>0.02</v>
       </c>
       <c r="L7">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="M7" t="s">
         <v>36</v>
@@ -2308,7 +2360,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -2410,33 +2462,155 @@
         <v>1</v>
       </c>
     </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>238</v>
+      </c>
+      <c r="B10" t="s">
+        <v>235</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>244</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>238</v>
+      </c>
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0.02</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10" t="s">
+        <v>36</v>
+      </c>
+      <c r="N10" t="s">
+        <v>35</v>
+      </c>
+      <c r="O10">
+        <v>20</v>
+      </c>
+      <c r="P10">
+        <v>2.75E-2</v>
+      </c>
+      <c r="Q10">
+        <v>5</v>
+      </c>
+      <c r="R10">
+        <v>999</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10" t="s">
+        <v>55</v>
+      </c>
+      <c r="U10" t="b">
+        <v>0</v>
+      </c>
+      <c r="V10" t="s">
+        <v>216</v>
+      </c>
+      <c r="W10" t="s">
+        <v>20</v>
+      </c>
+      <c r="X10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y10">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="AA10" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AB10" s="56">
+        <v>123</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE10" s="24">
+        <v>0.6976</v>
+      </c>
+      <c r="AF10" s="24">
+        <v>0.6976</v>
+      </c>
+      <c r="AI10" s="61">
+        <v>0.1</v>
+      </c>
+      <c r="AJ10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM10">
+        <v>0</v>
+      </c>
+      <c r="AN10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AP10" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>230</v>
+        <v>250</v>
       </c>
       <c r="B11" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>207</v>
+        <v>245</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="H11" t="b">
         <v>0</v>
       </c>
       <c r="I11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" t="b">
         <v>0</v>
@@ -2445,7 +2619,7 @@
         <v>0.02</v>
       </c>
       <c r="L11">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="M11" t="s">
         <v>36</v>
@@ -2496,16 +2670,18 @@
         <v>123</v>
       </c>
       <c r="AC11" t="s">
-        <v>31</v>
+        <v>227</v>
       </c>
       <c r="AD11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AE11" s="24">
-        <v>0.6976</v>
-      </c>
-      <c r="AF11" s="24">
-        <v>0.6976</v>
+        <v>228</v>
+      </c>
+      <c r="AE11" s="24"/>
+      <c r="AF11" s="24"/>
+      <c r="AG11" s="62">
+        <v>81825573157</v>
+      </c>
+      <c r="AH11" s="62">
+        <v>81825573157</v>
       </c>
       <c r="AI11" s="61">
         <v>0.1</v>
@@ -2534,10 +2710,10 @@
     </row>
     <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="B12" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -2546,16 +2722,16 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>209</v>
+        <v>245</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="H12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
@@ -2567,7 +2743,7 @@
         <v>0.02</v>
       </c>
       <c r="L12">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="M12" t="s">
         <v>36</v>
@@ -2656,136 +2832,134 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>245</v>
-      </c>
-      <c r="B13" t="s">
-        <v>241</v>
-      </c>
-      <c r="C13" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" t="s">
-        <v>209</v>
-      </c>
-      <c r="F13" t="b">
-        <v>0</v>
-      </c>
-      <c r="G13" t="s">
-        <v>230</v>
-      </c>
-      <c r="H13" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>252</v>
+      </c>
+      <c r="B15" t="s">
+        <v>233</v>
+      </c>
+      <c r="C15" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>246</v>
+      </c>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>238</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" t="b">
+        <v>1</v>
+      </c>
+      <c r="K15">
         <v>0.02</v>
       </c>
-      <c r="L13">
-        <v>0.02</v>
-      </c>
-      <c r="M13" t="s">
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15" t="s">
         <v>36</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N15" t="s">
         <v>35</v>
       </c>
-      <c r="O13">
+      <c r="O15">
         <v>20</v>
       </c>
-      <c r="P13">
+      <c r="P15">
         <v>2.75E-2</v>
       </c>
-      <c r="Q13">
+      <c r="Q15">
         <v>5</v>
       </c>
-      <c r="R13">
+      <c r="R15">
         <v>999</v>
       </c>
-      <c r="S13">
-        <v>0</v>
-      </c>
-      <c r="T13" t="s">
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15" t="s">
         <v>55</v>
       </c>
-      <c r="U13" t="b">
-        <v>0</v>
-      </c>
-      <c r="V13" t="s">
+      <c r="U15" t="b">
+        <v>0</v>
+      </c>
+      <c r="V15" t="s">
         <v>216</v>
       </c>
-      <c r="W13" t="s">
+      <c r="W15" t="s">
         <v>20</v>
       </c>
-      <c r="X13">
+      <c r="X15">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="Y13">
+      <c r="Y15">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="Z13" s="3">
+      <c r="Z15" s="3">
         <v>0.12</v>
       </c>
-      <c r="AA13" s="5">
+      <c r="AA15" s="5">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AB13" s="56">
+      <c r="AB15" s="56">
         <v>123</v>
       </c>
-      <c r="AC13" t="s">
-        <v>227</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>228</v>
-      </c>
-      <c r="AE13" s="24"/>
-      <c r="AF13" s="24"/>
-      <c r="AG13" s="62">
-        <v>81825573157</v>
-      </c>
-      <c r="AH13" s="62">
-        <v>81825573157</v>
-      </c>
-      <c r="AI13" s="61">
+      <c r="AC15" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE15" s="24">
+        <v>0.6976</v>
+      </c>
+      <c r="AF15" s="24">
+        <v>0.6976</v>
+      </c>
+      <c r="AI15" s="61">
         <v>0.1</v>
       </c>
-      <c r="AJ13" t="b">
-        <v>1</v>
-      </c>
-      <c r="AK13" t="b">
-        <v>1</v>
-      </c>
-      <c r="AL13" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM13">
-        <v>0</v>
-      </c>
-      <c r="AN13" t="s">
+      <c r="AJ15" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK15" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL15" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM15">
+        <v>0</v>
+      </c>
+      <c r="AN15" t="s">
         <v>3</v>
       </c>
-      <c r="AO13" t="b">
-        <v>1</v>
-      </c>
-      <c r="AP13" s="22" t="b">
+      <c r="AO15" t="b">
+        <v>1</v>
+      </c>
+      <c r="AP15" s="22" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>231</v>
+        <v>253</v>
       </c>
       <c r="B16" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
@@ -2794,13 +2968,13 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>207</v>
+        <v>244</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="H16" t="b">
         <v>0</v>
@@ -2902,134 +3076,134 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>232</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>254</v>
+      </c>
+      <c r="B19" t="s">
+        <v>256</v>
+      </c>
+      <c r="C19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>247</v>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
         <v>238</v>
       </c>
-      <c r="C17" t="b">
-        <v>0</v>
-      </c>
-      <c r="D17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E17" t="s">
-        <v>207</v>
-      </c>
-      <c r="F17" t="b">
-        <v>0</v>
-      </c>
-      <c r="G17" t="s">
-        <v>230</v>
-      </c>
-      <c r="H17" t="b">
-        <v>0</v>
-      </c>
-      <c r="I17" t="b">
-        <v>1</v>
-      </c>
-      <c r="J17" t="b">
-        <v>1</v>
-      </c>
-      <c r="K17">
+      <c r="H19" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19">
         <v>0.02</v>
       </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17" t="s">
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19" t="s">
         <v>36</v>
       </c>
-      <c r="N17" t="s">
+      <c r="N19" t="s">
         <v>35</v>
       </c>
-      <c r="O17">
+      <c r="O19">
         <v>20</v>
       </c>
-      <c r="P17">
+      <c r="P19">
         <v>2.75E-2</v>
       </c>
-      <c r="Q17">
+      <c r="Q19">
         <v>5</v>
       </c>
-      <c r="R17">
+      <c r="R19">
         <v>999</v>
       </c>
-      <c r="S17">
-        <v>0</v>
-      </c>
-      <c r="T17" t="s">
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19" t="s">
         <v>55</v>
       </c>
-      <c r="U17" t="b">
-        <v>0</v>
-      </c>
-      <c r="V17" t="s">
+      <c r="U19" t="b">
+        <v>0</v>
+      </c>
+      <c r="V19" t="s">
         <v>216</v>
       </c>
-      <c r="W17" t="s">
+      <c r="W19" t="s">
         <v>20</v>
       </c>
-      <c r="X17">
+      <c r="X19">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="Y17">
+      <c r="Y19">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="Z17" s="3">
+      <c r="Z19" s="3">
         <v>0.12</v>
       </c>
-      <c r="AA17" s="5">
+      <c r="AA19" s="5">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AB17" s="56">
+      <c r="AB19" s="56">
         <v>123</v>
       </c>
-      <c r="AC17" t="s">
+      <c r="AC19" t="s">
         <v>31</v>
       </c>
-      <c r="AD17" t="s">
+      <c r="AD19" t="s">
         <v>31</v>
       </c>
-      <c r="AE17" s="24">
+      <c r="AE19" s="24">
         <v>0.6976</v>
       </c>
-      <c r="AF17" s="24">
+      <c r="AF19" s="24">
         <v>0.6976</v>
       </c>
-      <c r="AI17" s="61">
+      <c r="AI19" s="61">
         <v>0.1</v>
       </c>
-      <c r="AJ17" t="b">
-        <v>1</v>
-      </c>
-      <c r="AK17" t="b">
-        <v>1</v>
-      </c>
-      <c r="AL17" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM17">
-        <v>0</v>
-      </c>
-      <c r="AN17" t="s">
+      <c r="AJ19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM19">
+        <v>0</v>
+      </c>
+      <c r="AN19" t="s">
         <v>3</v>
       </c>
-      <c r="AO17" t="b">
-        <v>1</v>
-      </c>
-      <c r="AP17" s="22" t="b">
+      <c r="AO19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AP19" s="22" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="B20" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -3038,16 +3212,16 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>209</v>
+        <v>245</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="H20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" t="b">
         <v>1</v>
@@ -3146,137 +3320,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>247</v>
-      </c>
-      <c r="B21" t="s">
-        <v>243</v>
-      </c>
-      <c r="C21" t="b">
-        <v>0</v>
-      </c>
-      <c r="D21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E21" t="s">
-        <v>209</v>
-      </c>
-      <c r="F21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G21" t="s">
-        <v>230</v>
-      </c>
-      <c r="H21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I21" t="b">
-        <v>1</v>
-      </c>
-      <c r="J21" t="b">
-        <v>1</v>
-      </c>
-      <c r="K21">
-        <v>0.02</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21" t="s">
-        <v>36</v>
-      </c>
-      <c r="N21" t="s">
-        <v>35</v>
-      </c>
-      <c r="O21">
-        <v>20</v>
-      </c>
-      <c r="P21">
-        <v>2.75E-2</v>
-      </c>
-      <c r="Q21">
-        <v>5</v>
-      </c>
-      <c r="R21">
-        <v>999</v>
-      </c>
-      <c r="S21">
-        <v>0</v>
-      </c>
-      <c r="T21" t="s">
-        <v>55</v>
-      </c>
-      <c r="U21" t="b">
-        <v>0</v>
-      </c>
-      <c r="V21" t="s">
-        <v>216</v>
-      </c>
-      <c r="W21" t="s">
-        <v>20</v>
-      </c>
-      <c r="X21">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="Y21">
-        <v>7.7200000000000005E-2</v>
-      </c>
-      <c r="Z21" s="3">
-        <v>0.12</v>
-      </c>
-      <c r="AA21" s="5">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AB21" s="56">
-        <v>123</v>
-      </c>
-      <c r="AC21" t="s">
-        <v>31</v>
-      </c>
-      <c r="AD21" t="s">
-        <v>31</v>
-      </c>
-      <c r="AE21" s="24">
-        <v>0.6976</v>
-      </c>
-      <c r="AF21" s="24">
-        <v>0.6976</v>
-      </c>
-      <c r="AI21" s="61">
-        <v>0.1</v>
-      </c>
-      <c r="AJ21" t="b">
-        <v>1</v>
-      </c>
-      <c r="AK21" t="b">
-        <v>1</v>
-      </c>
-      <c r="AL21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM21">
-        <v>0</v>
-      </c>
-      <c r="AN21" t="s">
-        <v>3</v>
-      </c>
-      <c r="AO21" t="b">
-        <v>1</v>
-      </c>
-      <c r="AP21" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK5:AL8 C5:C8 AK11:AL13 C11:C13 AK16:AL17 C16:C17 AK20:AL21 C20:C21" xr:uid="{1240F49A-5091-456D-B77A-0673AD56E758}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK5:AL8 C5:C8 AK10:AL12 C10:C12 AK15:AL16 C15:C16 AK19:AL20 C19:C20" xr:uid="{1240F49A-5091-456D-B77A-0673AD56E758}">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V5:V8 V11:V13 V16:V17 V20:V21" xr:uid="{8909875A-86FC-4594-BBAF-A364A5851F3C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V5:V8 V10:V12 V15:V16 V19:V20" xr:uid="{8909875A-86FC-4594-BBAF-A364A5851F3C}">
       <formula1>"simple, internal"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D8 D11:D13 D16:D17 D20:D21" xr:uid="{EC327A6A-3FD9-4228-86E6-BF4DFCBDFAEB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D8 D10:D12 D15:D16 D19:D20" xr:uid="{EC327A6A-3FD9-4228-86E6-BF4DFCBDFAEB}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3288,35 +3340,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62142380-6405-410A-A4D9-17F48F5CE536}">
-  <dimension ref="A3:Q8"/>
+  <dimension ref="A3:R14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" customWidth="1"/>
     <col min="6" max="6" width="17.140625" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
     <col min="8" max="9" width="17.42578125" customWidth="1"/>
     <col min="10" max="10" width="20.28515625" customWidth="1"/>
     <col min="11" max="11" width="19.7109375" customWidth="1"/>
     <col min="12" max="12" width="22" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" customWidth="1"/>
-    <col min="14" max="14" width="25.7109375" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" customWidth="1"/>
-    <col min="17" max="17" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="23.42578125" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" customWidth="1"/>
+    <col min="15" max="15" width="25.7109375" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" customWidth="1"/>
+    <col min="18" max="18" width="14.28515625" customWidth="1"/>
+    <col min="19" max="19" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:17" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -3339,8 +3393,11 @@
         <v>222</v>
       </c>
       <c r="L3" s="57"/>
-    </row>
-    <row r="4" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="57" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>167</v>
       </c>
@@ -3377,23 +3434,26 @@
       <c r="L4" s="58" t="s">
         <v>210</v>
       </c>
-      <c r="M4" s="12" t="s">
+      <c r="M4" s="58" t="s">
+        <v>242</v>
+      </c>
+      <c r="N4" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="O4" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>162</v>
       </c>
@@ -3427,75 +3487,28 @@
       <c r="L5">
         <v>2018</v>
       </c>
-      <c r="M5" t="b">
-        <v>1</v>
-      </c>
-      <c r="N5" s="61">
+      <c r="N5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O5" s="61">
         <v>0.11</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>0.02</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>0.05</v>
       </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>207</v>
-      </c>
-      <c r="C6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" t="s">
-        <v>166</v>
-      </c>
-      <c r="F6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6">
-        <v>2.75E-2</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>2018</v>
-      </c>
-      <c r="M6" t="b">
-        <v>1</v>
-      </c>
-      <c r="N6" s="61">
-        <v>0.11</v>
-      </c>
-      <c r="O6">
-        <v>0.02</v>
-      </c>
-      <c r="P6">
-        <v>0.05</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O6" s="61"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>209</v>
+        <v>244</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -3522,36 +3535,298 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K7">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="L7">
         <v>2018</v>
       </c>
-      <c r="M7" t="b">
-        <v>1</v>
-      </c>
-      <c r="N7" s="61">
+      <c r="N7" t="b">
+        <v>1</v>
+      </c>
+      <c r="O7" s="61">
         <v>0.11</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>0.02</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>0.05</v>
       </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N8" s="61"/>
+      <c r="R7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>245</v>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" t="s">
+        <v>166</v>
+      </c>
+      <c r="F8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8">
+        <v>2.75E-2</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K8">
+        <v>0.01</v>
+      </c>
+      <c r="L8">
+        <v>2018</v>
+      </c>
+      <c r="N8" t="b">
+        <v>1</v>
+      </c>
+      <c r="O8" s="61">
+        <v>0.11</v>
+      </c>
+      <c r="P8">
+        <v>0.02</v>
+      </c>
+      <c r="Q8">
+        <v>0.05</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O9" s="61"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>246</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10">
+        <v>2.75E-2</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>2018</v>
+      </c>
+      <c r="M10">
+        <v>0.01</v>
+      </c>
+      <c r="N10" t="b">
+        <v>1</v>
+      </c>
+      <c r="O10" s="61">
+        <v>0.11</v>
+      </c>
+      <c r="P10">
+        <v>0.02</v>
+      </c>
+      <c r="Q10">
+        <v>0.05</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>247</v>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" t="s">
+        <v>166</v>
+      </c>
+      <c r="F11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11">
+        <v>2.75E-2</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K11">
+        <v>0.01</v>
+      </c>
+      <c r="L11">
+        <v>2018</v>
+      </c>
+      <c r="M11">
+        <v>0.01</v>
+      </c>
+      <c r="N11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O11" s="61">
+        <v>0.11</v>
+      </c>
+      <c r="P11">
+        <v>0.02</v>
+      </c>
+      <c r="Q11">
+        <v>0.05</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>248</v>
+      </c>
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" t="s">
+        <v>166</v>
+      </c>
+      <c r="F13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13">
+        <v>2.75E-2</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>2018</v>
+      </c>
+      <c r="M13">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="N13" t="b">
+        <v>1</v>
+      </c>
+      <c r="O13" s="61">
+        <v>0.11</v>
+      </c>
+      <c r="P13">
+        <v>0.02</v>
+      </c>
+      <c r="Q13">
+        <v>0.05</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>249</v>
+      </c>
+      <c r="C14" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" t="s">
+        <v>166</v>
+      </c>
+      <c r="F14" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14">
+        <v>2.75E-2</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K14">
+        <v>0.01</v>
+      </c>
+      <c r="L14">
+        <v>2018</v>
+      </c>
+      <c r="M14">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="N14" t="b">
+        <v>1</v>
+      </c>
+      <c r="O14" s="61">
+        <v>0.11</v>
+      </c>
+      <c r="P14">
+        <v>0.02</v>
+      </c>
+      <c r="Q14">
+        <v>0.05</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D7" xr:uid="{73B0AF26-6A4C-427C-B7EA-75439AFB0B6E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D8 D10:D11 D13:D14" xr:uid="{73B0AF26-6A4C-427C-B7EA-75439AFB0B6E}">
       <formula1>"singleTier,multiTier"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C7" xr:uid="{BD331DEC-2DB8-437E-B2EB-02992BFDA38C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C8 C10:C11 C13:C14" xr:uid="{BD331DEC-2DB8-437E-B2EB-02992BFDA38C}">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3566,7 +3841,7 @@
   <dimension ref="A3:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3613,7 +3888,7 @@
         <v>2018</v>
       </c>
       <c r="B4">
-        <v>500</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>32</v>
@@ -3650,7 +3925,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U15" sqref="U15"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5307,4 +5582,277 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C9FDD0-43C0-4547-B8AB-B7BD31607ED6}">
+  <dimension ref="A3:B53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update before adding tier sfty
</commit_message>
<xml_diff>
--- a/model/RunControl.xlsx
+++ b/model/RunControl.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB389D16-440B-49EB-BFF2-19DD9BA0A4FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698A6160-4E3F-4A3D-8A68-6DEA67278BFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="524" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params_sim" sheetId="22" r:id="rId1"/>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="279">
   <si>
     <t>nsim</t>
   </si>
@@ -906,9 +906,6 @@
     <t>cola_assumed_override</t>
   </si>
   <si>
-    <t>COLA rsuspension</t>
-  </si>
-  <si>
     <t>twoTiers_bf2</t>
   </si>
   <si>
@@ -1015,6 +1012,12 @@
   </si>
   <si>
     <t>Misc+inds</t>
+  </si>
+  <si>
+    <t>COLA suspension</t>
+  </si>
+  <si>
+    <t>lower cola assumption, high UAAL</t>
   </si>
 </sst>
 </file>
@@ -1031,7 +1034,7 @@
     <numFmt numFmtId="168" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="169" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1124,12 +1127,6 @@
       <color rgb="FF000000"/>
       <name val="Lucida Console"/>
       <family val="3"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1522,10 +1519,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1841,17 +1834,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D014B46A-D012-4D18-AEAB-1D829080B2CE}">
   <dimension ref="A2:AP20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H32" sqref="H32"/>
+      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
     <col min="3" max="3" width="8.140625" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.85546875" customWidth="1"/>
@@ -2571,7 +2564,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -2681,7 +2674,7 @@
     </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B11" t="s">
         <v>236</v>
@@ -2693,7 +2686,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -2805,7 +2798,7 @@
     </row>
     <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B12" t="s">
         <v>237</v>
@@ -2817,7 +2810,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
@@ -2929,7 +2922,7 @@
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B14" t="s">
         <v>233</v>
@@ -2941,7 +2934,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -3051,7 +3044,7 @@
     </row>
     <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B15" t="s">
         <v>234</v>
@@ -3063,7 +3056,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -3173,10 +3166,10 @@
     </row>
     <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B16" t="s">
-        <v>234</v>
+        <v>278</v>
       </c>
       <c r="C16" t="b">
         <v>1</v>
@@ -3185,7 +3178,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
@@ -3295,10 +3288,10 @@
     </row>
     <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
@@ -3307,7 +3300,7 @@
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
@@ -3417,10 +3410,10 @@
     </row>
     <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
@@ -3429,7 +3422,7 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
@@ -3539,10 +3532,10 @@
     </row>
     <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C20" t="b">
         <v>1</v>
@@ -3551,7 +3544,7 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
@@ -3695,12 +3688,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B2" s="37">
         <v>80223070</v>
@@ -3712,7 +3705,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B3" s="37">
         <f>3589902866/1000</f>
@@ -3725,7 +3718,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B4" s="37">
         <f>SUM(B2:B3)</f>
@@ -3746,7 +3739,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B5" s="65">
         <f>10551342261/1000</f>
@@ -3759,7 +3752,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B6" s="65">
         <f>33326594392/1000</f>
@@ -3772,7 +3765,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B7" s="65">
         <f>8540511923/1000</f>
@@ -3785,7 +3778,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B8" s="37">
         <f>136231421398/1000</f>
@@ -3802,7 +3795,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B10" s="37">
         <v>259890776</v>
@@ -3810,7 +3803,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B11" s="37">
         <v>64796136</v>
@@ -3818,7 +3811,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B12" s="37">
         <v>29308589</v>
@@ -3826,7 +3819,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B14" s="37">
         <v>365580900</v>
@@ -3843,10 +3836,10 @@
   <dimension ref="A3:R14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E29" sqref="E29"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3894,7 +3887,7 @@
       </c>
       <c r="L3" s="57"/>
       <c r="M3" s="57" t="s">
-        <v>241</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4008,7 +4001,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -4058,7 +4051,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
@@ -4111,7 +4104,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -4164,7 +4157,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -4217,7 +4210,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -4270,7 +4263,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -6088,7 +6081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C9FDD0-43C0-4547-B8AB-B7BD31607ED6}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
@@ -6101,20 +6094,20 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B3" s="37">
         <v>259890776</v>
@@ -6125,7 +6118,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B4" s="37">
         <v>64796136</v>
@@ -6136,7 +6129,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B5" s="37">
         <v>29308589</v>
@@ -6147,7 +6140,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B6" s="37">
         <v>113876</v>
@@ -6158,7 +6151,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B7" s="37">
         <v>39631</v>
@@ -6169,7 +6162,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B8" s="37">
         <v>1525514</v>
@@ -6180,7 +6173,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B9" s="37">
         <v>1495746</v>
@@ -6191,7 +6184,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B10" s="37">
         <v>116135</v>
@@ -6202,7 +6195,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B11" s="37">
         <v>365580900</v>

</xml_diff>

<commit_message>
add tier data for sftyAll tier
</commit_message>
<xml_diff>
--- a/model/RunControl.xlsx
+++ b/model/RunControl.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698A6160-4E3F-4A3D-8A68-6DEA67278BFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52630053-B6D0-4C63-B931-ACBC928F35B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-7590" windowWidth="16440" windowHeight="28440" tabRatio="524" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params_sim" sheetId="22" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="returns" sheetId="2" r:id="rId5"/>
     <sheet name="targetVals_2018" sheetId="20" r:id="rId6"/>
     <sheet name="targeVals_raw" sheetId="23" r:id="rId7"/>
-    <sheet name="shares" sheetId="24" r:id="rId8"/>
+    <sheet name="groupWgts" sheetId="24" r:id="rId8"/>
     <sheet name="Sheet1" sheetId="25" r:id="rId9"/>
     <sheet name="Sheet2" sheetId="26" r:id="rId10"/>
   </sheets>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="298">
   <si>
     <t>nsim</t>
   </si>
@@ -774,27 +774,9 @@
     <t>Contribution required (% current payroll)</t>
   </si>
   <si>
-    <t>misc t1</t>
-  </si>
-  <si>
-    <t>misc t2</t>
-  </si>
-  <si>
-    <t>inds t1</t>
-  </si>
-  <si>
-    <t>inds t2</t>
-  </si>
-  <si>
     <t>actives</t>
   </si>
   <si>
-    <t>retirees</t>
-  </si>
-  <si>
-    <t>AL</t>
-  </si>
-  <si>
     <t>discount rate</t>
   </si>
   <si>
@@ -1018,13 +1000,88 @@
   </si>
   <si>
     <t>lower cola assumption, high UAAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">misc </t>
+  </si>
+  <si>
+    <t>receiving pmt</t>
+  </si>
+  <si>
+    <t>AV2018 np15-19 2018-06-30</t>
+  </si>
+  <si>
+    <t>misc-classic</t>
+  </si>
+  <si>
+    <t>misc-PEPRA</t>
+  </si>
+  <si>
+    <t>CAFR2018-19 ep154 state members column 2018</t>
+  </si>
+  <si>
+    <t>safety-classic</t>
+  </si>
+  <si>
+    <t>safety-PEPRA</t>
+  </si>
+  <si>
+    <t>survivors&amp;beneficiaires</t>
+  </si>
+  <si>
+    <t>retireed</t>
+  </si>
+  <si>
+    <t>Total-classic</t>
+  </si>
+  <si>
+    <t>Total-PEPRA</t>
+  </si>
+  <si>
+    <t>For tier miscAll</t>
+  </si>
+  <si>
+    <t>misc-pepra</t>
+  </si>
+  <si>
+    <t>inds-classic</t>
+  </si>
+  <si>
+    <t>inds-pepra</t>
+  </si>
+  <si>
+    <t>Actives</t>
+  </si>
+  <si>
+    <t>safety-pepra</t>
+  </si>
+  <si>
+    <t>poff-classic</t>
+  </si>
+  <si>
+    <t>poff-pepra</t>
+  </si>
+  <si>
+    <t>chp-classic</t>
+  </si>
+  <si>
+    <t>chp-pepra</t>
+  </si>
+  <si>
+    <t>classic/pepra shares in type</t>
+  </si>
+  <si>
+    <t>share in tier</t>
+  </si>
+  <si>
+    <t>For tier sftyAll</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="8">
+  <numFmts count="9">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
@@ -1033,8 +1090,9 @@
     <numFmt numFmtId="167" formatCode="0.0%"/>
     <numFmt numFmtId="168" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="169" formatCode="0.000%"/>
+    <numFmt numFmtId="178" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1127,6 +1185,15 @@
       <color rgb="FF000000"/>
       <name val="Lucida Console"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1328,7 +1395,7 @@
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1416,6 +1483,8 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1834,11 +1903,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D014B46A-D012-4D18-AEAB-1D829080B2CE}">
   <dimension ref="A2:AP20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
+      <selection pane="bottomRight" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1894,12 +1963,12 @@
       </c>
       <c r="F3" s="19"/>
       <c r="G3" s="63" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="H3" s="63"/>
       <c r="I3" s="63"/>
       <c r="J3" s="57" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K3" s="57"/>
       <c r="L3" s="57"/>
@@ -1964,22 +2033,22 @@
         <v>171</v>
       </c>
       <c r="G4" s="64" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="H4" s="64" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="I4" s="64" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="J4" s="58" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="K4" s="58" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="L4" s="58" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="M4" s="10" t="s">
         <v>11</v>
@@ -2027,7 +2096,7 @@
         <v>47</v>
       </c>
       <c r="AB4" s="7" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="AC4" s="8" t="s">
         <v>57</v>
@@ -2048,7 +2117,7 @@
         <v>33</v>
       </c>
       <c r="AI4" s="8" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="AJ4" s="12" t="s">
         <v>59</v>
@@ -2134,7 +2203,7 @@
         <v>0</v>
       </c>
       <c r="V5" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="W5" t="s">
         <v>20</v>
@@ -2193,7 +2262,7 @@
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -2202,13 +2271,13 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
@@ -2253,7 +2322,7 @@
         <v>0</v>
       </c>
       <c r="V6" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="W6" t="s">
         <v>20</v>
@@ -2312,7 +2381,7 @@
     </row>
     <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
@@ -2321,13 +2390,13 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
@@ -2372,7 +2441,7 @@
         <v>0</v>
       </c>
       <c r="V7" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="W7" t="s">
         <v>20</v>
@@ -2393,10 +2462,10 @@
         <v>123</v>
       </c>
       <c r="AC7" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="AD7" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="AE7" s="24"/>
       <c r="AF7" s="24"/>
@@ -2433,7 +2502,7 @@
     </row>
     <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -2442,13 +2511,13 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -2493,7 +2562,7 @@
         <v>0</v>
       </c>
       <c r="V8" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="W8" t="s">
         <v>20</v>
@@ -2552,25 +2621,25 @@
     </row>
     <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
         <v>235</v>
       </c>
-      <c r="C10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s">
-        <v>241</v>
-      </c>
       <c r="F10" t="b">
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H10" t="b">
         <v>0</v>
@@ -2615,7 +2684,7 @@
         <v>0</v>
       </c>
       <c r="V10" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="W10" t="s">
         <v>20</v>
@@ -2674,25 +2743,25 @@
     </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="B11" t="s">
+        <v>230</v>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
         <v>236</v>
       </c>
-      <c r="C11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" t="s">
-        <v>242</v>
-      </c>
       <c r="F11" t="b">
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H11" t="b">
         <v>0</v>
@@ -2737,7 +2806,7 @@
         <v>0</v>
       </c>
       <c r="V11" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="W11" t="s">
         <v>20</v>
@@ -2758,10 +2827,10 @@
         <v>123</v>
       </c>
       <c r="AC11" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="AD11" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="AE11" s="24"/>
       <c r="AF11" s="24"/>
@@ -2798,10 +2867,10 @@
     </row>
     <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B12" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -2810,13 +2879,13 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H12" t="b">
         <v>1</v>
@@ -2861,7 +2930,7 @@
         <v>0</v>
       </c>
       <c r="V12" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="W12" t="s">
         <v>20</v>
@@ -2882,10 +2951,10 @@
         <v>123</v>
       </c>
       <c r="AC12" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="AD12" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="AE12" s="24"/>
       <c r="AF12" s="24"/>
@@ -2922,10 +2991,10 @@
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B14" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -2934,13 +3003,13 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H14" t="b">
         <v>0</v>
@@ -2985,7 +3054,7 @@
         <v>0</v>
       </c>
       <c r="V14" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="W14" t="s">
         <v>20</v>
@@ -3044,10 +3113,10 @@
     </row>
     <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="B15" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -3056,13 +3125,13 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H15" t="b">
         <v>0</v>
@@ -3107,7 +3176,7 @@
         <v>0</v>
       </c>
       <c r="V15" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="W15" t="s">
         <v>20</v>
@@ -3166,10 +3235,10 @@
     </row>
     <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="B16" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C16" t="b">
         <v>1</v>
@@ -3178,13 +3247,13 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H16" t="b">
         <v>1</v>
@@ -3229,7 +3298,7 @@
         <v>0</v>
       </c>
       <c r="V16" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="W16" t="s">
         <v>20</v>
@@ -3288,10 +3357,10 @@
     </row>
     <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="B18" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
@@ -3300,13 +3369,13 @@
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H18" t="b">
         <v>0</v>
@@ -3351,7 +3420,7 @@
         <v>0</v>
       </c>
       <c r="V18" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="W18" t="s">
         <v>20</v>
@@ -3410,10 +3479,10 @@
     </row>
     <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B19" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
@@ -3422,13 +3491,13 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H19" t="b">
         <v>1</v>
@@ -3473,7 +3542,7 @@
         <v>0</v>
       </c>
       <c r="V19" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="W19" t="s">
         <v>20</v>
@@ -3532,10 +3601,10 @@
     </row>
     <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B20" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C20" t="b">
         <v>1</v>
@@ -3544,13 +3613,13 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H20" t="b">
         <v>1</v>
@@ -3595,7 +3664,7 @@
         <v>0</v>
       </c>
       <c r="V20" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="W20" t="s">
         <v>20</v>
@@ -3688,12 +3757,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="B2" s="37">
         <v>80223070</v>
@@ -3705,7 +3774,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="B3" s="37">
         <f>3589902866/1000</f>
@@ -3718,7 +3787,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="B4" s="37">
         <f>SUM(B2:B3)</f>
@@ -3739,7 +3808,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="B5" s="65">
         <f>10551342261/1000</f>
@@ -3752,7 +3821,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="B6" s="65">
         <f>33326594392/1000</f>
@@ -3765,7 +3834,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="B7" s="65">
         <f>8540511923/1000</f>
@@ -3778,7 +3847,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B8" s="37">
         <f>136231421398/1000</f>
@@ -3795,7 +3864,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B10" s="37">
         <v>259890776</v>
@@ -3803,7 +3872,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B11" s="37">
         <v>64796136</v>
@@ -3811,7 +3880,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B12" s="37">
         <v>29308589</v>
@@ -3819,7 +3888,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="B14" s="37">
         <v>365580900</v>
@@ -3880,14 +3949,14 @@
       </c>
       <c r="I3" s="18"/>
       <c r="J3" s="59" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="K3" s="57" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="L3" s="57"/>
       <c r="M3" s="57" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3922,28 +3991,28 @@
         <v>6</v>
       </c>
       <c r="K4" s="58" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="L4" s="58" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="M4" s="58" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="N4" s="12" t="s">
         <v>59</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -4001,7 +4070,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -4051,7 +4120,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
@@ -4104,7 +4173,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -4157,7 +4226,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -4210,7 +4279,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -4263,7 +4332,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -4432,7 +4501,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4515,7 +4584,7 @@
         <v>0.03</v>
       </c>
       <c r="G3" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -4540,12 +4609,12 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G4" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B5" s="4">
         <v>7.0000000000000007E-2</v>
@@ -4570,7 +4639,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B6" s="4">
         <v>0.03</v>
@@ -4589,12 +4658,12 @@
         <v>0.02</v>
       </c>
       <c r="G6" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B7" s="4">
         <v>-0.24</v>
@@ -4619,7 +4688,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B8" s="4">
         <v>0.12</v>
@@ -4644,7 +4713,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B9" s="4">
         <v>0.12</v>
@@ -4669,7 +4738,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B10" s="4">
         <v>0.12</v>
@@ -4694,7 +4763,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B11" s="4">
         <v>7.0000000000000007E-2</v>
@@ -4714,7 +4783,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G11" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -4728,7 +4797,7 @@
   <dimension ref="A1:M58"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6035,41 +6104,351 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3E00125-AE25-4C2C-BBE6-6A6AFF0CBB38}">
-  <dimension ref="A3:E7"/>
+  <dimension ref="A2:N27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" customWidth="1"/>
+    <col min="9" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>275</v>
+      </c>
+      <c r="I2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C3" t="s">
-        <v>198</v>
-      </c>
-      <c r="D3" t="s">
-        <v>199</v>
-      </c>
-      <c r="E3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>203</v>
+      <c r="B4" s="37">
+        <v>174402</v>
+      </c>
+      <c r="C4" s="37">
+        <v>11811</v>
+      </c>
+      <c r="D4" s="37">
+        <v>28335</v>
+      </c>
+      <c r="E4" s="37">
+        <v>41289</v>
+      </c>
+      <c r="F4" s="37">
+        <v>7311</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="I4" s="37">
+        <v>200645</v>
+      </c>
+      <c r="J4" s="37">
+        <v>76222</v>
+      </c>
+      <c r="K4" s="37">
+        <v>64165</v>
+      </c>
+      <c r="L4" s="37">
+        <v>26540</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B5" s="37">
+        <v>195158</v>
+      </c>
+      <c r="C5" s="37">
+        <v>14642</v>
+      </c>
+      <c r="D5" s="37">
+        <v>25749</v>
+      </c>
+      <c r="E5" s="37">
+        <v>39947</v>
+      </c>
+      <c r="F5" s="37">
+        <v>9158</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="I5" s="37"/>
+      <c r="M5" s="37">
+        <v>595483</v>
+      </c>
+      <c r="N5" s="37">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="H6" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="M6" s="37">
+        <v>98457</v>
+      </c>
+      <c r="N6">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="67" t="s">
+        <v>296</v>
+      </c>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="H7" s="1"/>
+      <c r="M7" s="37"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B8" s="68">
+        <f>B4/SUM($B4:$C4)</f>
+        <v>0.93657263456364481</v>
+      </c>
+      <c r="C8" s="68">
+        <f>C4/SUM($B4:$C4)</f>
+        <v>6.3427365436355146E-2</v>
+      </c>
+      <c r="D8" s="68">
+        <f>D4/SUM($D4:$F4)</f>
+        <v>0.36829791382335736</v>
+      </c>
+      <c r="E8" s="68">
+        <f t="shared" ref="E8:F9" si="0">E4/SUM($D4:$F4)</f>
+        <v>0.5366738155585884</v>
+      </c>
+      <c r="F8" s="68">
+        <f t="shared" si="0"/>
+        <v>9.5028270618054203E-2</v>
+      </c>
+      <c r="H8" s="67" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B9" s="68">
+        <f>B5/SUM($B5:$C5)</f>
+        <v>0.93020972354623455</v>
+      </c>
+      <c r="C9" s="68">
+        <f>C5/SUM($B5:$C5)</f>
+        <v>6.9790276453765496E-2</v>
+      </c>
+      <c r="D9" s="68">
+        <f>D5/SUM($D5:$F5)</f>
+        <v>0.34398963315253694</v>
+      </c>
+      <c r="E9" s="68">
+        <f t="shared" si="0"/>
+        <v>0.53366553557592111</v>
+      </c>
+      <c r="F9" s="68">
+        <f t="shared" si="0"/>
+        <v>0.12234483127154193</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="I9" s="24">
+        <f>I4/SUM($I4:$J4)</f>
+        <v>0.72469814026229196</v>
+      </c>
+      <c r="J9" s="24">
+        <f>J4/SUM($I4:$J4)</f>
+        <v>0.27530185973770799</v>
+      </c>
+      <c r="K9" s="24">
+        <f>K4/SUM($K4:$L4)</f>
+        <v>0.70740312000440986</v>
+      </c>
+      <c r="L9" s="24">
+        <f>L4/SUM($K4:$L4)</f>
+        <v>0.29259687999559009</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="H10" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="M10" s="24">
+        <f>M5/SUM($M5:$N5)</f>
+        <v>0.99910405240118993</v>
+      </c>
+      <c r="N10" s="24">
+        <f>N5/SUM($M5:$N5)</f>
+        <v>8.9594759881010102E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H11" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="M11" s="24">
+        <f>M6/SUM($M6:$N6)</f>
+        <v>0.9990259048430794</v>
+      </c>
+      <c r="N11" s="24">
+        <f>N6/SUM($M6:$N6)</f>
+        <v>9.7409515692064165E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>279</v>
+      </c>
+      <c r="B22" s="4">
+        <f>D8*K9</f>
+        <v>0.26053509332975827</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>290</v>
+      </c>
+      <c r="B23" s="4">
+        <f>D8*L9</f>
+        <v>0.10776282049359907</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>291</v>
+      </c>
+      <c r="B24" s="4">
+        <f>E8*K9</f>
+        <v>0.37964473155081663</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>292</v>
+      </c>
+      <c r="B25" s="4">
+        <f>E8*L9</f>
+        <v>0.15702908400777174</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>293</v>
+      </c>
+      <c r="B26" s="4">
+        <f>F8*K9</f>
+        <v>6.7223295123834931E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>294</v>
+      </c>
+      <c r="B27" s="4">
+        <f>F8*L9</f>
+        <v>2.7804975494219265E-2</v>
       </c>
     </row>
   </sheetData>
@@ -6082,7 +6461,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6094,20 +6473,20 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C1" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B3" s="37">
         <v>259890776</v>
@@ -6118,7 +6497,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B4" s="37">
         <v>64796136</v>
@@ -6129,7 +6508,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B5" s="37">
         <v>29308589</v>
@@ -6140,7 +6519,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B6" s="37">
         <v>113876</v>
@@ -6151,7 +6530,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="B7" s="37">
         <v>39631</v>
@@ -6162,7 +6541,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B8" s="37">
         <v>1525514</v>
@@ -6173,7 +6552,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B9" s="37">
         <v>1495746</v>
@@ -6184,7 +6563,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="B10" s="37">
         <v>116135</v>
@@ -6195,7 +6574,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="B11" s="37">
         <v>365580900</v>

</xml_diff>

<commit_message>
add html notebook for prelim results
</commit_message>
<xml_diff>
--- a/model/RunControl.xlsx
+++ b/model/RunControl.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7DD7A0-A178-4A71-A3B5-D50740277438}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FE92AE-D76D-427D-A800-EC185B9DA8F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="18240" windowHeight="28440" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params_sim" sheetId="22" r:id="rId1"/>
@@ -626,9 +626,6 @@
     <t>twoTiers_cola_highERC</t>
   </si>
   <si>
-    <t>twoTiers_bf1&amp;cola_highERC</t>
-  </si>
-  <si>
     <t>combine the two "lowERC" runs</t>
   </si>
   <si>
@@ -860,12 +857,6 @@
     <t>sftyAll_bf75_cola1p5</t>
   </si>
   <si>
-    <t>sftyAll_benCut2&amp;colaCut2_lowERC</t>
-  </si>
-  <si>
-    <t>sftyAll_benCut2&amp;colsCut2_highERC</t>
-  </si>
-  <si>
     <t>miscAll_baseline</t>
   </si>
   <si>
@@ -902,12 +893,6 @@
     <t>miscAll_colaCut1_highERC</t>
   </si>
   <si>
-    <t>miscAll_benCut1&amp;colaCut1_lowERC</t>
-  </si>
-  <si>
-    <t>miscAll_benCut1&amp;colaCut1_highERC</t>
-  </si>
-  <si>
     <t>Misc members: baseline</t>
   </si>
   <si>
@@ -938,12 +923,6 @@
     <t>sftyAll_benCut1_highERC</t>
   </si>
   <si>
-    <t>sftyAll_benCut1&amp;colaCut1_lowERC</t>
-  </si>
-  <si>
-    <t>sftyAll_benCut1&amp;colsCut1_highERC</t>
-  </si>
-  <si>
     <t>miscAll_benCut2_lowERC</t>
   </si>
   <si>
@@ -956,12 +935,6 @@
     <t>miscAll_colaCut2_highERC</t>
   </si>
   <si>
-    <t>miscAll_benCut2&amp;colaCut2_lowERC</t>
-  </si>
-  <si>
-    <t>miscAll_benCut2&amp;colaCut2_highERC</t>
-  </si>
-  <si>
     <t>sftyAll_bf50_cola2</t>
   </si>
   <si>
@@ -1011,6 +984,33 @@
   </si>
   <si>
     <t>miscAll, 1.5%bfactor(new), 1.5%cola</t>
+  </si>
+  <si>
+    <t>miscAll_benCut1_colaCut1_lowERC</t>
+  </si>
+  <si>
+    <t>miscAll_benCut1_colaCut1_highERC</t>
+  </si>
+  <si>
+    <t>miscAll_benCut2_colaCut2_lowERC</t>
+  </si>
+  <si>
+    <t>miscAll_benCut2_colaCut2_highERC</t>
+  </si>
+  <si>
+    <t>sftyAll_benCut1_colaCut1_lowERC</t>
+  </si>
+  <si>
+    <t>sftyAll_benCut1_colsCut1_highERC</t>
+  </si>
+  <si>
+    <t>sftyAll_benCut2_colaCut2_lowERC</t>
+  </si>
+  <si>
+    <t>sftyAll_benCut2_colsCut2_highERC</t>
+  </si>
+  <si>
+    <t>twoTiers_bf1_cola_highERC</t>
   </si>
 </sst>
 </file>
@@ -1675,17 +1675,17 @@
   <dimension ref="A2:AP60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B65" sqref="B65"/>
+      <selection pane="bottomRight" activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.42578125" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
@@ -2392,15 +2392,15 @@
     </row>
     <row r="9" spans="1:42">
       <c r="B9" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:42">
       <c r="A10" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B10" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
@@ -2409,13 +2409,13 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H10" t="b">
         <v>0</v>
@@ -2528,7 +2528,7 @@
     </row>
     <row r="12" spans="1:42">
       <c r="B12" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="Z12" s="3"/>
       <c r="AA12" s="5"/>
@@ -2540,7 +2540,7 @@
     </row>
     <row r="13" spans="1:42">
       <c r="A13" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B13" t="s">
         <v>138</v>
@@ -2552,13 +2552,13 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H13" t="b">
         <v>0</v>
@@ -2664,10 +2664,10 @@
     </row>
     <row r="14" spans="1:42">
       <c r="A14" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C14" t="b">
         <v>1</v>
@@ -2676,13 +2676,13 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H14" t="b">
         <v>1</v>
@@ -2788,7 +2788,7 @@
     </row>
     <row r="16" spans="1:42">
       <c r="A16" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B16" t="s">
         <v>136</v>
@@ -2800,13 +2800,13 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H16" t="b">
         <v>0</v>
@@ -2910,10 +2910,10 @@
     </row>
     <row r="17" spans="1:42">
       <c r="A17" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C17" t="b">
         <v>1</v>
@@ -2922,13 +2922,13 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H17" t="b">
         <v>1</v>
@@ -3032,10 +3032,10 @@
     </row>
     <row r="19" spans="1:42">
       <c r="A19" t="s">
-        <v>237</v>
+        <v>265</v>
       </c>
       <c r="B19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C19" t="b">
         <v>1</v>
@@ -3044,13 +3044,13 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H19" t="b">
         <v>0</v>
@@ -3154,10 +3154,10 @@
     </row>
     <row r="20" spans="1:42">
       <c r="A20" t="s">
-        <v>238</v>
+        <v>266</v>
       </c>
       <c r="B20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C20" t="b">
         <v>1</v>
@@ -3166,13 +3166,13 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H20" t="b">
         <v>1</v>
@@ -3285,7 +3285,7 @@
     </row>
     <row r="22" spans="1:42">
       <c r="B22" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C22" t="b">
         <v>1</v>
@@ -3293,7 +3293,7 @@
     </row>
     <row r="23" spans="1:42">
       <c r="A23" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="B23" t="s">
         <v>138</v>
@@ -3305,13 +3305,13 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H23" t="b">
         <v>0</v>
@@ -3417,10 +3417,10 @@
     </row>
     <row r="24" spans="1:42">
       <c r="A24" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="B24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C24" t="b">
         <v>1</v>
@@ -3429,13 +3429,13 @@
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="F24" t="b">
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H24" t="b">
         <v>1</v>
@@ -3541,7 +3541,7 @@
     </row>
     <row r="26" spans="1:42">
       <c r="A26" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="B26" t="s">
         <v>136</v>
@@ -3553,13 +3553,13 @@
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H26" t="b">
         <v>0</v>
@@ -3663,10 +3663,10 @@
     </row>
     <row r="27" spans="1:42">
       <c r="A27" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="B27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C27" t="b">
         <v>1</v>
@@ -3675,13 +3675,13 @@
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H27" t="b">
         <v>1</v>
@@ -3785,10 +3785,10 @@
     </row>
     <row r="29" spans="1:42">
       <c r="A29" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="B29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C29" t="b">
         <v>1</v>
@@ -3797,13 +3797,13 @@
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="F29" t="b">
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H29" t="b">
         <v>0</v>
@@ -3907,10 +3907,10 @@
     </row>
     <row r="30" spans="1:42">
       <c r="A30" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="B30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C30" t="b">
         <v>1</v>
@@ -3919,13 +3919,13 @@
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="F30" t="b">
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H30" t="b">
         <v>1</v>
@@ -4029,30 +4029,30 @@
     </row>
     <row r="34" spans="1:42">
       <c r="B34" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="35" spans="1:42">
       <c r="A35" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B35" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35" t="b">
         <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F35" t="b">
         <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H35" t="b">
         <v>0</v>
@@ -4165,7 +4165,7 @@
     </row>
     <row r="37" spans="1:42">
       <c r="B37" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="Z37" s="3"/>
       <c r="AA37" s="5"/>
@@ -4177,25 +4177,25 @@
     </row>
     <row r="38" spans="1:42">
       <c r="A38" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B38" t="s">
         <v>138</v>
       </c>
       <c r="C38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" t="b">
         <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="F38" t="b">
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H38" t="b">
         <v>0</v>
@@ -4301,25 +4301,25 @@
     </row>
     <row r="39" spans="1:42">
       <c r="A39" t="s">
+        <v>243</v>
+      </c>
+      <c r="B39" t="s">
+        <v>199</v>
+      </c>
+      <c r="C39" t="b">
+        <v>0</v>
+      </c>
+      <c r="D39" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
         <v>248</v>
       </c>
-      <c r="B39" t="s">
-        <v>200</v>
-      </c>
-      <c r="C39" t="b">
-        <v>1</v>
-      </c>
-      <c r="D39" t="b">
-        <v>0</v>
-      </c>
-      <c r="E39" t="s">
-        <v>257</v>
-      </c>
       <c r="F39" t="b">
         <v>0</v>
       </c>
       <c r="G39" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H39" t="b">
         <v>1</v>
@@ -4429,25 +4429,25 @@
     </row>
     <row r="41" spans="1:42">
       <c r="A41" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B41" t="s">
         <v>136</v>
       </c>
       <c r="C41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41" t="b">
         <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F41" t="b">
         <v>0</v>
       </c>
       <c r="G41" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H41" t="b">
         <v>0</v>
@@ -4551,25 +4551,25 @@
     </row>
     <row r="42" spans="1:42">
       <c r="A42" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B42" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D42" t="b">
         <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F42" t="b">
         <v>0</v>
       </c>
       <c r="G42" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H42" t="b">
         <v>1</v>
@@ -4673,25 +4673,25 @@
     </row>
     <row r="44" spans="1:42">
       <c r="A44" t="s">
+        <v>269</v>
+      </c>
+      <c r="B44" t="s">
+        <v>145</v>
+      </c>
+      <c r="C44" t="b">
+        <v>0</v>
+      </c>
+      <c r="D44" t="b">
+        <v>0</v>
+      </c>
+      <c r="E44" t="s">
         <v>249</v>
       </c>
-      <c r="B44" t="s">
-        <v>146</v>
-      </c>
-      <c r="C44" t="b">
-        <v>1</v>
-      </c>
-      <c r="D44" t="b">
-        <v>0</v>
-      </c>
-      <c r="E44" t="s">
-        <v>258</v>
-      </c>
       <c r="F44" t="b">
         <v>0</v>
       </c>
       <c r="G44" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H44" t="b">
         <v>0</v>
@@ -4795,25 +4795,25 @@
     </row>
     <row r="45" spans="1:42">
       <c r="A45" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="B45" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D45" t="b">
         <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="F45" t="b">
         <v>0</v>
       </c>
       <c r="G45" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H45" t="b">
         <v>1</v>
@@ -4926,7 +4926,7 @@
     </row>
     <row r="47" spans="1:42">
       <c r="B47" s="1" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="Z47" s="3"/>
       <c r="AA47" s="5"/>
@@ -4938,7 +4938,7 @@
     </row>
     <row r="48" spans="1:42">
       <c r="A48" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B48" t="s">
         <v>138</v>
@@ -4950,13 +4950,13 @@
         <v>0</v>
       </c>
       <c r="E48" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F48" t="b">
         <v>0</v>
       </c>
       <c r="G48" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H48" t="b">
         <v>0</v>
@@ -5062,10 +5062,10 @@
     </row>
     <row r="49" spans="1:42">
       <c r="A49" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B49" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C49" t="b">
         <v>0</v>
@@ -5074,13 +5074,13 @@
         <v>0</v>
       </c>
       <c r="E49" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F49" t="b">
         <v>0</v>
       </c>
       <c r="G49" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H49" t="b">
         <v>1</v>
@@ -5190,7 +5190,7 @@
     </row>
     <row r="51" spans="1:42">
       <c r="A51" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B51" t="s">
         <v>136</v>
@@ -5202,13 +5202,13 @@
         <v>0</v>
       </c>
       <c r="E51" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F51" t="b">
         <v>0</v>
       </c>
       <c r="G51" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H51" t="b">
         <v>0</v>
@@ -5312,10 +5312,10 @@
     </row>
     <row r="52" spans="1:42">
       <c r="A52" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B52" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C52" t="b">
         <v>0</v>
@@ -5324,13 +5324,13 @@
         <v>0</v>
       </c>
       <c r="E52" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F52" t="b">
         <v>0</v>
       </c>
       <c r="G52" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H52" t="b">
         <v>1</v>
@@ -5434,10 +5434,10 @@
     </row>
     <row r="54" spans="1:42">
       <c r="A54" t="s">
-        <v>223</v>
+        <v>271</v>
       </c>
       <c r="B54" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C54" t="b">
         <v>0</v>
@@ -5446,13 +5446,13 @@
         <v>0</v>
       </c>
       <c r="E54" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F54" t="b">
         <v>0</v>
       </c>
       <c r="G54" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H54" t="b">
         <v>0</v>
@@ -5556,10 +5556,10 @@
     </row>
     <row r="55" spans="1:42">
       <c r="A55" t="s">
-        <v>224</v>
+        <v>272</v>
       </c>
       <c r="B55" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C55" t="b">
         <v>0</v>
@@ -5568,13 +5568,13 @@
         <v>0</v>
       </c>
       <c r="E55" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F55" t="b">
         <v>0</v>
       </c>
       <c r="G55" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H55" t="b">
         <v>1</v>
@@ -5678,7 +5678,7 @@
     </row>
     <row r="58" spans="1:42">
       <c r="B58" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="59" spans="1:42">
@@ -5805,10 +5805,10 @@
     </row>
     <row r="60" spans="1:42">
       <c r="A60" t="s">
-        <v>145</v>
+        <v>273</v>
       </c>
       <c r="B60" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C60" t="b">
         <v>0</v>
@@ -5951,7 +5951,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B57" sqref="B57"/>
+      <selection pane="bottomRight" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5999,14 +5999,14 @@
       </c>
       <c r="L3" s="39"/>
       <c r="M3" s="39" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="N3" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O3" s="19"/>
       <c r="P3" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Q3" s="15"/>
       <c r="R3" s="15"/>
@@ -6122,10 +6122,10 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -6175,13 +6175,13 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="B8" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
         <v>70</v>
@@ -6228,10 +6228,10 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C9" t="b">
         <v>1</v>
@@ -6284,10 +6284,10 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C11" t="b">
         <v>1</v>
@@ -6340,13 +6340,13 @@
     </row>
     <row r="12" spans="1:18">
       <c r="A12" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="B12" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="C12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" t="s">
         <v>70</v>
@@ -6396,10 +6396,10 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C13" t="b">
         <v>1</v>
@@ -6452,10 +6452,10 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C15" t="b">
         <v>1</v>
@@ -6508,13 +6508,13 @@
     </row>
     <row r="16" spans="1:18">
       <c r="A16" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="B16" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="C16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" t="s">
         <v>70</v>
@@ -6564,10 +6564,10 @@
     </row>
     <row r="17" spans="1:18">
       <c r="A17" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C17" t="b">
         <v>1</v>
@@ -6620,10 +6620,10 @@
     </row>
     <row r="20" spans="1:18">
       <c r="A20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B20" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -6632,7 +6632,7 @@
         <v>70</v>
       </c>
       <c r="E20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F20" t="s">
         <v>68</v>
@@ -6673,10 +6673,10 @@
     </row>
     <row r="21" spans="1:18">
       <c r="A21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B21" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -6685,7 +6685,7 @@
         <v>70</v>
       </c>
       <c r="E21" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F21" t="s">
         <v>68</v>
@@ -6726,19 +6726,19 @@
     </row>
     <row r="22" spans="1:18">
       <c r="A22" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B22" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="C22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" t="s">
         <v>70</v>
       </c>
       <c r="E22" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F22" t="s">
         <v>68</v>
@@ -6782,10 +6782,10 @@
     </row>
     <row r="24" spans="1:18">
       <c r="A24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B24" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
@@ -6794,7 +6794,7 @@
         <v>70</v>
       </c>
       <c r="E24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F24" t="s">
         <v>68</v>
@@ -6838,10 +6838,10 @@
     </row>
     <row r="25" spans="1:18">
       <c r="A25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B25" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
@@ -6850,7 +6850,7 @@
         <v>70</v>
       </c>
       <c r="E25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F25" t="s">
         <v>68</v>
@@ -6894,19 +6894,19 @@
     </row>
     <row r="26" spans="1:18">
       <c r="A26" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B26" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="C26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" t="s">
         <v>70</v>
       </c>
       <c r="E26" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F26" t="s">
         <v>68</v>
@@ -6950,10 +6950,10 @@
     </row>
     <row r="28" spans="1:18">
       <c r="A28" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B28" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
@@ -6962,7 +6962,7 @@
         <v>70</v>
       </c>
       <c r="E28" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F28" t="s">
         <v>68</v>
@@ -7006,10 +7006,10 @@
     </row>
     <row r="29" spans="1:18">
       <c r="A29" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B29" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
@@ -7018,7 +7018,7 @@
         <v>70</v>
       </c>
       <c r="E29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F29" t="s">
         <v>68</v>
@@ -7062,19 +7062,19 @@
     </row>
     <row r="30" spans="1:18">
       <c r="A30" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B30" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="C30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" t="s">
         <v>70</v>
       </c>
       <c r="E30" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F30" t="s">
         <v>68</v>
@@ -7136,7 +7136,7 @@
   <dimension ref="A3:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7533,7 +7533,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A25" sqref="A25:XFD25"/>
+      <selection pane="bottomRight" activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -7549,7 +7549,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="26" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -7563,16 +7563,16 @@
         <v>85</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G3" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="H3" s="29" t="s">
         <v>208</v>
       </c>
-      <c r="H3" s="29" t="s">
+      <c r="I3" s="29" t="s">
         <v>209</v>
-      </c>
-      <c r="I3" s="29" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -8383,7 +8383,7 @@
   <dimension ref="A2:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8400,46 +8400,46 @@
   <sheetData>
     <row r="2" spans="1:14">
       <c r="B2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="I3" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>174</v>
-      </c>
       <c r="K3" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="M3" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -8479,7 +8479,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B5" s="24">
         <v>195158</v>
@@ -8497,7 +8497,7 @@
         <v>9158</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I5" s="24"/>
       <c r="M5" s="24">
@@ -8514,7 +8514,7 @@
       <c r="E6" s="24"/>
       <c r="F6" s="24"/>
       <c r="H6" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M6" s="24">
         <v>98457</v>
@@ -8525,7 +8525,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="49" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="24"/>
@@ -8560,12 +8560,12 @@
         <v>9.5028270618054203E-2</v>
       </c>
       <c r="H8" s="49" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B9" s="50">
         <f>B5/SUM($B5:$C5)</f>
@@ -8614,7 +8614,7 @@
       <c r="E10" s="24"/>
       <c r="F10" s="24"/>
       <c r="H10" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M10" s="23">
         <f>M5/SUM($M5:$N5)</f>
@@ -8627,7 +8627,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="H11" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M11" s="23">
         <f>M6/SUM($M6:$N6)</f>
@@ -8640,42 +8640,42 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B22" s="4">
         <f>D8*K9</f>
@@ -8684,7 +8684,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B23" s="4">
         <f>D8*L9</f>
@@ -8693,7 +8693,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B24" s="4">
         <f>E8*K9</f>
@@ -8702,7 +8702,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B25" s="4">
         <f>E8*L9</f>
@@ -8711,7 +8711,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B26" s="4">
         <f>F8*K9</f>
@@ -8720,7 +8720,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B27" s="4">
         <f>F8*L9</f>
@@ -8749,20 +8749,20 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="B1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="C2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B3" s="24">
         <v>259890776</v>
@@ -8773,7 +8773,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B4" s="24">
         <v>64796136</v>
@@ -8784,7 +8784,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B5" s="24">
         <v>29308589</v>
@@ -8795,7 +8795,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B6" s="24">
         <v>113876</v>
@@ -8806,7 +8806,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B7" s="24">
         <v>39631</v>
@@ -8817,7 +8817,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B8" s="24">
         <v>1525514</v>
@@ -8828,7 +8828,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B9" s="24">
         <v>1495746</v>
@@ -8839,7 +8839,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B10" s="24">
         <v>116135</v>
@@ -8850,7 +8850,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B11" s="24">
         <v>365580900</v>
@@ -8894,12 +8894,12 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B2" s="24">
         <v>80223070</v>
@@ -8911,7 +8911,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B3" s="24">
         <f>3589902866/1000</f>
@@ -8924,7 +8924,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B4" s="24">
         <f>SUM(B2:B3)</f>
@@ -8945,7 +8945,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B5" s="47">
         <f>10551342261/1000</f>
@@ -8958,7 +8958,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B6" s="47">
         <f>33326594392/1000</f>
@@ -8971,7 +8971,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B7" s="47">
         <f>8540511923/1000</f>
@@ -8984,7 +8984,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B8" s="24">
         <f>136231421398/1000</f>
@@ -9001,7 +9001,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B10" s="24">
         <v>259890776</v>
@@ -9009,7 +9009,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B11" s="24">
         <v>64796136</v>
@@ -9017,7 +9017,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B12" s="24">
         <v>29308589</v>
@@ -9025,7 +9025,7 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B14" s="24">
         <v>365580900</v>

</xml_diff>

<commit_message>
remove older versions of files
</commit_message>
<xml_diff>
--- a/model/RunControl.xlsx
+++ b/model/RunControl.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FE92AE-D76D-427D-A800-EC185B9DA8F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDDD273-A46A-4A86-8A94-B9D459EC1D6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1675,10 +1675,10 @@
   <dimension ref="A2:AP60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A62" sqref="A62"/>
+      <selection pane="bottomRight" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2546,7 +2546,7 @@
         <v>138</v>
       </c>
       <c r="C13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
@@ -2670,7 +2670,7 @@
         <v>199</v>
       </c>
       <c r="C14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
@@ -2794,7 +2794,7 @@
         <v>136</v>
       </c>
       <c r="C16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
@@ -2916,7 +2916,7 @@
         <v>168</v>
       </c>
       <c r="C17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
@@ -3038,7 +3038,7 @@
         <v>145</v>
       </c>
       <c r="C19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" t="b">
         <v>0</v>
@@ -3160,7 +3160,7 @@
         <v>146</v>
       </c>
       <c r="C20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
@@ -3288,7 +3288,7 @@
         <v>236</v>
       </c>
       <c r="C22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:42">
@@ -3299,7 +3299,7 @@
         <v>138</v>
       </c>
       <c r="C23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" t="b">
         <v>0</v>
@@ -3423,7 +3423,7 @@
         <v>199</v>
       </c>
       <c r="C24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" t="b">
         <v>0</v>
@@ -3547,7 +3547,7 @@
         <v>136</v>
       </c>
       <c r="C26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
@@ -3669,7 +3669,7 @@
         <v>168</v>
       </c>
       <c r="C27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" t="b">
         <v>0</v>
@@ -3791,7 +3791,7 @@
         <v>145</v>
       </c>
       <c r="C29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29" t="b">
         <v>0</v>
@@ -3913,7 +3913,7 @@
         <v>146</v>
       </c>
       <c r="C30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
@@ -4040,7 +4040,7 @@
         <v>238</v>
       </c>
       <c r="C35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" t="b">
         <v>0</v>
@@ -5927,7 +5927,7 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK5:AL8 C5:C8 AK10:AL14 AK51:AL52 AK54:AL55 AK16:AL17 AK44:AL49 AK19:AL21 AK59:AL60 C59:C60 AK23:AL24 AK26:AL27 AK41:AL42 AK29:AL30 C10:C30 AK35:AL39 C35:C55" xr:uid="{1240F49A-5091-456D-B77A-0673AD56E758}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK5:AL8 C5:C8 AK10:AL14 AK51:AL52 AK54:AL55 AK16:AL17 AK44:AL49 AK19:AL21 AK59:AL60 C59:C60 AK23:AL24 AK26:AL27 AK41:AL42 AK29:AL30 C35:C55 AK35:AL39 C10:C30" xr:uid="{1240F49A-5091-456D-B77A-0673AD56E758}">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V5:V8 V10:V14 V51:V52 V29:V30 V54:V55 V16:V17 V19:V21 V59:V60 V23:V24 V26:V27 V35:V39 V44:V49 V41:V42" xr:uid="{8909875A-86FC-4594-BBAF-A364A5851F3C}">

</xml_diff>

<commit_message>
multiple tiers, step 1
</commit_message>
<xml_diff>
--- a/model/RunControl.xlsx
+++ b/model/RunControl.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBCB44C-D1A2-49C7-9FFD-16C34F1BBB22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE0E58E-CA1F-4D70-B156-6DDE22B8A248}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6270" windowWidth="29040" windowHeight="15840" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1845" windowWidth="29040" windowHeight="15840" tabRatio="524" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params_sim" sheetId="22" r:id="rId1"/>
@@ -216,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="301">
   <si>
     <t>nsim</t>
   </si>
@@ -1173,6 +1173,15 @@
   </si>
   <si>
     <t>sftyAll_colaCut2lowerDR_highERC</t>
+  </si>
+  <si>
+    <t>mix_bf100_cola2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mix of miscAll and sftyAll, current policy, for testing </t>
+  </si>
+  <si>
+    <t>"miscAll","sftyAll"</t>
   </si>
 </sst>
 </file>
@@ -1861,11 +1870,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D014B46A-D012-4D18-AEAB-1D829080B2CE}">
   <dimension ref="A2:AR70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="G32" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="G41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C65" sqref="C65"/>
+      <selection pane="bottomRight" activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6701,26 +6710,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62142380-6405-410A-A4D9-17F48F5CE536}">
-  <dimension ref="A3:R37"/>
+  <dimension ref="A3:R39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="G14" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="J14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E49" sqref="E49"/>
+      <selection pane="bottomRight" activeCell="Q42" sqref="Q42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="50" customWidth="1"/>
+    <col min="2" max="2" width="56.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" customWidth="1"/>
     <col min="6" max="6" width="17.140625" customWidth="1"/>
     <col min="7" max="7" width="21.7109375" customWidth="1"/>
     <col min="8" max="9" width="17.42578125" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" customWidth="1"/>
+    <col min="10" max="10" width="24" customWidth="1"/>
     <col min="11" max="11" width="19.7109375" customWidth="1"/>
     <col min="12" max="12" width="22" customWidth="1"/>
     <col min="13" max="13" width="23.42578125" customWidth="1"/>
@@ -7883,7 +7892,7 @@
         <v>287</v>
       </c>
       <c r="C33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" t="s">
         <v>70</v>
@@ -7936,7 +7945,7 @@
         <v>288</v>
       </c>
       <c r="C34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" t="s">
         <v>70</v>
@@ -7989,7 +7998,7 @@
         <v>289</v>
       </c>
       <c r="C36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D36" t="s">
         <v>70</v>
@@ -8045,7 +8054,7 @@
         <v>290</v>
       </c>
       <c r="C37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D37" t="s">
         <v>70</v>
@@ -8093,12 +8102,65 @@
         <v>0</v>
       </c>
     </row>
+    <row r="39" spans="1:18">
+      <c r="A39" t="s">
+        <v>298</v>
+      </c>
+      <c r="B39" t="s">
+        <v>299</v>
+      </c>
+      <c r="C39" t="b">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>70</v>
+      </c>
+      <c r="E39" t="s">
+        <v>300</v>
+      </c>
+      <c r="F39" t="s">
+        <v>68</v>
+      </c>
+      <c r="G39">
+        <v>2.75E-2</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39" t="b">
+        <v>1</v>
+      </c>
+      <c r="J39">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+      <c r="L39">
+        <v>2018</v>
+      </c>
+      <c r="N39" t="b">
+        <v>1</v>
+      </c>
+      <c r="O39" s="43">
+        <v>0.11</v>
+      </c>
+      <c r="P39">
+        <v>0.03</v>
+      </c>
+      <c r="Q39">
+        <v>0.05</v>
+      </c>
+      <c r="R39">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D24:D26 D5:D9 D11:D13 D28:D31 D20:D22 D15:D17 D33:D34 D36:D37" xr:uid="{73B0AF26-6A4C-427C-B7EA-75439AFB0B6E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D24:D26 D5:D9 D11:D13 D28:D31 D20:D22 D15:D17 D33:D34 D36:D37 D39" xr:uid="{73B0AF26-6A4C-427C-B7EA-75439AFB0B6E}">
       <formula1>"singleTier,multiTier"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C36:C37 C33:C34 C5:C31" xr:uid="{BD331DEC-2DB8-437E-B2EB-02992BFDA38C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C33:C37 C5:C31 C39" xr:uid="{BD331DEC-2DB8-437E-B2EB-02992BFDA38C}">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8113,7 +8175,7 @@
   <dimension ref="A3:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
first working version with multiple tiers in a single run
</commit_message>
<xml_diff>
--- a/model/RunControl.xlsx
+++ b/model/RunControl.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE0E58E-CA1F-4D70-B156-6DDE22B8A248}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFAF636-7207-4B64-A8BC-C0E3778EC6AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1845" windowWidth="29040" windowHeight="15840" tabRatio="524" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params_sim" sheetId="22" r:id="rId1"/>
@@ -216,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="302">
   <si>
     <t>nsim</t>
   </si>
@@ -1182,6 +1182,9 @@
   </si>
   <si>
     <t>"miscAll","sftyAll"</t>
+  </si>
+  <si>
+    <t>mix_baseline</t>
   </si>
 </sst>
 </file>
@@ -1870,11 +1873,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D014B46A-D012-4D18-AEAB-1D829080B2CE}">
   <dimension ref="A2:AR70"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="G41" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="D41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B62" sqref="B62"/>
+      <selection pane="bottomRight" activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5901,7 +5904,7 @@
         <v>136</v>
       </c>
       <c r="C59" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D59" t="b">
         <v>0</v>
@@ -6029,7 +6032,7 @@
         <v>168</v>
       </c>
       <c r="C60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D60" t="b">
         <v>0</v>
@@ -6166,7 +6169,7 @@
         <v>136</v>
       </c>
       <c r="C62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D62" t="b">
         <v>0</v>
@@ -6294,7 +6297,7 @@
         <v>168</v>
       </c>
       <c r="C63" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D63" t="b">
         <v>0</v>
@@ -6433,13 +6436,126 @@
       <c r="AR65" s="22"/>
     </row>
     <row r="66" spans="1:44">
-      <c r="AB66" s="3"/>
-      <c r="AC66" s="5"/>
-      <c r="AD66" s="38"/>
-      <c r="AG66" s="23"/>
-      <c r="AH66" s="23"/>
-      <c r="AK66" s="43"/>
-      <c r="AR66" s="22"/>
+      <c r="A66" t="s">
+        <v>301</v>
+      </c>
+      <c r="B66" t="s">
+        <v>234</v>
+      </c>
+      <c r="C66" t="b">
+        <v>1</v>
+      </c>
+      <c r="D66" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" t="s">
+        <v>298</v>
+      </c>
+      <c r="F66" t="b">
+        <v>0</v>
+      </c>
+      <c r="G66" t="s">
+        <v>301</v>
+      </c>
+      <c r="H66" t="b">
+        <v>0</v>
+      </c>
+      <c r="I66" t="b">
+        <v>0</v>
+      </c>
+      <c r="J66" t="b">
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <v>0.02</v>
+      </c>
+      <c r="L66">
+        <v>0</v>
+      </c>
+      <c r="O66" t="s">
+        <v>36</v>
+      </c>
+      <c r="P66" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q66">
+        <v>20</v>
+      </c>
+      <c r="R66">
+        <v>2.75E-2</v>
+      </c>
+      <c r="S66">
+        <v>5</v>
+      </c>
+      <c r="T66">
+        <v>999</v>
+      </c>
+      <c r="U66">
+        <v>0</v>
+      </c>
+      <c r="V66" t="s">
+        <v>55</v>
+      </c>
+      <c r="W66" t="b">
+        <v>0</v>
+      </c>
+      <c r="X66" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y66" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z66">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA66">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="AB66" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="AC66" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AD66" s="38">
+        <v>123</v>
+      </c>
+      <c r="AE66" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF66" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG66" s="23">
+        <v>0.6976</v>
+      </c>
+      <c r="AH66" s="23">
+        <v>0.6976</v>
+      </c>
+      <c r="AK66" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="AL66" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM66" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN66" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO66">
+        <v>0</v>
+      </c>
+      <c r="AP66" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ66" t="b">
+        <v>1</v>
+      </c>
+      <c r="AR66" s="22" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="68" spans="1:44">
       <c r="B68" s="56" t="s">
@@ -6692,7 +6808,7 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM5:AN8 C5:C8 AM10:AN14 AM51:AN52 AM54:AN56 AM16:AN17 AM44:AN49 AM19:AN21 AM69:AN70 C69:C70 AM23:AN24 AM26:AN27 AM41:AN42 AM29:AN30 C59:C66 AM35:AN39 C10:C30 AM59:AN66 C35:C56" xr:uid="{1240F49A-5091-456D-B77A-0673AD56E758}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM5:AN8 C5:C8 AM10:AN14 AM51:AN52 AM54:AN56 AM16:AN17 AM44:AN49 AM19:AN21 AM69:AN70 C69:C70 AM23:AN24 AM26:AN27 AM41:AN42 AM29:AN30 C35:C56 AM35:AN39 C10:C30 C59:C66 AM59:AN66" xr:uid="{1240F49A-5091-456D-B77A-0673AD56E758}">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X5:X8 X10:X14 X51:X52 X29:X30 X54:X56 X16:X17 X19:X21 X69:X70 X23:X24 X26:X27 X35:X39 X44:X49 X41:X42 X59:X66" xr:uid="{8909875A-86FC-4594-BBAF-A364A5851F3C}">
@@ -6712,11 +6828,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62142380-6405-410A-A4D9-17F48F5CE536}">
   <dimension ref="A3:R39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="J14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Q42" sqref="Q42"/>
+      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8149,7 +8265,7 @@
         <v>0.03</v>
       </c>
       <c r="Q39">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="R39">
         <v>0</v>

</xml_diff>

<commit_message>
valuation with separately modeled classic and pepra members
</commit_message>
<xml_diff>
--- a/model/RunControl.xlsx
+++ b/model/RunControl.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFAF636-7207-4B64-A8BC-C0E3778EC6AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C190728-1051-4881-8420-88F8DB80A5F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1845" windowWidth="29040" windowHeight="15840" tabRatio="524" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params_sim" sheetId="22" r:id="rId1"/>
@@ -216,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="305">
   <si>
     <t>nsim</t>
   </si>
@@ -1185,6 +1185,15 @@
   </si>
   <si>
     <t>mix_baseline</t>
+  </si>
+  <si>
+    <t>misc_bf100_cola2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mix of misc_classic and misc_pepra, current policy, for testing </t>
+  </si>
+  <si>
+    <t>"misc_classic","misc_pepra"</t>
   </si>
 </sst>
 </file>
@@ -1873,11 +1882,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D014B46A-D012-4D18-AEAB-1D829080B2CE}">
   <dimension ref="A2:AR70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D41" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="D50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C74" sqref="C74"/>
+      <selection pane="bottomRight" activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6443,7 +6452,7 @@
         <v>234</v>
       </c>
       <c r="C66" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D66" t="b">
         <v>0</v>
@@ -6554,6 +6563,128 @@
         <v>1</v>
       </c>
       <c r="AR66" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:44">
+      <c r="A67" t="s">
+        <v>302</v>
+      </c>
+      <c r="B67" t="s">
+        <v>234</v>
+      </c>
+      <c r="C67" t="b">
+        <v>1</v>
+      </c>
+      <c r="D67" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" t="s">
+        <v>302</v>
+      </c>
+      <c r="F67" t="b">
+        <v>0</v>
+      </c>
+      <c r="G67" t="s">
+        <v>301</v>
+      </c>
+      <c r="H67" t="b">
+        <v>0</v>
+      </c>
+      <c r="I67" t="b">
+        <v>0</v>
+      </c>
+      <c r="J67" t="b">
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <v>0.02</v>
+      </c>
+      <c r="L67">
+        <v>0</v>
+      </c>
+      <c r="O67" t="s">
+        <v>36</v>
+      </c>
+      <c r="P67" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q67">
+        <v>20</v>
+      </c>
+      <c r="R67">
+        <v>2.75E-2</v>
+      </c>
+      <c r="S67">
+        <v>5</v>
+      </c>
+      <c r="T67">
+        <v>999</v>
+      </c>
+      <c r="U67">
+        <v>0</v>
+      </c>
+      <c r="V67" t="s">
+        <v>55</v>
+      </c>
+      <c r="W67" t="b">
+        <v>0</v>
+      </c>
+      <c r="X67" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y67" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z67">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA67">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="AB67" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="AC67" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AD67" s="38">
+        <v>123</v>
+      </c>
+      <c r="AE67" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF67" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG67" s="23">
+        <v>0.6976</v>
+      </c>
+      <c r="AH67" s="23">
+        <v>0.6976</v>
+      </c>
+      <c r="AK67" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="AL67" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM67" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN67" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO67">
+        <v>0</v>
+      </c>
+      <c r="AP67" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ67" t="b">
+        <v>1</v>
+      </c>
+      <c r="AR67" s="22" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6808,13 +6939,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM5:AN8 C5:C8 AM10:AN14 AM51:AN52 AM54:AN56 AM16:AN17 AM44:AN49 AM19:AN21 AM69:AN70 C69:C70 AM23:AN24 AM26:AN27 AM41:AN42 AM29:AN30 C35:C56 AM35:AN39 C10:C30 C59:C66 AM59:AN66" xr:uid="{1240F49A-5091-456D-B77A-0673AD56E758}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM5:AN8 C5:C8 AM10:AN14 AM51:AN52 AM54:AN56 AM16:AN17 AM44:AN49 AM19:AN21 AM69:AN70 C69:C70 AM23:AN24 AM26:AN27 AM41:AN42 AM29:AN30 C35:C56 AM35:AN39 C10:C30 C59:C67 AM59:AN67" xr:uid="{1240F49A-5091-456D-B77A-0673AD56E758}">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X5:X8 X10:X14 X51:X52 X29:X30 X54:X56 X16:X17 X19:X21 X69:X70 X23:X24 X26:X27 X35:X39 X44:X49 X41:X42 X59:X66" xr:uid="{8909875A-86FC-4594-BBAF-A364A5851F3C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X5:X8 X10:X14 X51:X52 X29:X30 X54:X56 X16:X17 X19:X21 X69:X70 X23:X24 X26:X27 X35:X39 X44:X49 X41:X42 X59:X67" xr:uid="{8909875A-86FC-4594-BBAF-A364A5851F3C}">
       <formula1>"simple, internal"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D8 D10:D14 D51:D52 D29:D30 D54:D56 D16:D17 D19:D21 D69:D70 D23:D24 D26:D27 D35:D39 D44:D49 D41:D42 D59:D66" xr:uid="{EC327A6A-3FD9-4228-86E6-BF4DFCBDFAEB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D8 D10:D14 D51:D52 D29:D30 D54:D56 D16:D17 D19:D21 D69:D70 D23:D24 D26:D27 D35:D39 D44:D49 D41:D42 D59:D67" xr:uid="{EC327A6A-3FD9-4228-86E6-BF4DFCBDFAEB}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6826,13 +6957,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62142380-6405-410A-A4D9-17F48F5CE536}">
-  <dimension ref="A3:R39"/>
+  <dimension ref="A3:R41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="J14" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="J20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
+      <selection pane="bottomRight" activeCell="P42" sqref="P42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6841,7 +6972,7 @@
     <col min="2" max="2" width="56.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" customWidth="1"/>
     <col min="6" max="6" width="17.140625" customWidth="1"/>
     <col min="7" max="7" width="21.7109375" customWidth="1"/>
     <col min="8" max="9" width="17.42578125" customWidth="1"/>
@@ -8226,7 +8357,7 @@
         <v>299</v>
       </c>
       <c r="C39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D39" t="s">
         <v>70</v>
@@ -8271,12 +8402,65 @@
         <v>0</v>
       </c>
     </row>
+    <row r="41" spans="1:18">
+      <c r="A41" t="s">
+        <v>302</v>
+      </c>
+      <c r="B41" t="s">
+        <v>303</v>
+      </c>
+      <c r="C41" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>70</v>
+      </c>
+      <c r="E41" t="s">
+        <v>304</v>
+      </c>
+      <c r="F41" t="s">
+        <v>68</v>
+      </c>
+      <c r="G41">
+        <v>2.75E-2</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41" t="b">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>2018</v>
+      </c>
+      <c r="N41" t="b">
+        <v>1</v>
+      </c>
+      <c r="O41" s="43">
+        <v>0.11</v>
+      </c>
+      <c r="P41">
+        <v>0.02</v>
+      </c>
+      <c r="Q41">
+        <v>0.05</v>
+      </c>
+      <c r="R41">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D24:D26 D5:D9 D11:D13 D28:D31 D20:D22 D15:D17 D33:D34 D36:D37 D39" xr:uid="{73B0AF26-6A4C-427C-B7EA-75439AFB0B6E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D24:D26 D5:D9 D11:D13 D28:D31 D20:D22 D15:D17 D33:D34 D36:D37 D39 D41" xr:uid="{73B0AF26-6A4C-427C-B7EA-75439AFB0B6E}">
       <formula1>"singleTier,multiTier"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C33:C37 C5:C31 C39" xr:uid="{BD331DEC-2DB8-437E-B2EB-02992BFDA38C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C33:C37 C5:C31 C39 C41" xr:uid="{BD331DEC-2DB8-437E-B2EB-02992BFDA38C}">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8291,7 +8475,7 @@
   <dimension ref="A3:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8688,7 +8872,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C54" sqref="C54"/>
+      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -9538,7 +9722,7 @@
   <dimension ref="A2:R34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
update contingent COLA with mulitple tiers
</commit_message>
<xml_diff>
--- a/model/RunControl.xlsx
+++ b/model/RunControl.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C190728-1051-4881-8420-88F8DB80A5F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5072618-8B2E-4233-9E51-CB41A47FCCC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1845" windowWidth="29040" windowHeight="15840" tabRatio="524" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1845" windowWidth="29040" windowHeight="15840" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params_sim" sheetId="22" r:id="rId1"/>
@@ -216,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="307">
   <si>
     <t>nsim</t>
   </si>
@@ -1019,13 +1019,7 @@
     <t>sftyAll_benCut1_colaCut1_lowERC</t>
   </si>
   <si>
-    <t>sftyAll_benCut1_colsCut1_highERC</t>
-  </si>
-  <si>
     <t>sftyAll_benCut2_colaCut2_lowERC</t>
-  </si>
-  <si>
-    <t>sftyAll_benCut2_colsCut2_highERC</t>
   </si>
   <si>
     <t>twoTiers_bf1_cola_highERC</t>
@@ -1194,6 +1188,18 @@
   </si>
   <si>
     <t>"misc_classic","misc_pepra"</t>
+  </si>
+  <si>
+    <t>test runs</t>
+  </si>
+  <si>
+    <t>sftyAll_benCut2_colaCut2_highERC</t>
+  </si>
+  <si>
+    <t>sftyAll_benCut1_colaCut1_highERC</t>
+  </si>
+  <si>
+    <t>misc_bf100_colaCut</t>
   </si>
 </sst>
 </file>
@@ -1880,13 +1886,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D014B46A-D012-4D18-AEAB-1D829080B2CE}">
-  <dimension ref="A2:AR70"/>
+  <dimension ref="A2:AR74"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D50" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="D44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A67" sqref="A67"/>
+      <selection pane="bottomRight" activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1895,7 +1901,7 @@
     <col min="2" max="2" width="32.85546875" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" customWidth="1"/>
     <col min="8" max="8" width="17.42578125" customWidth="1"/>
@@ -1903,7 +1909,7 @@
     <col min="10" max="11" width="14.5703125" customWidth="1"/>
     <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.85546875" customWidth="1"/>
-    <col min="14" max="14" width="25.85546875" customWidth="1"/>
+    <col min="14" max="14" width="24.42578125" customWidth="1"/>
     <col min="15" max="15" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7.85546875" customWidth="1"/>
@@ -2034,10 +2040,10 @@
         <v>123</v>
       </c>
       <c r="M4" s="40" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="N4" s="40" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="O4" s="10" t="s">
         <v>11</v>
@@ -5010,7 +5016,7 @@
     </row>
     <row r="45" spans="1:44">
       <c r="A45" t="s">
-        <v>267</v>
+        <v>305</v>
       </c>
       <c r="B45" t="s">
         <v>146</v>
@@ -5649,7 +5655,7 @@
     </row>
     <row r="54" spans="1:44">
       <c r="A54" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B54" t="s">
         <v>145</v>
@@ -5771,7 +5777,7 @@
     </row>
     <row r="55" spans="1:44">
       <c r="A55" t="s">
-        <v>269</v>
+        <v>304</v>
       </c>
       <c r="B55" t="s">
         <v>146</v>
@@ -5902,12 +5908,12 @@
     </row>
     <row r="58" spans="1:44">
       <c r="B58" s="56" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="59" spans="1:44">
       <c r="A59" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B59" t="s">
         <v>136</v>
@@ -6035,7 +6041,7 @@
     </row>
     <row r="60" spans="1:44">
       <c r="A60" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B60" t="s">
         <v>168</v>
@@ -6172,7 +6178,7 @@
     </row>
     <row r="62" spans="1:44">
       <c r="A62" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B62" t="s">
         <v>136</v>
@@ -6300,7 +6306,7 @@
     </row>
     <row r="63" spans="1:44">
       <c r="A63" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B63" t="s">
         <v>168</v>
@@ -6436,6 +6442,9 @@
       <c r="AR64" s="22"/>
     </row>
     <row r="65" spans="1:44">
+      <c r="B65" s="56" t="s">
+        <v>303</v>
+      </c>
       <c r="AB65" s="3"/>
       <c r="AC65" s="5"/>
       <c r="AD65" s="38"/>
@@ -6446,7 +6455,7 @@
     </row>
     <row r="66" spans="1:44">
       <c r="A66" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B66" t="s">
         <v>234</v>
@@ -6458,13 +6467,13 @@
         <v>0</v>
       </c>
       <c r="E66" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F66" t="b">
         <v>0</v>
       </c>
       <c r="G66" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H66" t="b">
         <v>0</v>
@@ -6568,7 +6577,7 @@
     </row>
     <row r="67" spans="1:44">
       <c r="A67" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B67" t="s">
         <v>234</v>
@@ -6580,13 +6589,13 @@
         <v>0</v>
       </c>
       <c r="E67" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F67" t="b">
         <v>0</v>
       </c>
       <c r="G67" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H67" t="b">
         <v>0</v>
@@ -6689,263 +6698,412 @@
       </c>
     </row>
     <row r="68" spans="1:44">
-      <c r="B68" s="56" t="s">
+      <c r="A68" t="s">
+        <v>306</v>
+      </c>
+      <c r="B68" t="s">
+        <v>234</v>
+      </c>
+      <c r="C68" t="b">
+        <v>0</v>
+      </c>
+      <c r="D68" t="b">
+        <v>0</v>
+      </c>
+      <c r="E68" t="s">
+        <v>300</v>
+      </c>
+      <c r="F68" t="b">
+        <v>0</v>
+      </c>
+      <c r="G68" t="s">
+        <v>299</v>
+      </c>
+      <c r="H68" t="b">
+        <v>0</v>
+      </c>
+      <c r="I68" t="b">
+        <v>0</v>
+      </c>
+      <c r="J68" t="b">
+        <v>1</v>
+      </c>
+      <c r="K68">
+        <v>0.02</v>
+      </c>
+      <c r="L68">
+        <v>0.01</v>
+      </c>
+      <c r="O68" t="s">
+        <v>36</v>
+      </c>
+      <c r="P68" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q68">
+        <v>20</v>
+      </c>
+      <c r="R68">
+        <v>2.75E-2</v>
+      </c>
+      <c r="S68">
+        <v>5</v>
+      </c>
+      <c r="T68">
+        <v>999</v>
+      </c>
+      <c r="U68">
+        <v>0</v>
+      </c>
+      <c r="V68" t="s">
+        <v>55</v>
+      </c>
+      <c r="W68" t="b">
+        <v>0</v>
+      </c>
+      <c r="X68" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y68" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z68">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA68">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="AB68" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="AC68" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AD68" s="38">
+        <v>123</v>
+      </c>
+      <c r="AE68" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF68" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG68" s="23">
+        <v>0.6976</v>
+      </c>
+      <c r="AH68" s="23">
+        <v>0.6976</v>
+      </c>
+      <c r="AK68" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="AL68" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM68" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN68" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO68">
+        <v>0</v>
+      </c>
+      <c r="AP68" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ68" t="b">
+        <v>1</v>
+      </c>
+      <c r="AR68" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:44">
+      <c r="AB69" s="3"/>
+      <c r="AC69" s="5"/>
+      <c r="AD69" s="38"/>
+      <c r="AG69" s="23"/>
+      <c r="AH69" s="23"/>
+      <c r="AK69" s="43"/>
+      <c r="AR69" s="22"/>
+    </row>
+    <row r="70" spans="1:44">
+      <c r="AB70" s="3"/>
+      <c r="AC70" s="5"/>
+      <c r="AD70" s="38"/>
+      <c r="AG70" s="23"/>
+      <c r="AH70" s="23"/>
+      <c r="AK70" s="43"/>
+      <c r="AR70" s="22"/>
+    </row>
+    <row r="71" spans="1:44">
+      <c r="AB71" s="3"/>
+      <c r="AC71" s="5"/>
+      <c r="AD71" s="38"/>
+      <c r="AG71" s="23"/>
+      <c r="AH71" s="23"/>
+      <c r="AK71" s="43"/>
+      <c r="AR71" s="22"/>
+    </row>
+    <row r="72" spans="1:44">
+      <c r="B72" s="56" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="69" spans="1:44">
-      <c r="A69" t="s">
+    <row r="73" spans="1:44">
+      <c r="A73" t="s">
         <v>144</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B73" t="s">
         <v>137</v>
       </c>
-      <c r="C69" t="b">
-        <v>0</v>
-      </c>
-      <c r="D69" t="b">
-        <v>0</v>
-      </c>
-      <c r="E69" t="s">
+      <c r="C73" t="b">
+        <v>0</v>
+      </c>
+      <c r="D73" t="b">
+        <v>0</v>
+      </c>
+      <c r="E73" t="s">
         <v>142</v>
       </c>
-      <c r="F69" t="b">
-        <v>0</v>
-      </c>
-      <c r="G69" t="s">
+      <c r="F73" t="b">
+        <v>0</v>
+      </c>
+      <c r="G73" t="s">
         <v>139</v>
       </c>
-      <c r="H69" t="b">
-        <v>0</v>
-      </c>
-      <c r="I69" t="b">
-        <v>1</v>
-      </c>
-      <c r="J69" t="b">
-        <v>1</v>
-      </c>
-      <c r="K69">
+      <c r="H73" t="b">
+        <v>0</v>
+      </c>
+      <c r="I73" t="b">
+        <v>1</v>
+      </c>
+      <c r="J73" t="b">
+        <v>1</v>
+      </c>
+      <c r="K73">
         <v>0.02</v>
       </c>
-      <c r="L69">
-        <v>0</v>
-      </c>
-      <c r="O69" t="s">
+      <c r="L73">
+        <v>0</v>
+      </c>
+      <c r="O73" t="s">
         <v>36</v>
       </c>
-      <c r="P69" t="s">
+      <c r="P73" t="s">
         <v>35</v>
       </c>
-      <c r="Q69">
+      <c r="Q73">
         <v>20</v>
       </c>
-      <c r="R69">
+      <c r="R73">
         <v>2.75E-2</v>
       </c>
-      <c r="S69">
+      <c r="S73">
         <v>5</v>
       </c>
-      <c r="T69">
+      <c r="T73">
         <v>999</v>
       </c>
-      <c r="U69">
-        <v>0</v>
-      </c>
-      <c r="V69" t="s">
+      <c r="U73">
+        <v>0</v>
+      </c>
+      <c r="V73" t="s">
         <v>55</v>
       </c>
-      <c r="W69" t="b">
-        <v>0</v>
-      </c>
-      <c r="X69" t="s">
+      <c r="W73" t="b">
+        <v>0</v>
+      </c>
+      <c r="X73" t="s">
         <v>119</v>
       </c>
-      <c r="Y69" t="s">
+      <c r="Y73" t="s">
         <v>20</v>
       </c>
-      <c r="Z69">
+      <c r="Z73">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AA69">
+      <c r="AA73">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AB69" s="3">
+      <c r="AB73" s="3">
         <v>0.12</v>
       </c>
-      <c r="AC69" s="5">
+      <c r="AC73" s="5">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AD69" s="38">
+      <c r="AD73" s="38">
         <v>123</v>
       </c>
-      <c r="AE69" t="s">
+      <c r="AE73" t="s">
         <v>31</v>
       </c>
-      <c r="AF69" t="s">
+      <c r="AF73" t="s">
         <v>31</v>
       </c>
-      <c r="AG69" s="23">
+      <c r="AG73" s="23">
         <v>0.6976</v>
       </c>
-      <c r="AH69" s="23">
+      <c r="AH73" s="23">
         <v>0.6976</v>
       </c>
-      <c r="AK69" s="43">
+      <c r="AK73" s="43">
         <v>0.1</v>
       </c>
-      <c r="AL69" t="b">
-        <v>1</v>
-      </c>
-      <c r="AM69" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN69" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO69">
-        <v>0</v>
-      </c>
-      <c r="AP69" t="s">
+      <c r="AL73" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM73" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN73" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO73">
+        <v>0</v>
+      </c>
+      <c r="AP73" t="s">
         <v>3</v>
       </c>
-      <c r="AQ69" t="b">
-        <v>1</v>
-      </c>
-      <c r="AR69" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:44">
-      <c r="A70" t="s">
-        <v>270</v>
-      </c>
-      <c r="B70" t="s">
+      <c r="AQ73" t="b">
+        <v>1</v>
+      </c>
+      <c r="AR73" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:44">
+      <c r="A74" t="s">
+        <v>268</v>
+      </c>
+      <c r="B74" t="s">
         <v>146</v>
       </c>
-      <c r="C70" t="b">
-        <v>0</v>
-      </c>
-      <c r="D70" t="b">
-        <v>0</v>
-      </c>
-      <c r="E70" t="s">
+      <c r="C74" t="b">
+        <v>0</v>
+      </c>
+      <c r="D74" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" t="s">
         <v>143</v>
       </c>
-      <c r="F70" t="b">
-        <v>0</v>
-      </c>
-      <c r="G70" t="s">
+      <c r="F74" t="b">
+        <v>0</v>
+      </c>
+      <c r="G74" t="s">
         <v>139</v>
       </c>
-      <c r="H70" t="b">
-        <v>1</v>
-      </c>
-      <c r="I70" t="b">
-        <v>1</v>
-      </c>
-      <c r="J70" t="b">
-        <v>1</v>
-      </c>
-      <c r="K70">
+      <c r="H74" t="b">
+        <v>1</v>
+      </c>
+      <c r="I74" t="b">
+        <v>1</v>
+      </c>
+      <c r="J74" t="b">
+        <v>1</v>
+      </c>
+      <c r="K74">
         <v>0.02</v>
       </c>
-      <c r="L70">
-        <v>0</v>
-      </c>
-      <c r="O70" t="s">
+      <c r="L74">
+        <v>0</v>
+      </c>
+      <c r="O74" t="s">
         <v>36</v>
       </c>
-      <c r="P70" t="s">
+      <c r="P74" t="s">
         <v>35</v>
       </c>
-      <c r="Q70">
+      <c r="Q74">
         <v>20</v>
       </c>
-      <c r="R70">
+      <c r="R74">
         <v>2.75E-2</v>
       </c>
-      <c r="S70">
+      <c r="S74">
         <v>5</v>
       </c>
-      <c r="T70">
+      <c r="T74">
         <v>999</v>
       </c>
-      <c r="U70">
-        <v>0</v>
-      </c>
-      <c r="V70" t="s">
+      <c r="U74">
+        <v>0</v>
+      </c>
+      <c r="V74" t="s">
         <v>55</v>
       </c>
-      <c r="W70" t="b">
-        <v>0</v>
-      </c>
-      <c r="X70" t="s">
+      <c r="W74" t="b">
+        <v>0</v>
+      </c>
+      <c r="X74" t="s">
         <v>119</v>
       </c>
-      <c r="Y70" t="s">
+      <c r="Y74" t="s">
         <v>20</v>
       </c>
-      <c r="Z70">
+      <c r="Z74">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AA70">
+      <c r="AA74">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AB70" s="3">
+      <c r="AB74" s="3">
         <v>0.12</v>
       </c>
-      <c r="AC70" s="5">
+      <c r="AC74" s="5">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AD70" s="38">
+      <c r="AD74" s="38">
         <v>123</v>
       </c>
-      <c r="AE70" t="s">
+      <c r="AE74" t="s">
         <v>31</v>
       </c>
-      <c r="AF70" t="s">
+      <c r="AF74" t="s">
         <v>31</v>
       </c>
-      <c r="AG70" s="23">
+      <c r="AG74" s="23">
         <v>0.6976</v>
       </c>
-      <c r="AH70" s="23">
+      <c r="AH74" s="23">
         <v>0.6976</v>
       </c>
-      <c r="AK70" s="43">
+      <c r="AK74" s="43">
         <v>0.1</v>
       </c>
-      <c r="AL70" t="b">
-        <v>1</v>
-      </c>
-      <c r="AM70" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN70" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO70">
-        <v>0</v>
-      </c>
-      <c r="AP70" t="s">
+      <c r="AL74" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM74" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN74" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO74">
+        <v>0</v>
+      </c>
+      <c r="AP74" t="s">
         <v>3</v>
       </c>
-      <c r="AQ70" t="b">
-        <v>1</v>
-      </c>
-      <c r="AR70" s="22" t="b">
+      <c r="AQ74" t="b">
+        <v>1</v>
+      </c>
+      <c r="AR74" s="22" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM5:AN8 C5:C8 AM10:AN14 AM51:AN52 AM54:AN56 AM16:AN17 AM44:AN49 AM19:AN21 AM69:AN70 C69:C70 AM23:AN24 AM26:AN27 AM41:AN42 AM29:AN30 C35:C56 AM35:AN39 C10:C30 C59:C67 AM59:AN67" xr:uid="{1240F49A-5091-456D-B77A-0673AD56E758}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM5:AN8 C5:C8 AM10:AN14 AM51:AN52 AM54:AN56 AM16:AN17 AM44:AN49 AM19:AN21 AM73:AN74 C73:C74 AM23:AN24 AM26:AN27 AM41:AN42 AM29:AN30 C35:C56 AM35:AN39 C10:C30 AM59:AN71 C59:C71" xr:uid="{1240F49A-5091-456D-B77A-0673AD56E758}">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X5:X8 X10:X14 X51:X52 X29:X30 X54:X56 X16:X17 X19:X21 X69:X70 X23:X24 X26:X27 X35:X39 X44:X49 X41:X42 X59:X67" xr:uid="{8909875A-86FC-4594-BBAF-A364A5851F3C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X5:X8 X10:X14 X51:X52 X29:X30 X54:X56 X16:X17 X19:X21 X73:X74 X23:X24 X26:X27 X35:X39 X44:X49 X41:X42 X59:X71" xr:uid="{8909875A-86FC-4594-BBAF-A364A5851F3C}">
       <formula1>"simple, internal"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D8 D10:D14 D51:D52 D29:D30 D54:D56 D16:D17 D19:D21 D69:D70 D23:D24 D26:D27 D35:D39 D44:D49 D41:D42 D59:D67" xr:uid="{EC327A6A-3FD9-4228-86E6-BF4DFCBDFAEB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D8 D10:D14 D51:D52 D29:D30 D54:D56 D16:D17 D19:D21 D73:D74 D23:D24 D26:D27 D35:D39 D44:D49 D41:D42 D59:D71" xr:uid="{EC327A6A-3FD9-4228-86E6-BF4DFCBDFAEB}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6959,11 +7117,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62142380-6405-410A-A4D9-17F48F5CE536}">
   <dimension ref="A3:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="J20" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="J14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="P42" sqref="P42"/>
+      <selection pane="bottomRight" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8133,10 +8291,10 @@
     </row>
     <row r="33" spans="1:18">
       <c r="A33" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B33" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C33" t="b">
         <v>0</v>
@@ -8186,10 +8344,10 @@
     </row>
     <row r="34" spans="1:18">
       <c r="A34" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B34" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C34" t="b">
         <v>0</v>
@@ -8239,10 +8397,10 @@
     </row>
     <row r="36" spans="1:18">
       <c r="A36" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B36" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C36" t="b">
         <v>0</v>
@@ -8295,10 +8453,10 @@
     </row>
     <row r="37" spans="1:18">
       <c r="A37" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B37" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C37" t="b">
         <v>0</v>
@@ -8351,10 +8509,10 @@
     </row>
     <row r="39" spans="1:18">
       <c r="A39" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B39" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C39" t="b">
         <v>0</v>
@@ -8363,7 +8521,7 @@
         <v>70</v>
       </c>
       <c r="E39" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F39" t="s">
         <v>68</v>
@@ -8404,10 +8562,10 @@
     </row>
     <row r="41" spans="1:18">
       <c r="A41" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B41" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C41" t="b">
         <v>1</v>
@@ -8416,7 +8574,7 @@
         <v>70</v>
       </c>
       <c r="E41" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F41" t="s">
         <v>68</v>
@@ -9742,22 +9900,22 @@
   <sheetData>
     <row r="2" spans="1:18">
       <c r="B2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="B3" s="57" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C3" s="57"/>
       <c r="D3" s="57" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E3" s="57"/>
       <c r="F3" s="57"/>
@@ -9798,10 +9956,10 @@
         <v>178</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -9878,7 +10036,7 @@
         <v>534</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="Q6">
         <f>148525+24916</f>
@@ -9905,7 +10063,7 @@
         <v>96</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="Q7">
         <f>10827+2402</f>
@@ -9918,7 +10076,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="49" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B8" s="24"/>
       <c r="C8" s="24"/>
@@ -9956,7 +10114,7 @@
         <v>189</v>
       </c>
       <c r="P9" s="49" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -10032,7 +10190,7 @@
         <v>8.9594759881010102E-4</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="Q11" s="6">
         <f t="shared" ref="Q11:R11" si="1">Q6/SUM($Q6:$R6)</f>
@@ -10056,7 +10214,7 @@
         <v>9.7409515692064165E-4</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="Q12" s="6">
         <f t="shared" ref="Q12:R12" si="2">Q7/SUM($Q7:$R7)</f>
@@ -10106,7 +10264,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="55" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B19" s="50">
         <f>B16*Q10</f>
@@ -10115,7 +10273,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="55" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B20" s="50">
         <f>B16*R10</f>
@@ -10127,7 +10285,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B22" s="50">
         <f>1-B16</f>

</xml_diff>

<commit_message>
update for draft report
</commit_message>
<xml_diff>
--- a/model/RunControl.xlsx
+++ b/model/RunControl.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EEA27E5-39C8-42D5-91E7-A75702AB4DE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E09E99-5654-4D20-8729-833A70291F32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1845" windowWidth="29040" windowHeight="15840" tabRatio="524" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params_sim" sheetId="22" r:id="rId1"/>
@@ -362,7 +362,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1589" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1618" uniqueCount="392">
   <si>
     <t>nsim</t>
   </si>
@@ -1553,6 +1553,54 @@
   </si>
   <si>
     <t>"sfty_classic","sfty_pepra"</t>
+  </si>
+  <si>
+    <t>All members</t>
+  </si>
+  <si>
+    <t>state members</t>
+  </si>
+  <si>
+    <t>of CalPERS</t>
+  </si>
+  <si>
+    <t>of PERF A</t>
+  </si>
+  <si>
+    <t>misc2t_bf100_cola2_DR5</t>
+  </si>
+  <si>
+    <t>misc2t, 2%bfactor, 2%cola, current policy, 5% discount</t>
+  </si>
+  <si>
+    <t>sfty2t_bf100_cola2_DR5</t>
+  </si>
+  <si>
+    <t>sfty2t, 3%bfactor, 2%cola, current policy, 5% discount</t>
+  </si>
+  <si>
+    <t>misc2t_bf50_cola1_DR5</t>
+  </si>
+  <si>
+    <t>misc2t, 1%bfactor(new), 1%cola, 5% discount</t>
+  </si>
+  <si>
+    <t>sfty2t_bf50_cola1_DR5</t>
+  </si>
+  <si>
+    <t>sfty2t, 1.5%bfactor(new), 1%cola(cola suspension), 5% discount</t>
+  </si>
+  <si>
+    <t>misc2t_bf100_colap5</t>
+  </si>
+  <si>
+    <t>sfty2t_bf100_colap5</t>
+  </si>
+  <si>
+    <t>Misc 2 tiers, 2%bfactor, 0.5%cola</t>
+  </si>
+  <si>
+    <t>sfty2t, 3%bfactor, 0.5%cola(cola suspension)</t>
   </si>
 </sst>
 </file>
@@ -1806,7 +1854,7 @@
     </xf>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1888,9 +1936,14 @@
     <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -2266,11 +2319,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D014B46A-D012-4D18-AEAB-1D829080B2CE}">
   <dimension ref="A2:AR73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D32" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="K23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E63" sqref="E63"/>
+      <selection pane="bottomRight" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3877,9 +3930,6 @@
       <c r="B21" s="56" t="s">
         <v>233</v>
       </c>
-      <c r="C21" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="22" spans="1:44">
       <c r="A22" t="s">
@@ -4630,7 +4680,7 @@
         <v>235</v>
       </c>
       <c r="C34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" t="b">
         <v>0</v>
@@ -4757,9 +4807,6 @@
       <c r="B36" s="56" t="s">
         <v>238</v>
       </c>
-      <c r="C36" t="b">
-        <v>0</v>
-      </c>
       <c r="AB36" s="3"/>
       <c r="AC36" s="5"/>
       <c r="AD36" s="38"/>
@@ -5521,9 +5568,6 @@
       <c r="B46" s="56" t="s">
         <v>237</v>
       </c>
-      <c r="C46" t="b">
-        <v>0</v>
-      </c>
       <c r="AB46" s="3"/>
       <c r="AC46" s="5"/>
       <c r="AD46" s="38"/>
@@ -6559,7 +6603,7 @@
         <v>136</v>
       </c>
       <c r="C61" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D61" t="b">
         <v>0</v>
@@ -6687,7 +6731,7 @@
         <v>168</v>
       </c>
       <c r="C62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D62" t="b">
         <v>0</v>
@@ -7473,7 +7517,7 @@
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM5:AN8 C5:C8 AM50:AN51 AM53:AN55 AM15:AN16 AM43:AN48 AM18:AN20 AM72:AN73 C72:C73 AM22:AN23 AM25:AN26 AM40:AN41 AM28:AN29 C10:C29 AM34:AN38 AM58:AN70 C58:C70 AM10:AN13 C34:C55" xr:uid="{1240F49A-5091-456D-B77A-0673AD56E758}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM5:AN8 C5:C8 AM50:AN51 AM53:AN55 AM15:AN16 AM43:AN48 AM18:AN20 AM72:AN73 C72:C73 AM22:AN23 AM25:AN26 AM40:AN41 AM28:AN29 C34:C35 AM34:AN38 AM58:AN70 C37:C55 AM10:AN13 C10:C29 C58:C70" xr:uid="{1240F49A-5091-456D-B77A-0673AD56E758}">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X5:X8 X50:X51 X28:X29 X53:X55 X15:X16 X18:X20 X72:X73 X22:X23 X25:X26 X34:X38 X43:X48 X40:X41 X58:X70 X10:X13" xr:uid="{8909875A-86FC-4594-BBAF-A364A5851F3C}">
@@ -7491,20 +7535,22 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C9FDD0-43C0-4547-B8AB-B7BD31607ED6}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="B1" t="s">
         <v>158</v>
       </c>
@@ -7512,12 +7558,12 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:5">
       <c r="C2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>156</v>
       </c>
@@ -7527,8 +7573,13 @@
       <c r="C3" s="24">
         <v>273275278</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="24"/>
+      <c r="E3" s="25">
+        <f t="shared" ref="E3:E10" si="0">B3/$B$11</f>
+        <v>0.71089812405407393</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>148</v>
       </c>
@@ -7538,8 +7589,13 @@
       <c r="C4" s="24">
         <v>68156741</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="24"/>
+      <c r="E4" s="25">
+        <f t="shared" si="0"/>
+        <v>0.17724157908687244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>149</v>
       </c>
@@ -7549,8 +7605,13 @@
       <c r="C5" s="24">
         <v>31179414</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" s="24"/>
+      <c r="E5" s="25">
+        <f t="shared" si="0"/>
+        <v>8.016991314371183E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>150</v>
       </c>
@@ -7560,8 +7621,13 @@
       <c r="C6" s="24">
         <v>114404</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" s="24"/>
+      <c r="E6" s="25">
+        <f t="shared" si="0"/>
+        <v>3.1149329737959505E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>151</v>
       </c>
@@ -7571,8 +7637,13 @@
       <c r="C7" s="24">
         <v>10169</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="24"/>
+      <c r="E7" s="25">
+        <f t="shared" si="0"/>
+        <v>1.0840555401007E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>152</v>
       </c>
@@ -7582,8 +7653,13 @@
       <c r="C8" s="24">
         <v>1710089</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" s="24"/>
+      <c r="E8" s="25">
+        <f t="shared" si="0"/>
+        <v>4.1728492927283678E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>153</v>
       </c>
@@ -7593,8 +7669,13 @@
       <c r="C9" s="24">
         <v>1684986</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" s="24"/>
+      <c r="E9" s="25">
+        <f t="shared" si="0"/>
+        <v>4.0914227192941424E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>154</v>
       </c>
@@ -7604,8 +7685,13 @@
       <c r="C10" s="24">
         <v>114051</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" s="24"/>
+      <c r="E10" s="25">
+        <f t="shared" si="0"/>
+        <v>3.176725042254669E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>155</v>
       </c>
@@ -7615,17 +7701,51 @@
       <c r="C11" s="24">
         <v>386062132</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D11" s="24"/>
+      <c r="E11" s="25">
+        <f>B11/$B$11</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="B13">
         <f>SUM(B3:B5)/B11</f>
         <v>0.96830961628465817</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:5">
       <c r="B16">
         <f>B3/SUM(B3:B5)</f>
         <v>0.73416406498341347</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="F17">
+        <v>136231421</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>377</v>
+      </c>
+      <c r="B18">
+        <v>136231421</v>
+      </c>
+      <c r="E18" s="25">
+        <f>B18/$B$11</f>
+        <v>0.37264370485438381</v>
+      </c>
+      <c r="F18" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="E19" s="25">
+        <f>B18/B3</f>
+        <v>0.52418721086122733</v>
+      </c>
+      <c r="F19" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -7796,13 +7916,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19F07677-8B44-417E-B263-203C3A91094A}">
-  <dimension ref="A3:R66"/>
+  <dimension ref="A3:R76"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D29" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="D49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A69" sqref="A69"/>
+      <selection pane="bottomRight" activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9188,65 +9308,65 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:18">
-      <c r="A40" t="s">
-        <v>300</v>
-      </c>
-      <c r="B40" t="s">
-        <v>301</v>
-      </c>
-      <c r="C40" t="b">
-        <v>0</v>
-      </c>
-      <c r="D40" t="s">
+    <row r="42" spans="1:18">
+      <c r="A42" s="60" t="s">
+        <v>307</v>
+      </c>
+      <c r="B42" t="s">
+        <v>316</v>
+      </c>
+      <c r="C42" t="b">
+        <v>0</v>
+      </c>
+      <c r="D42" t="s">
         <v>70</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E42" t="s">
         <v>302</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F42" t="s">
         <v>68</v>
       </c>
-      <c r="G40">
+      <c r="G42">
         <v>2.75E-2</v>
       </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40" t="b">
-        <v>1</v>
-      </c>
-      <c r="J40">
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42" t="b">
+        <v>1</v>
+      </c>
+      <c r="J42">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="K40">
-        <v>0</v>
-      </c>
-      <c r="L40">
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42">
         <v>2018</v>
       </c>
-      <c r="N40" t="b">
-        <v>1</v>
-      </c>
-      <c r="O40" s="43">
+      <c r="N42" t="b">
+        <v>1</v>
+      </c>
+      <c r="O42" s="43">
         <v>0.11</v>
       </c>
-      <c r="P40">
+      <c r="P42">
         <v>0.02</v>
       </c>
-      <c r="Q40">
+      <c r="Q42">
         <v>0.05</v>
       </c>
-      <c r="R40">
+      <c r="R42">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:18">
-      <c r="A43" t="s">
-        <v>307</v>
+      <c r="A43" s="60" t="s">
+        <v>308</v>
       </c>
       <c r="B43" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C43" t="b">
         <v>0</v>
@@ -9273,7 +9393,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K43">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="L43">
         <v>2018</v>
@@ -9295,11 +9415,11 @@
       </c>
     </row>
     <row r="44" spans="1:18">
-      <c r="A44" t="s">
-        <v>308</v>
+      <c r="A44" s="60" t="s">
+        <v>309</v>
       </c>
       <c r="B44" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C44" t="b">
         <v>0</v>
@@ -9326,7 +9446,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K44">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="L44">
         <v>2018</v>
@@ -9348,67 +9468,71 @@
       </c>
     </row>
     <row r="45" spans="1:18">
-      <c r="A45" t="s">
-        <v>309</v>
-      </c>
-      <c r="B45" t="s">
-        <v>318</v>
-      </c>
-      <c r="C45" t="b">
-        <v>0</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="A45" s="60"/>
+      <c r="O45" s="43"/>
+    </row>
+    <row r="46" spans="1:18">
+      <c r="A46" s="60" t="s">
+        <v>310</v>
+      </c>
+      <c r="B46" t="s">
+        <v>319</v>
+      </c>
+      <c r="C46" t="b">
+        <v>0</v>
+      </c>
+      <c r="D46" t="s">
         <v>70</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E46" t="s">
         <v>302</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F46" t="s">
         <v>68</v>
       </c>
-      <c r="G45">
+      <c r="G46">
         <v>2.75E-2</v>
       </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
-      <c r="I45" t="b">
-        <v>1</v>
-      </c>
-      <c r="J45">
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46" t="b">
+        <v>1</v>
+      </c>
+      <c r="J46">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="K45">
-        <v>0.5</v>
-      </c>
-      <c r="L45">
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
         <v>2018</v>
       </c>
-      <c r="N45" t="b">
-        <v>1</v>
-      </c>
-      <c r="O45" s="43">
+      <c r="M46">
+        <v>0.01</v>
+      </c>
+      <c r="N46" t="b">
+        <v>1</v>
+      </c>
+      <c r="O46" s="43">
         <v>0.11</v>
       </c>
-      <c r="P45">
+      <c r="P46">
         <v>0.02</v>
       </c>
-      <c r="Q45">
+      <c r="Q46">
         <v>0.05</v>
       </c>
-      <c r="R45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18">
-      <c r="O46" s="43"/>
+      <c r="R46">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:18">
-      <c r="A47" t="s">
-        <v>310</v>
+      <c r="A47" s="60" t="s">
+        <v>311</v>
       </c>
       <c r="B47" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C47" t="b">
         <v>0</v>
@@ -9435,7 +9559,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K47">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="L47">
         <v>2018</v>
@@ -9460,11 +9584,11 @@
       </c>
     </row>
     <row r="48" spans="1:18">
-      <c r="A48" t="s">
-        <v>311</v>
+      <c r="A48" s="60" t="s">
+        <v>312</v>
       </c>
       <c r="B48" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C48" t="b">
         <v>0</v>
@@ -9491,7 +9615,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K48">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="L48">
         <v>2018</v>
@@ -9516,67 +9640,70 @@
       </c>
     </row>
     <row r="49" spans="1:18">
-      <c r="A49" t="s">
-        <v>312</v>
-      </c>
-      <c r="B49" t="s">
-        <v>321</v>
-      </c>
-      <c r="C49" t="b">
-        <v>0</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="A49" s="60"/>
+    </row>
+    <row r="50" spans="1:18">
+      <c r="A50" s="60" t="s">
+        <v>313</v>
+      </c>
+      <c r="B50" t="s">
+        <v>322</v>
+      </c>
+      <c r="C50" t="b">
+        <v>0</v>
+      </c>
+      <c r="D50" t="s">
         <v>70</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E50" t="s">
         <v>302</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F50" t="s">
         <v>68</v>
       </c>
-      <c r="G49">
+      <c r="G50">
         <v>2.75E-2</v>
       </c>
-      <c r="H49">
-        <v>0</v>
-      </c>
-      <c r="I49" t="b">
-        <v>1</v>
-      </c>
-      <c r="J49">
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50" t="b">
+        <v>1</v>
+      </c>
+      <c r="J50">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="K49">
-        <v>0.5</v>
-      </c>
-      <c r="L49">
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="L50">
         <v>2018</v>
       </c>
-      <c r="M49">
-        <v>0.01</v>
-      </c>
-      <c r="N49" t="b">
-        <v>1</v>
-      </c>
-      <c r="O49" s="43">
+      <c r="M50">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="N50" t="b">
+        <v>1</v>
+      </c>
+      <c r="O50" s="43">
         <v>0.11</v>
       </c>
-      <c r="P49">
+      <c r="P50">
         <v>0.02</v>
       </c>
-      <c r="Q49">
+      <c r="Q50">
         <v>0.05</v>
       </c>
-      <c r="R49">
+      <c r="R50">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:18">
-      <c r="A51" t="s">
-        <v>313</v>
+      <c r="A51" s="60" t="s">
+        <v>314</v>
       </c>
       <c r="B51" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C51" t="b">
         <v>0</v>
@@ -9603,7 +9730,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K51">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="L51">
         <v>2018</v>
@@ -9628,11 +9755,11 @@
       </c>
     </row>
     <row r="52" spans="1:18">
-      <c r="A52" t="s">
-        <v>314</v>
+      <c r="A52" s="60" t="s">
+        <v>315</v>
       </c>
       <c r="B52" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C52" t="b">
         <v>0</v>
@@ -9659,7 +9786,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K52">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="L52">
         <v>2018</v>
@@ -9684,120 +9811,77 @@
       </c>
     </row>
     <row r="53" spans="1:18">
-      <c r="A53" t="s">
-        <v>315</v>
-      </c>
-      <c r="B53" t="s">
-        <v>324</v>
-      </c>
-      <c r="C53" t="b">
-        <v>0</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="A53" s="60"/>
+    </row>
+    <row r="54" spans="1:18">
+      <c r="A54" s="60" t="s">
+        <v>388</v>
+      </c>
+      <c r="B54" t="s">
+        <v>390</v>
+      </c>
+      <c r="C54" t="b">
+        <v>1</v>
+      </c>
+      <c r="D54" t="s">
         <v>70</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E54" t="s">
         <v>302</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F54" t="s">
         <v>68</v>
       </c>
-      <c r="G53">
+      <c r="G54">
         <v>2.75E-2</v>
       </c>
-      <c r="H53">
-        <v>0</v>
-      </c>
-      <c r="I53" t="b">
-        <v>1</v>
-      </c>
-      <c r="J53">
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54" t="b">
+        <v>1</v>
+      </c>
+      <c r="J54">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="K53">
-        <v>0.5</v>
-      </c>
-      <c r="L53">
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="L54">
         <v>2018</v>
       </c>
-      <c r="M53">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="N53" t="b">
-        <v>1</v>
-      </c>
-      <c r="O53" s="43">
+      <c r="M54">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N54" t="b">
+        <v>1</v>
+      </c>
+      <c r="O54" s="43">
         <v>0.11</v>
       </c>
-      <c r="P53">
+      <c r="P54">
         <v>0.02</v>
       </c>
-      <c r="Q53">
+      <c r="Q54">
         <v>0.05</v>
       </c>
-      <c r="R53">
-        <v>0</v>
-      </c>
+      <c r="R54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18">
+      <c r="A55" s="60"/>
+      <c r="O55" s="43"/>
     </row>
     <row r="56" spans="1:18">
-      <c r="A56" t="s">
+      <c r="A56" s="60"/>
+    </row>
+    <row r="57" spans="1:18">
+      <c r="A57" s="60" t="s">
         <v>357</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>358</v>
-      </c>
-      <c r="C56" t="b">
-        <v>1</v>
-      </c>
-      <c r="D56" t="s">
-        <v>70</v>
-      </c>
-      <c r="E56" t="s">
-        <v>375</v>
-      </c>
-      <c r="F56" t="s">
-        <v>68</v>
-      </c>
-      <c r="G56">
-        <v>2.75E-2</v>
-      </c>
-      <c r="H56">
-        <v>0</v>
-      </c>
-      <c r="I56" t="b">
-        <v>1</v>
-      </c>
-      <c r="J56">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="K56">
-        <v>0</v>
-      </c>
-      <c r="L56">
-        <v>2018</v>
-      </c>
-      <c r="N56" t="b">
-        <v>1</v>
-      </c>
-      <c r="O56" s="43">
-        <v>0.11</v>
-      </c>
-      <c r="P56">
-        <v>0.03</v>
-      </c>
-      <c r="Q56">
-        <v>0.05</v>
-      </c>
-      <c r="R56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18">
-      <c r="A57" t="s">
-        <v>359</v>
-      </c>
-      <c r="B57" t="s">
-        <v>360</v>
       </c>
       <c r="C57" t="b">
         <v>1</v>
@@ -9824,7 +9908,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K57">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="L57">
         <v>2018</v>
@@ -9836,7 +9920,7 @@
         <v>0.11</v>
       </c>
       <c r="P57">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="Q57">
         <v>0.05</v>
@@ -9846,11 +9930,11 @@
       </c>
     </row>
     <row r="58" spans="1:18">
-      <c r="A58" t="s">
-        <v>361</v>
+      <c r="A58" s="60" t="s">
+        <v>359</v>
       </c>
       <c r="B58" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C58" t="b">
         <v>1</v>
@@ -9877,7 +9961,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K58">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="L58">
         <v>2018</v>
@@ -9899,70 +9983,68 @@
       </c>
     </row>
     <row r="59" spans="1:18">
-      <c r="O59" s="43"/>
+      <c r="A59" s="60" t="s">
+        <v>361</v>
+      </c>
+      <c r="B59" t="s">
+        <v>362</v>
+      </c>
+      <c r="C59" t="b">
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
+        <v>70</v>
+      </c>
+      <c r="E59" t="s">
+        <v>375</v>
+      </c>
+      <c r="F59" t="s">
+        <v>68</v>
+      </c>
+      <c r="G59">
+        <v>2.75E-2</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59" t="b">
+        <v>1</v>
+      </c>
+      <c r="J59">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K59">
+        <v>0.5</v>
+      </c>
+      <c r="L59">
+        <v>2018</v>
+      </c>
+      <c r="N59" t="b">
+        <v>1</v>
+      </c>
+      <c r="O59" s="43">
+        <v>0.11</v>
+      </c>
+      <c r="P59">
+        <v>0.03</v>
+      </c>
+      <c r="Q59">
+        <v>0.05</v>
+      </c>
+      <c r="R59">
+        <v>0</v>
+      </c>
     </row>
     <row r="60" spans="1:18">
-      <c r="A60" t="s">
+      <c r="A60" s="60"/>
+      <c r="O60" s="43"/>
+    </row>
+    <row r="61" spans="1:18">
+      <c r="A61" s="60" t="s">
         <v>363</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>364</v>
-      </c>
-      <c r="C60" t="b">
-        <v>1</v>
-      </c>
-      <c r="D60" t="s">
-        <v>70</v>
-      </c>
-      <c r="E60" t="s">
-        <v>375</v>
-      </c>
-      <c r="F60" t="s">
-        <v>68</v>
-      </c>
-      <c r="G60">
-        <v>2.75E-2</v>
-      </c>
-      <c r="H60">
-        <v>0</v>
-      </c>
-      <c r="I60" t="b">
-        <v>1</v>
-      </c>
-      <c r="J60">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="K60">
-        <v>0</v>
-      </c>
-      <c r="L60">
-        <v>2018</v>
-      </c>
-      <c r="M60">
-        <v>0.01</v>
-      </c>
-      <c r="N60" t="b">
-        <v>1</v>
-      </c>
-      <c r="O60" s="43">
-        <v>0.11</v>
-      </c>
-      <c r="P60">
-        <v>0.03</v>
-      </c>
-      <c r="Q60">
-        <v>0.05</v>
-      </c>
-      <c r="R60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:18">
-      <c r="A61" t="s">
-        <v>365</v>
-      </c>
-      <c r="B61" t="s">
-        <v>366</v>
       </c>
       <c r="C61" t="b">
         <v>1</v>
@@ -9989,7 +10071,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K61">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="L61">
         <v>2018</v>
@@ -10014,11 +10096,11 @@
       </c>
     </row>
     <row r="62" spans="1:18">
-      <c r="A62" t="s">
-        <v>367</v>
+      <c r="A62" s="60" t="s">
+        <v>365</v>
       </c>
       <c r="B62" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C62" t="b">
         <v>1</v>
@@ -10045,7 +10127,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K62">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="L62">
         <v>2018</v>
@@ -10069,68 +10151,71 @@
         <v>0</v>
       </c>
     </row>
+    <row r="63" spans="1:18">
+      <c r="A63" s="60" t="s">
+        <v>367</v>
+      </c>
+      <c r="B63" t="s">
+        <v>368</v>
+      </c>
+      <c r="C63" t="b">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
+        <v>70</v>
+      </c>
+      <c r="E63" t="s">
+        <v>375</v>
+      </c>
+      <c r="F63" t="s">
+        <v>68</v>
+      </c>
+      <c r="G63">
+        <v>2.75E-2</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63" t="b">
+        <v>1</v>
+      </c>
+      <c r="J63">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K63">
+        <v>0.5</v>
+      </c>
+      <c r="L63">
+        <v>2018</v>
+      </c>
+      <c r="M63">
+        <v>0.01</v>
+      </c>
+      <c r="N63" t="b">
+        <v>1</v>
+      </c>
+      <c r="O63" s="43">
+        <v>0.11</v>
+      </c>
+      <c r="P63">
+        <v>0.03</v>
+      </c>
+      <c r="Q63">
+        <v>0.05</v>
+      </c>
+      <c r="R63">
+        <v>0</v>
+      </c>
+    </row>
     <row r="64" spans="1:18">
-      <c r="A64" t="s">
+      <c r="A64" s="60"/>
+    </row>
+    <row r="65" spans="1:18">
+      <c r="A65" s="60" t="s">
         <v>369</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>370</v>
-      </c>
-      <c r="C64" t="b">
-        <v>1</v>
-      </c>
-      <c r="D64" t="s">
-        <v>70</v>
-      </c>
-      <c r="E64" t="s">
-        <v>375</v>
-      </c>
-      <c r="F64" t="s">
-        <v>68</v>
-      </c>
-      <c r="G64">
-        <v>2.75E-2</v>
-      </c>
-      <c r="H64">
-        <v>0</v>
-      </c>
-      <c r="I64" t="b">
-        <v>1</v>
-      </c>
-      <c r="J64">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="K64">
-        <v>0</v>
-      </c>
-      <c r="L64">
-        <v>2018</v>
-      </c>
-      <c r="M64">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="N64" t="b">
-        <v>1</v>
-      </c>
-      <c r="O64" s="43">
-        <v>0.11</v>
-      </c>
-      <c r="P64">
-        <v>0.03</v>
-      </c>
-      <c r="Q64">
-        <v>0.05</v>
-      </c>
-      <c r="R64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18">
-      <c r="A65" t="s">
-        <v>371</v>
-      </c>
-      <c r="B65" t="s">
-        <v>372</v>
       </c>
       <c r="C65" t="b">
         <v>1</v>
@@ -10157,7 +10242,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K65">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="L65">
         <v>2018</v>
@@ -10182,11 +10267,11 @@
       </c>
     </row>
     <row r="66" spans="1:18">
-      <c r="A66" t="s">
-        <v>373</v>
+      <c r="A66" s="60" t="s">
+        <v>371</v>
       </c>
       <c r="B66" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C66" t="b">
         <v>1</v>
@@ -10213,7 +10298,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="K66">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="L66">
         <v>2018</v>
@@ -10237,12 +10322,345 @@
         <v>0</v>
       </c>
     </row>
+    <row r="67" spans="1:18">
+      <c r="A67" s="60" t="s">
+        <v>373</v>
+      </c>
+      <c r="B67" t="s">
+        <v>374</v>
+      </c>
+      <c r="C67" t="b">
+        <v>1</v>
+      </c>
+      <c r="D67" t="s">
+        <v>70</v>
+      </c>
+      <c r="E67" t="s">
+        <v>375</v>
+      </c>
+      <c r="F67" t="s">
+        <v>68</v>
+      </c>
+      <c r="G67">
+        <v>2.75E-2</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67" t="b">
+        <v>1</v>
+      </c>
+      <c r="J67">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K67">
+        <v>0.5</v>
+      </c>
+      <c r="L67">
+        <v>2018</v>
+      </c>
+      <c r="M67">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="N67" t="b">
+        <v>1</v>
+      </c>
+      <c r="O67" s="43">
+        <v>0.11</v>
+      </c>
+      <c r="P67">
+        <v>0.03</v>
+      </c>
+      <c r="Q67">
+        <v>0.05</v>
+      </c>
+      <c r="R67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18">
+      <c r="A68" s="60"/>
+    </row>
+    <row r="69" spans="1:18">
+      <c r="A69" s="60" t="s">
+        <v>389</v>
+      </c>
+      <c r="B69" t="s">
+        <v>391</v>
+      </c>
+      <c r="C69" t="b">
+        <v>1</v>
+      </c>
+      <c r="D69" t="s">
+        <v>70</v>
+      </c>
+      <c r="E69" t="s">
+        <v>375</v>
+      </c>
+      <c r="F69" t="s">
+        <v>68</v>
+      </c>
+      <c r="G69">
+        <v>2.75E-2</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69" t="b">
+        <v>1</v>
+      </c>
+      <c r="J69">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K69">
+        <v>0</v>
+      </c>
+      <c r="L69">
+        <v>2018</v>
+      </c>
+      <c r="M69">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N69" t="b">
+        <v>1</v>
+      </c>
+      <c r="O69" s="43">
+        <v>0.11</v>
+      </c>
+      <c r="P69">
+        <v>0.03</v>
+      </c>
+      <c r="Q69">
+        <v>0.05</v>
+      </c>
+      <c r="R69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18">
+      <c r="A72" t="s">
+        <v>380</v>
+      </c>
+      <c r="B72" t="s">
+        <v>381</v>
+      </c>
+      <c r="C72" t="b">
+        <v>0</v>
+      </c>
+      <c r="D72" t="s">
+        <v>70</v>
+      </c>
+      <c r="E72" t="s">
+        <v>302</v>
+      </c>
+      <c r="F72" t="s">
+        <v>68</v>
+      </c>
+      <c r="G72">
+        <v>2.75E-2</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72" t="b">
+        <v>1</v>
+      </c>
+      <c r="J72">
+        <v>0.05</v>
+      </c>
+      <c r="K72">
+        <v>0</v>
+      </c>
+      <c r="L72">
+        <v>2018</v>
+      </c>
+      <c r="N72" t="b">
+        <v>1</v>
+      </c>
+      <c r="O72" s="43">
+        <v>0.11</v>
+      </c>
+      <c r="P72">
+        <v>0.02</v>
+      </c>
+      <c r="Q72">
+        <v>0.05</v>
+      </c>
+      <c r="R72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18">
+      <c r="A73" t="s">
+        <v>382</v>
+      </c>
+      <c r="B73" t="s">
+        <v>383</v>
+      </c>
+      <c r="C73" t="b">
+        <v>0</v>
+      </c>
+      <c r="D73" t="s">
+        <v>70</v>
+      </c>
+      <c r="E73" t="s">
+        <v>375</v>
+      </c>
+      <c r="F73" t="s">
+        <v>68</v>
+      </c>
+      <c r="G73">
+        <v>2.75E-2</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73" t="b">
+        <v>1</v>
+      </c>
+      <c r="J73">
+        <v>0.05</v>
+      </c>
+      <c r="K73">
+        <v>0</v>
+      </c>
+      <c r="L73">
+        <v>2018</v>
+      </c>
+      <c r="N73" t="b">
+        <v>1</v>
+      </c>
+      <c r="O73" s="43">
+        <v>0.11</v>
+      </c>
+      <c r="P73">
+        <v>0.03</v>
+      </c>
+      <c r="Q73">
+        <v>0.05</v>
+      </c>
+      <c r="R73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18">
+      <c r="A75" t="s">
+        <v>384</v>
+      </c>
+      <c r="B75" t="s">
+        <v>385</v>
+      </c>
+      <c r="C75" t="b">
+        <v>0</v>
+      </c>
+      <c r="D75" t="s">
+        <v>70</v>
+      </c>
+      <c r="E75" t="s">
+        <v>302</v>
+      </c>
+      <c r="F75" t="s">
+        <v>68</v>
+      </c>
+      <c r="G75">
+        <v>2.75E-2</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75" t="b">
+        <v>1</v>
+      </c>
+      <c r="J75">
+        <v>0.05</v>
+      </c>
+      <c r="K75">
+        <v>0.5</v>
+      </c>
+      <c r="L75">
+        <v>2018</v>
+      </c>
+      <c r="M75">
+        <v>0.01</v>
+      </c>
+      <c r="N75" t="b">
+        <v>1</v>
+      </c>
+      <c r="O75" s="43">
+        <v>0.11</v>
+      </c>
+      <c r="P75">
+        <v>0.02</v>
+      </c>
+      <c r="Q75">
+        <v>0.05</v>
+      </c>
+      <c r="R75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18">
+      <c r="A76" t="s">
+        <v>386</v>
+      </c>
+      <c r="B76" t="s">
+        <v>387</v>
+      </c>
+      <c r="C76" t="b">
+        <v>0</v>
+      </c>
+      <c r="D76" t="s">
+        <v>70</v>
+      </c>
+      <c r="E76" t="s">
+        <v>375</v>
+      </c>
+      <c r="F76" t="s">
+        <v>68</v>
+      </c>
+      <c r="G76">
+        <v>2.75E-2</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+      <c r="I76" t="b">
+        <v>1</v>
+      </c>
+      <c r="J76">
+        <v>0.05</v>
+      </c>
+      <c r="K76">
+        <v>0.5</v>
+      </c>
+      <c r="L76">
+        <v>2018</v>
+      </c>
+      <c r="M76">
+        <v>0.01</v>
+      </c>
+      <c r="N76" t="b">
+        <v>1</v>
+      </c>
+      <c r="O76" s="43">
+        <v>0.11</v>
+      </c>
+      <c r="P76">
+        <v>0.03</v>
+      </c>
+      <c r="Q76">
+        <v>0.05</v>
+      </c>
+      <c r="R76">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C33:C37 C5:C31 C40 C56:C66 C43:C53" xr:uid="{CE4DB086-8939-4E0F-A217-D1528E507A37}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C33:C37 C5:C31 C42:C52 C54:C55 C72:C76 C57:C69" xr:uid="{CE4DB086-8939-4E0F-A217-D1528E507A37}">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D24:D26 D5:D9 D11:D13 D28:D31 D20:D22 D15:D17 D33:D34 D36:D37 D40 D43:D45 D47:D49 D51:D53 D60:D62 D64:D66 D56:D58" xr:uid="{B6635BCF-58EB-45FF-9851-3E5464D67D97}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D24:D26 D5:D9 D11:D13 D28:D31 D20:D22 D15:D17 D33:D34 D36:D37 D42:D44 D46:D48 D50:D52 D61:D63 D65:D67 D57:D59 D72:D73 D75:D76 D54:D55 D69" xr:uid="{B6635BCF-58EB-45FF-9851-3E5464D67D97}">
       <formula1>"singleTier,multiTier"</formula1>
     </dataValidation>
   </dataValidations>
@@ -17001,7 +17419,7 @@
   <dimension ref="A3:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17051,7 +17469,7 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -17099,7 +17517,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17196,7 +17614,7 @@
         <v>0.12</v>
       </c>
       <c r="D4">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" si="0"/>
@@ -17250,10 +17668,10 @@
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="F6" s="6">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="G6" t="s">
         <v>115</v>
@@ -17370,7 +17788,7 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
@@ -17392,13 +17810,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD963C7-C30C-4F41-9ED1-A3A9BFD95FFA}">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomRight" activeCell="I24" sqref="I24:I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -17409,15 +17827,17 @@
     <col min="4" max="4" width="16.5703125" style="27" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="26"/>
     <col min="6" max="9" width="14.85546875" style="26" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="26"/>
+    <col min="10" max="10" width="9.140625" style="26"/>
+    <col min="11" max="11" width="18.5703125" style="26" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" s="26" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:11">
       <c r="B3" s="28" t="s">
         <v>83</v>
       </c>
@@ -17439,13 +17859,16 @@
       <c r="I3" s="29" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="K3" s="58" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="29" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:11">
       <c r="A5" s="26" t="s">
         <v>89</v>
       </c>
@@ -17468,8 +17891,16 @@
       <c r="H5" s="26">
         <v>7311</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="I5" s="27">
+        <f t="shared" ref="I5:I6" si="0">SUM(F5:H5)</f>
+        <v>76935</v>
+      </c>
+      <c r="K5" s="57">
+        <f>SUM(D5,I5)</f>
+        <v>263148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="26" t="s">
         <v>90</v>
       </c>
@@ -17480,7 +17911,7 @@
         <v>8909</v>
       </c>
       <c r="D6" s="27">
-        <f t="shared" ref="D6:D25" si="0">SUM(B6:C6)</f>
+        <f t="shared" ref="D6:D25" si="1">SUM(B6:C6)</f>
         <v>46495</v>
       </c>
       <c r="F6" s="27">
@@ -17492,8 +17923,16 @@
       <c r="H6" s="26">
         <v>265</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="I6" s="27">
+        <f t="shared" si="0"/>
+        <v>12394</v>
+      </c>
+      <c r="K6" s="57">
+        <f t="shared" ref="K6:K12" si="2">SUM(D6,I6)</f>
+        <v>58889</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="26" t="s">
         <v>91</v>
       </c>
@@ -17504,7 +17943,7 @@
         <v>3566</v>
       </c>
       <c r="D7" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>64571</v>
       </c>
       <c r="F7" s="27">
@@ -17520,8 +17959,12 @@
         <f>SUM(F7:H7)</f>
         <v>14632</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="K7" s="57">
+        <f t="shared" si="2"/>
+        <v>79203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="26" t="s">
         <v>92</v>
       </c>
@@ -17532,7 +17975,7 @@
         <v>14642</v>
       </c>
       <c r="D8" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>209800</v>
       </c>
       <c r="F8" s="27">
@@ -17545,11 +17988,15 @@
         <v>9158</v>
       </c>
       <c r="I8" s="27">
-        <f t="shared" ref="I8:I25" si="1">SUM(F8:H8)</f>
+        <f t="shared" ref="I8:I25" si="3">SUM(F8:H8)</f>
         <v>74854</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="K8" s="57">
+        <f t="shared" si="2"/>
+        <v>284654</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="26" t="s">
         <v>71</v>
       </c>
@@ -17560,7 +18007,7 @@
         <v>38928</v>
       </c>
       <c r="D9" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>507079</v>
       </c>
       <c r="F9" s="27">
@@ -17573,16 +18020,20 @@
         <v>17185</v>
       </c>
       <c r="I9" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>178815</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="K9" s="57">
+        <f t="shared" si="2"/>
+        <v>685894</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="G10" s="27"/>
       <c r="H10" s="27"/>
       <c r="I10" s="27"/>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1">
+    <row r="11" spans="1:11" ht="15" customHeight="1">
       <c r="A11" s="30" t="s">
         <v>98</v>
       </c>
@@ -17593,7 +18044,7 @@
         <v>699252899</v>
       </c>
       <c r="D11" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12950836352</v>
       </c>
       <c r="F11" s="27">
@@ -17606,11 +18057,15 @@
         <v>871895121</v>
       </c>
       <c r="I11" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6710667300</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1">
+      <c r="K11" s="57">
+        <f t="shared" si="2"/>
+        <v>19661503652</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15" customHeight="1">
       <c r="A12" s="30" t="s">
         <v>99</v>
       </c>
@@ -17621,7 +18076,7 @@
         <v>738240618</v>
       </c>
       <c r="D12" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13672926421</v>
       </c>
       <c r="F12" s="27">
@@ -17634,18 +18089,22 @@
         <v>920508723</v>
       </c>
       <c r="I12" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7084828944</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1">
+      <c r="K12" s="57">
+        <f t="shared" si="2"/>
+        <v>20757755365</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15" customHeight="1">
       <c r="A13" s="30"/>
       <c r="B13" s="31"/>
       <c r="G13" s="27"/>
       <c r="H13" s="27"/>
       <c r="I13" s="27"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:11">
       <c r="A14" s="29" t="s">
         <v>87</v>
       </c>
@@ -17653,7 +18112,7 @@
       <c r="H14" s="27"/>
       <c r="I14" s="27"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:11">
       <c r="A15" s="30" t="s">
         <v>93</v>
       </c>
@@ -17664,7 +18123,7 @@
         <v>5746905539</v>
       </c>
       <c r="D15" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>138193579136</v>
       </c>
       <c r="F15" s="51">
@@ -17677,11 +18136,15 @@
         <v>15894543442</v>
       </c>
       <c r="I15" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>91425617716</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="K15" s="57">
+        <f t="shared" ref="K15:K18" si="4">SUM(D15,I15)</f>
+        <v>229619196852</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="30" t="s">
         <v>94</v>
       </c>
@@ -17692,7 +18155,7 @@
         <v>4670036601</v>
       </c>
       <c r="D16" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>120139095571</v>
       </c>
       <c r="F16" s="51">
@@ -17705,11 +18168,15 @@
         <v>13383782393</v>
       </c>
       <c r="I16" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>75766994231</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="K16" s="57">
+        <f t="shared" si="4"/>
+        <v>195906089802</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="30" t="s">
         <v>95</v>
       </c>
@@ -17720,7 +18187,7 @@
         <v>3589902866</v>
       </c>
       <c r="D17" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>83812972822</v>
       </c>
       <c r="F17" s="51">
@@ -17733,11 +18200,15 @@
         <v>8540511923</v>
       </c>
       <c r="I17" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>52418448576</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="K17" s="57">
+        <f t="shared" si="4"/>
+        <v>136231421398</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="30" t="s">
         <v>96</v>
       </c>
@@ -17748,7 +18219,7 @@
         <v>1080133735</v>
       </c>
       <c r="D18" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36326122749</v>
       </c>
       <c r="F18" s="51">
@@ -17761,11 +18232,15 @@
         <v>4843270470</v>
       </c>
       <c r="I18" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>23348545655</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="K18" s="57">
+        <f t="shared" si="4"/>
+        <v>59674668404</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="30" t="s">
         <v>97</v>
       </c>
@@ -17795,14 +18270,18 @@
         <f>I17/I16</f>
         <v>0.69183750930102272</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="K19" s="36">
+        <f>K17/K16</f>
+        <v>0.69539145789540036</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="30"/>
       <c r="G20" s="27"/>
       <c r="H20" s="27"/>
       <c r="I20" s="27"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:11">
       <c r="A21" s="29" t="s">
         <v>88</v>
       </c>
@@ -17810,7 +18289,7 @@
       <c r="H21" s="27"/>
       <c r="I21" s="27"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:11">
       <c r="A22" s="30" t="s">
         <v>100</v>
       </c>
@@ -17821,7 +18300,7 @@
         <v>134810119</v>
       </c>
       <c r="D22" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2309480985</v>
       </c>
       <c r="F22" s="52">
@@ -17834,11 +18313,15 @@
         <v>274753444</v>
       </c>
       <c r="I22" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1953487065</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="K22" s="57">
+        <f t="shared" ref="K22:K25" si="5">SUM(D22,I22)</f>
+        <v>4262968050</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="30" t="s">
         <v>101</v>
       </c>
@@ -17849,7 +18332,7 @@
         <v>58830395</v>
       </c>
       <c r="D23" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>951994767</v>
       </c>
       <c r="F23" s="52">
@@ -17862,11 +18345,15 @@
         <v>96865133</v>
       </c>
       <c r="I23" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>779306151</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="K23" s="57">
+        <f t="shared" si="5"/>
+        <v>1731300918</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="30" t="s">
         <v>102</v>
       </c>
@@ -17877,7 +18364,7 @@
         <v>75979724</v>
       </c>
       <c r="D24" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1357486218</v>
       </c>
       <c r="F24" s="52">
@@ -17890,11 +18377,15 @@
         <v>177888311</v>
       </c>
       <c r="I24" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1174180914</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="15" customHeight="1">
+      <c r="K24" s="57">
+        <f t="shared" si="5"/>
+        <v>2531667132</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15" customHeight="1">
       <c r="A25" s="30" t="s">
         <v>103</v>
       </c>
@@ -17905,7 +18396,7 @@
         <v>77744321</v>
       </c>
       <c r="D25" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2802909539</v>
       </c>
       <c r="F25" s="52">
@@ -17918,16 +18409,20 @@
         <v>354215017</v>
       </c>
       <c r="I25" s="27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1639603725</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="25.5">
+      <c r="K25" s="57">
+        <f t="shared" si="5"/>
+        <v>4442513264</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="25.5">
       <c r="A27" s="33" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:11">
       <c r="A28" s="30" t="s">
         <v>100</v>
       </c>
@@ -17954,8 +18449,12 @@
         <f>I22/$I$12</f>
         <v>0.27572819053794789</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="K28" s="36">
+        <f>K22/$K$12</f>
+        <v>0.20536748675571453</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" s="30" t="s">
         <v>101</v>
       </c>
@@ -17966,7 +18465,7 @@
         <v>7.9689999999999997E-2</v>
       </c>
       <c r="D29" s="36">
-        <f t="shared" ref="D29:D31" si="2">D23/$D$12</f>
+        <f t="shared" ref="D29:D31" si="6">D23/$D$12</f>
         <v>6.9626262709777217E-2</v>
       </c>
       <c r="F29" s="53">
@@ -17979,11 +18478,15 @@
         <v>0.10523</v>
       </c>
       <c r="I29" s="36">
-        <f t="shared" ref="I29:I31" si="3">I23/$I$12</f>
+        <f t="shared" ref="I29:I31" si="7">I23/$I$12</f>
         <v>0.10999646669803917</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="K29" s="36">
+        <f t="shared" ref="K29:K31" si="8">K23/$K$12</f>
+        <v>8.3405015983528522E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" s="30" t="s">
         <v>102</v>
       </c>
@@ -17994,7 +18497,7 @@
         <v>0.10292</v>
       </c>
       <c r="D30" s="36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>9.9282785279606378E-2</v>
       </c>
       <c r="F30" s="53">
@@ -18007,11 +18510,15 @@
         <v>0.19325000000000001</v>
       </c>
       <c r="I30" s="36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.1657317238399087</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="15" customHeight="1">
+      <c r="K30" s="36">
+        <f t="shared" si="8"/>
+        <v>0.12196247077218601</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="15" customHeight="1">
       <c r="A31" s="30" t="s">
         <v>103</v>
       </c>
@@ -18022,7 +18529,7 @@
         <v>0.10531</v>
       </c>
       <c r="D31" s="36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.20499704691565238</v>
       </c>
       <c r="F31" s="53">
@@ -18035,11 +18542,15 @@
         <v>0.38479999999999998</v>
       </c>
       <c r="I31" s="36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.23142460290287567</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="K31" s="36">
+        <f t="shared" si="8"/>
+        <v>0.21401703536262867</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32" s="30" t="s">
         <v>71</v>
       </c>
@@ -18066,13 +18577,17 @@
         <f>SUM(I24:I25)/$I$12</f>
         <v>0.39715632674278439</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="25.5">
+      <c r="K32" s="36">
+        <f>SUM(K24:K25)/$K$12</f>
+        <v>0.3359795061348147</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="25.5">
       <c r="A34" s="33" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:11">
       <c r="A35" s="30" t="s">
         <v>100</v>
       </c>
@@ -18104,107 +18619,123 @@
         <f>I22/I$11</f>
         <v>0.29110176047618991</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="K35" s="36">
+        <f>K22/K$11</f>
+        <v>0.21681800768917101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" s="30" t="s">
         <v>101</v>
       </c>
       <c r="B36" s="36">
-        <f t="shared" ref="B36:C38" si="4">B23/B$11</f>
+        <f t="shared" ref="B36:C38" si="9">B23/B$11</f>
         <v>7.2901953892441071E-2</v>
       </c>
       <c r="C36" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>8.4133215728005153E-2</v>
       </c>
       <c r="D36" s="36">
-        <f t="shared" ref="D36:F36" si="5">D23/D$11</f>
+        <f t="shared" ref="D36:F36" si="10">D23/D$11</f>
         <v>7.3508362018101112E-2</v>
       </c>
       <c r="F36" s="36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.110696043016053</v>
       </c>
       <c r="G36" s="36">
-        <f t="shared" ref="G36:H36" si="6">G23/G$11</f>
+        <f t="shared" ref="G36:H36" si="11">G23/G$11</f>
         <v>0.12094743606951874</v>
       </c>
       <c r="H36" s="36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.11109723023670871</v>
       </c>
       <c r="I36" s="36">
-        <f t="shared" ref="I36" si="7">I23/I$11</f>
+        <f t="shared" ref="I36:K36" si="12">I23/I$11</f>
         <v>0.11612945720018038</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="K36" s="36">
+        <f t="shared" si="12"/>
+        <v>8.8055366905973612E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37" s="30" t="s">
         <v>102</v>
       </c>
       <c r="B37" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.1045992543670918</v>
       </c>
       <c r="C37" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.10865843260522542</v>
       </c>
       <c r="D37" s="36">
-        <f t="shared" ref="D37:F37" si="8">D24/D$11</f>
+        <f t="shared" ref="D37:F37" si="13">D24/D$11</f>
         <v>0.10481842107366009</v>
       </c>
       <c r="F37" s="36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.13409160112945948</v>
       </c>
       <c r="G37" s="36">
-        <f t="shared" ref="G37:H37" si="9">G24/G$11</f>
+        <f t="shared" ref="G37:H37" si="14">G24/G$11</f>
         <v>0.19466033730326945</v>
       </c>
       <c r="H37" s="36">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0.20402489555851064</v>
       </c>
       <c r="I37" s="36">
-        <f t="shared" ref="I37" si="10">I24/I$11</f>
+        <f t="shared" ref="I37:K37" si="15">I24/I$11</f>
         <v>0.17497230327600952</v>
       </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="K37" s="36">
+        <f t="shared" si="15"/>
+        <v>0.12876264078319741</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38" s="30" t="s">
         <v>103</v>
       </c>
       <c r="B38" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.222433714666711</v>
       </c>
       <c r="C38" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.11118197881078788</v>
       </c>
       <c r="D38" s="36">
-        <f t="shared" ref="D38:F38" si="11">D25/D$11</f>
+        <f t="shared" ref="D38:F38" si="16">D25/D$11</f>
         <v>0.21642691350718413</v>
       </c>
       <c r="F38" s="36">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>9.3173975543692972E-2</v>
       </c>
       <c r="G38" s="36">
-        <f t="shared" ref="G38:H38" si="12">G25/G$11</f>
+        <f t="shared" ref="G38:H38" si="17">G25/G$11</f>
         <v>0.30363134916273504</v>
       </c>
       <c r="H38" s="36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>0.40625874427848757</v>
       </c>
       <c r="I38" s="36">
-        <f t="shared" ref="I38" si="13">I25/I$11</f>
+        <f t="shared" ref="I38:K38" si="18">I25/I$11</f>
         <v>0.24432797093070013</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="K38" s="36">
+        <f t="shared" si="18"/>
+        <v>0.22594982269060079</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39" s="30" t="s">
         <v>71</v>
       </c>
@@ -18213,28 +18744,32 @@
         <v>0.3270329690338028</v>
       </c>
       <c r="C39" s="36">
-        <f t="shared" ref="C39:D39" si="14">SUM(C24:C25)/C$11</f>
+        <f t="shared" ref="C39:D39" si="19">SUM(C24:C25)/C$11</f>
         <v>0.21984041141601332</v>
       </c>
       <c r="D39" s="36">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>0.3212453345808442</v>
       </c>
       <c r="F39" s="36">
-        <f t="shared" ref="F39:G39" si="15">SUM(F24:F25)/F$11</f>
+        <f t="shared" ref="F39:G39" si="20">SUM(F24:F25)/F$11</f>
         <v>0.22726557667315242</v>
       </c>
       <c r="G39" s="36">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>0.49829168646600452</v>
       </c>
       <c r="H39" s="36">
-        <f t="shared" ref="H39:I39" si="16">SUM(H24:H25)/H$11</f>
+        <f t="shared" ref="H39:I39" si="21">SUM(H24:H25)/H$11</f>
         <v>0.61028363983699829</v>
       </c>
       <c r="I39" s="36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>0.41930027420670968</v>
+      </c>
+      <c r="K39" s="36">
+        <f t="shared" ref="K39" si="22">SUM(K24:K25)/K$11</f>
+        <v>0.3547124634737982</v>
       </c>
     </row>
   </sheetData>
@@ -18278,15 +18813,15 @@
       </c>
     </row>
     <row r="3" spans="1:18">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="59" t="s">
         <v>269</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57" t="s">
+      <c r="C3" s="59"/>
+      <c r="D3" s="59" t="s">
         <v>270</v>
       </c>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="1"/>

</xml_diff>

<commit_message>
update with changes for demo
</commit_message>
<xml_diff>
--- a/model/RunControl.xlsx
+++ b/model/RunControl.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C4E785-5608-48B3-894A-30396D2720AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB9A9F4-0243-4CEA-B37C-65D2013A2717}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1845" windowWidth="29040" windowHeight="15840" tabRatio="524" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params_sim" sheetId="22" r:id="rId1"/>
@@ -44,6 +44,7 @@
     <author>Author</author>
     <author>tc={1E17415D-3C00-4D50-B13B-6BE374701D46}</author>
     <author>tc={CAF507CB-F634-4E84-8E7F-17CD8E2A0EDC}</author>
+    <author>tc={8515E407-C037-4E97-A4C6-62FC0108B1A6}</author>
   </authors>
   <commentList>
     <comment ref="E4" authorId="0" shapeId="0" xr:uid="{CDE40F89-78CF-4C3B-B38C-D04825AF5F6F}">
@@ -84,6 +85,14 @@
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     the DR used in determining COLA. Leave blank (NA when loaded) if the DR for regular valuation is used.</t>
+      </text>
+    </comment>
+    <comment ref="S4" authorId="3" shapeId="0" xr:uid="{8515E407-C037-4E97-A4C6-62FC0108B1A6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The esclator is calibrated from 2.75% to 3.5% to match the 2018 SC</t>
       </text>
     </comment>
     <comment ref="W4" authorId="0" shapeId="0" xr:uid="{568404F5-400A-46EF-8AA1-93D4C44E460E}">
@@ -372,7 +381,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1789" uniqueCount="439">
   <si>
     <t>nsim</t>
   </si>
@@ -1641,6 +1650,117 @@
   </si>
   <si>
     <t>Keep all existing amort. basis and do NOT add new basis for the policy changes</t>
+  </si>
+  <si>
+    <t>poff2t_bf100_cola2</t>
+  </si>
+  <si>
+    <t>poff2t, 3%bfactor, 2%cola, current policy</t>
+  </si>
+  <si>
+    <t>poff2t_bf75_cola2</t>
+  </si>
+  <si>
+    <t>poff2t, 2.25%bfactor(new), 2%cola</t>
+  </si>
+  <si>
+    <t>poff2t_bf50_cola2</t>
+  </si>
+  <si>
+    <t>poff2t, 1.5%bfactor(new), 2%cola</t>
+  </si>
+  <si>
+    <t>poff2t_bf100_cola1</t>
+  </si>
+  <si>
+    <t>poff2t, 3%bfactor, 1%cola(cola suspension)</t>
+  </si>
+  <si>
+    <t>poff2t_bf75_cola1</t>
+  </si>
+  <si>
+    <t>poff2t, 2.25%bfactor(new), 1%cola(cola suspension)</t>
+  </si>
+  <si>
+    <t>poff2t_bf50_cola1</t>
+  </si>
+  <si>
+    <t>poff2t, 1.5%bfactor(new), 1%cola(cola suspension)</t>
+  </si>
+  <si>
+    <t>poff2t_bf100_cola1p5</t>
+  </si>
+  <si>
+    <t>poff2t, 3%bfactor, 1.5%cola(cola suspension)</t>
+  </si>
+  <si>
+    <t>poff2t_bf75_cola1p5</t>
+  </si>
+  <si>
+    <t>poff2t, 2.25%bfactor(new), 1.5%cola(cola suspension)</t>
+  </si>
+  <si>
+    <t>poff2t_bf50_cola1p5</t>
+  </si>
+  <si>
+    <t>poff2t, 1.5%bfactor(new), 1.5%cola(cola suspension)</t>
+  </si>
+  <si>
+    <t>poff2t_bf100_colap5</t>
+  </si>
+  <si>
+    <t>poff2t, 3%bfactor, 0.5%cola(cola suspension)</t>
+  </si>
+  <si>
+    <t>"poff_classic","poff_pepra"</t>
+  </si>
+  <si>
+    <t>poff members: baseline</t>
+  </si>
+  <si>
+    <t>poff2t_baseline</t>
+  </si>
+  <si>
+    <t>PERF A policy for poff, poff, chp</t>
+  </si>
+  <si>
+    <t>poff2t_benCut1_lowERC</t>
+  </si>
+  <si>
+    <t>poff2t_benCut1_highERC</t>
+  </si>
+  <si>
+    <t>poff2t_colaCut1_lowERC</t>
+  </si>
+  <si>
+    <t>poff2t_colaCut1_highERC</t>
+  </si>
+  <si>
+    <t>poff2t_benCut1_colaCut1_lowERC</t>
+  </si>
+  <si>
+    <t>poff2t_benCut1_colaCut1_highERC</t>
+  </si>
+  <si>
+    <t>poff2t_benCut2_lowERC</t>
+  </si>
+  <si>
+    <t>poff2t_benCut2_highERC</t>
+  </si>
+  <si>
+    <t>poff2t_colaCut2_lowERC</t>
+  </si>
+  <si>
+    <t>poff2t_colaCut2_highERC</t>
+  </si>
+  <si>
+    <t>poff2t_benCut2_colaCut2_lowERC</t>
+  </si>
+  <si>
+    <t>poff2t_benCut2_colaCut2_highERC</t>
+  </si>
+  <si>
+    <t>total employer cost</t>
   </si>
 </sst>
 </file>
@@ -2006,10 +2126,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2313,6 +2429,9 @@
   <threadedComment ref="N4" dT="2020-08-16T01:43:29.52" personId="{00000000-0000-0000-0000-000000000000}" id="{CAF507CB-F634-4E84-8E7F-17CD8E2A0EDC}">
     <text>the DR used in determining COLA. Leave blank (NA when loaded) if the DR for regular valuation is used.</text>
   </threadedComment>
+  <threadedComment ref="S4" dT="2020-12-06T12:17:58.66" personId="{00000000-0000-0000-0000-000000000000}" id="{8515E407-C037-4E97-A4C6-62FC0108B1A6}">
+    <text>The esclator is calibrated from 2.75% to 3.5% to match the 2018 SC</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -2364,13 +2483,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D014B46A-D012-4D18-AEAB-1D829080B2CE}">
-  <dimension ref="A2:AS72"/>
+  <dimension ref="A2:AS91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomRight" activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2663,7 +2782,7 @@
         <v>20</v>
       </c>
       <c r="S5">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T5">
         <v>5</v>
@@ -2802,7 +2921,7 @@
         <v>20</v>
       </c>
       <c r="S8">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T8">
         <v>5</v>
@@ -2894,7 +3013,7 @@
         <v>138</v>
       </c>
       <c r="C10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
@@ -2936,7 +3055,7 @@
         <v>20</v>
       </c>
       <c r="S10">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T10">
         <v>5</v>
@@ -3021,7 +3140,7 @@
         <v>196</v>
       </c>
       <c r="C11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
@@ -3063,7 +3182,7 @@
         <v>20</v>
       </c>
       <c r="S11">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T11">
         <v>5</v>
@@ -3148,7 +3267,7 @@
         <v>136</v>
       </c>
       <c r="C13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
@@ -3190,7 +3309,7 @@
         <v>20</v>
       </c>
       <c r="S13">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T13">
         <v>5</v>
@@ -3273,7 +3392,7 @@
         <v>168</v>
       </c>
       <c r="C14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
@@ -3315,7 +3434,7 @@
         <v>20</v>
       </c>
       <c r="S14">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T14">
         <v>5</v>
@@ -3398,7 +3517,7 @@
         <v>145</v>
       </c>
       <c r="C16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
@@ -3440,7 +3559,7 @@
         <v>20</v>
       </c>
       <c r="S16">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T16">
         <v>5</v>
@@ -3523,7 +3642,7 @@
         <v>146</v>
       </c>
       <c r="C17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
@@ -3565,7 +3684,7 @@
         <v>20</v>
       </c>
       <c r="S17">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T17">
         <v>5</v>
@@ -3653,6 +3772,9 @@
       <c r="B19" s="56" t="s">
         <v>233</v>
       </c>
+      <c r="C19" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:45">
       <c r="A20" t="s">
@@ -3662,7 +3784,7 @@
         <v>138</v>
       </c>
       <c r="C20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
@@ -3704,7 +3826,7 @@
         <v>20</v>
       </c>
       <c r="S20">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T20">
         <v>5</v>
@@ -3789,7 +3911,7 @@
         <v>196</v>
       </c>
       <c r="C21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" t="b">
         <v>0</v>
@@ -3831,7 +3953,7 @@
         <v>20</v>
       </c>
       <c r="S21">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T21">
         <v>5</v>
@@ -3916,7 +4038,7 @@
         <v>136</v>
       </c>
       <c r="C23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" t="b">
         <v>0</v>
@@ -3958,7 +4080,7 @@
         <v>20</v>
       </c>
       <c r="S23">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T23">
         <v>5</v>
@@ -4041,7 +4163,7 @@
         <v>168</v>
       </c>
       <c r="C24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" t="b">
         <v>0</v>
@@ -4083,7 +4205,7 @@
         <v>20</v>
       </c>
       <c r="S24">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T24">
         <v>5</v>
@@ -4166,7 +4288,7 @@
         <v>145</v>
       </c>
       <c r="C26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
@@ -4208,7 +4330,7 @@
         <v>20</v>
       </c>
       <c r="S26">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T26">
         <v>5</v>
@@ -4291,7 +4413,7 @@
         <v>146</v>
       </c>
       <c r="C27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" t="b">
         <v>0</v>
@@ -4333,7 +4455,7 @@
         <v>20</v>
       </c>
       <c r="S27">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T27">
         <v>5</v>
@@ -4421,7 +4543,7 @@
         <v>235</v>
       </c>
       <c r="C32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" t="b">
         <v>0</v>
@@ -4463,7 +4585,7 @@
         <v>20</v>
       </c>
       <c r="S32">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T32">
         <v>5</v>
@@ -4567,7 +4689,7 @@
         <v>138</v>
       </c>
       <c r="C35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35" t="b">
         <v>0</v>
@@ -4609,7 +4731,7 @@
         <v>20</v>
       </c>
       <c r="S35">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T35">
         <v>5</v>
@@ -4694,7 +4816,7 @@
         <v>196</v>
       </c>
       <c r="C36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D36" t="b">
         <v>0</v>
@@ -4736,7 +4858,7 @@
         <v>20</v>
       </c>
       <c r="S36">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T36">
         <v>5</v>
@@ -4825,7 +4947,7 @@
         <v>136</v>
       </c>
       <c r="C38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" t="b">
         <v>0</v>
@@ -4867,7 +4989,7 @@
         <v>20</v>
       </c>
       <c r="S38">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T38">
         <v>5</v>
@@ -4950,7 +5072,7 @@
         <v>168</v>
       </c>
       <c r="C39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D39" t="b">
         <v>0</v>
@@ -4992,7 +5114,7 @@
         <v>20</v>
       </c>
       <c r="S39">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T39">
         <v>5</v>
@@ -5075,7 +5197,7 @@
         <v>145</v>
       </c>
       <c r="C41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41" t="b">
         <v>0</v>
@@ -5117,7 +5239,7 @@
         <v>20</v>
       </c>
       <c r="S41">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T41">
         <v>5</v>
@@ -5200,7 +5322,7 @@
         <v>146</v>
       </c>
       <c r="C42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D42" t="b">
         <v>0</v>
@@ -5242,7 +5364,7 @@
         <v>20</v>
       </c>
       <c r="S42">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T42">
         <v>5</v>
@@ -5330,6 +5452,9 @@
       <c r="B44" s="56" t="s">
         <v>237</v>
       </c>
+      <c r="C44" t="b">
+        <v>0</v>
+      </c>
       <c r="AC44" s="3"/>
       <c r="AD44" s="5"/>
       <c r="AE44" s="38"/>
@@ -5346,7 +5471,7 @@
         <v>138</v>
       </c>
       <c r="C45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D45" t="b">
         <v>0</v>
@@ -5388,7 +5513,7 @@
         <v>20</v>
       </c>
       <c r="S45">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T45">
         <v>5</v>
@@ -5473,7 +5598,7 @@
         <v>196</v>
       </c>
       <c r="C46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46" t="b">
         <v>0</v>
@@ -5515,7 +5640,7 @@
         <v>20</v>
       </c>
       <c r="S46">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T46">
         <v>5</v>
@@ -5604,7 +5729,7 @@
         <v>136</v>
       </c>
       <c r="C48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48" t="b">
         <v>0</v>
@@ -5646,7 +5771,7 @@
         <v>20</v>
       </c>
       <c r="S48">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T48">
         <v>5</v>
@@ -5729,7 +5854,7 @@
         <v>168</v>
       </c>
       <c r="C49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D49" t="b">
         <v>0</v>
@@ -5771,7 +5896,7 @@
         <v>20</v>
       </c>
       <c r="S49">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T49">
         <v>5</v>
@@ -5854,7 +5979,7 @@
         <v>145</v>
       </c>
       <c r="C51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D51" t="b">
         <v>0</v>
@@ -5896,7 +6021,7 @@
         <v>20</v>
       </c>
       <c r="S51">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T51">
         <v>5</v>
@@ -5979,7 +6104,7 @@
         <v>146</v>
       </c>
       <c r="C52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D52" t="b">
         <v>0</v>
@@ -6021,7 +6146,7 @@
         <v>20</v>
       </c>
       <c r="S52">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T52">
         <v>5</v>
@@ -6118,7 +6243,7 @@
         <v>136</v>
       </c>
       <c r="C56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D56" t="b">
         <v>0</v>
@@ -6166,7 +6291,7 @@
         <v>20</v>
       </c>
       <c r="S56">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T56">
         <v>5</v>
@@ -6249,7 +6374,7 @@
         <v>168</v>
       </c>
       <c r="C57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D57" t="b">
         <v>0</v>
@@ -6297,7 +6422,7 @@
         <v>20</v>
       </c>
       <c r="S57">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T57">
         <v>5</v>
@@ -6389,7 +6514,7 @@
         <v>136</v>
       </c>
       <c r="C59" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D59" t="b">
         <v>0</v>
@@ -6437,7 +6562,7 @@
         <v>20</v>
       </c>
       <c r="S59">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T59">
         <v>5</v>
@@ -6520,7 +6645,7 @@
         <v>168</v>
       </c>
       <c r="C60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D60" t="b">
         <v>0</v>
@@ -6568,7 +6693,7 @@
         <v>20</v>
       </c>
       <c r="S60">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T60">
         <v>5</v>
@@ -6660,7 +6785,7 @@
         <v>136</v>
       </c>
       <c r="C62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D62" t="b">
         <v>0</v>
@@ -6708,7 +6833,7 @@
         <v>20</v>
       </c>
       <c r="S62">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T62">
         <v>5</v>
@@ -6791,7 +6916,7 @@
         <v>168</v>
       </c>
       <c r="C63" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D63" t="b">
         <v>0</v>
@@ -6839,7 +6964,7 @@
         <v>20</v>
       </c>
       <c r="S63">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T63">
         <v>5</v>
@@ -6931,7 +7056,7 @@
         <v>136</v>
       </c>
       <c r="C65" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D65" t="b">
         <v>0</v>
@@ -6979,7 +7104,7 @@
         <v>20</v>
       </c>
       <c r="S65">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T65">
         <v>5</v>
@@ -7062,7 +7187,7 @@
         <v>168</v>
       </c>
       <c r="C66" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D66" t="b">
         <v>0</v>
@@ -7110,7 +7235,7 @@
         <v>20</v>
       </c>
       <c r="S66">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T66">
         <v>5</v>
@@ -7214,15 +7339,15 @@
     </row>
     <row r="70" spans="1:45">
       <c r="B70" s="56" t="s">
-        <v>226</v>
+        <v>423</v>
       </c>
     </row>
     <row r="71" spans="1:45">
       <c r="A71" t="s">
-        <v>144</v>
+        <v>424</v>
       </c>
       <c r="B71" t="s">
-        <v>137</v>
+        <v>425</v>
       </c>
       <c r="C71" t="b">
         <v>0</v>
@@ -7231,22 +7356,25 @@
         <v>0</v>
       </c>
       <c r="E71" t="s">
-        <v>142</v>
+        <v>402</v>
       </c>
       <c r="F71" t="b">
         <v>0</v>
       </c>
       <c r="G71" t="s">
-        <v>139</v>
+        <v>424</v>
       </c>
       <c r="H71" t="b">
         <v>0</v>
       </c>
+      <c r="I71" t="b">
+        <v>0</v>
+      </c>
       <c r="J71" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K71" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L71">
         <v>0.02</v>
@@ -7255,7 +7383,7 @@
         <v>0</v>
       </c>
       <c r="P71" t="s">
-        <v>36</v>
+        <v>338</v>
       </c>
       <c r="Q71" t="s">
         <v>35</v>
@@ -7264,7 +7392,7 @@
         <v>20</v>
       </c>
       <c r="S71">
-        <v>2.75E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="T71">
         <v>5</v>
@@ -7309,10 +7437,10 @@
         <v>31</v>
       </c>
       <c r="AH71" s="23">
-        <v>0.6976</v>
+        <v>0.68300000000000005</v>
       </c>
       <c r="AI71" s="23">
-        <v>0.6976</v>
+        <v>0.68300000000000005</v>
       </c>
       <c r="AL71" s="43">
         <v>0.1</v>
@@ -7340,137 +7468,1573 @@
       </c>
     </row>
     <row r="72" spans="1:45">
-      <c r="A72" t="s">
-        <v>268</v>
-      </c>
-      <c r="B72" t="s">
+      <c r="AC72" s="3"/>
+      <c r="AD72" s="5"/>
+      <c r="AE72" s="38"/>
+      <c r="AH72" s="23"/>
+      <c r="AI72" s="23"/>
+      <c r="AL72" s="43"/>
+      <c r="AS72" s="22"/>
+    </row>
+    <row r="73" spans="1:45">
+      <c r="B73" s="56" t="s">
+        <v>238</v>
+      </c>
+      <c r="AC73" s="3"/>
+      <c r="AD73" s="5"/>
+      <c r="AE73" s="38"/>
+      <c r="AH73" s="23"/>
+      <c r="AI73" s="23"/>
+      <c r="AL73" s="43"/>
+      <c r="AS73" s="22"/>
+    </row>
+    <row r="74" spans="1:45">
+      <c r="A74" t="s">
+        <v>426</v>
+      </c>
+      <c r="B74" t="s">
+        <v>138</v>
+      </c>
+      <c r="C74" t="b">
+        <v>0</v>
+      </c>
+      <c r="D74" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" t="s">
+        <v>406</v>
+      </c>
+      <c r="F74" t="b">
+        <v>0</v>
+      </c>
+      <c r="G74" t="s">
+        <v>424</v>
+      </c>
+      <c r="H74" t="b">
+        <v>1</v>
+      </c>
+      <c r="I74" t="b">
+        <v>1</v>
+      </c>
+      <c r="J74" t="b">
+        <v>1</v>
+      </c>
+      <c r="K74" t="b">
+        <v>0</v>
+      </c>
+      <c r="L74">
+        <v>0.02</v>
+      </c>
+      <c r="M74">
+        <v>0</v>
+      </c>
+      <c r="P74" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>35</v>
+      </c>
+      <c r="R74">
+        <v>20</v>
+      </c>
+      <c r="S74">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="T74">
+        <v>5</v>
+      </c>
+      <c r="U74">
+        <v>999</v>
+      </c>
+      <c r="V74">
+        <v>0</v>
+      </c>
+      <c r="W74" t="s">
+        <v>339</v>
+      </c>
+      <c r="X74" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y74" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z74" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA74">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB74">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="AC74" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="AD74" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AE74" s="38">
+        <v>123</v>
+      </c>
+      <c r="AF74" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG74" t="s">
+        <v>131</v>
+      </c>
+      <c r="AH74" s="23"/>
+      <c r="AI74" s="23"/>
+      <c r="AJ74" s="44">
+        <v>81825573157</v>
+      </c>
+      <c r="AK74" s="44">
+        <v>81825573157</v>
+      </c>
+      <c r="AL74" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="AM74" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN74" t="b">
+        <v>1</v>
+      </c>
+      <c r="AO74" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP74">
+        <v>0</v>
+      </c>
+      <c r="AQ74" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR74" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS74" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:45">
+      <c r="A75" t="s">
+        <v>427</v>
+      </c>
+      <c r="B75" t="s">
+        <v>196</v>
+      </c>
+      <c r="C75" t="b">
+        <v>0</v>
+      </c>
+      <c r="D75" t="b">
+        <v>0</v>
+      </c>
+      <c r="E75" t="s">
+        <v>406</v>
+      </c>
+      <c r="F75" t="b">
+        <v>0</v>
+      </c>
+      <c r="G75" t="s">
+        <v>424</v>
+      </c>
+      <c r="H75" t="b">
+        <v>1</v>
+      </c>
+      <c r="I75" t="b">
+        <v>0</v>
+      </c>
+      <c r="J75" t="b">
+        <v>1</v>
+      </c>
+      <c r="K75" t="b">
+        <v>0</v>
+      </c>
+      <c r="L75">
+        <v>0.02</v>
+      </c>
+      <c r="M75">
+        <v>0</v>
+      </c>
+      <c r="P75" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>35</v>
+      </c>
+      <c r="R75">
+        <v>20</v>
+      </c>
+      <c r="S75">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="T75">
+        <v>5</v>
+      </c>
+      <c r="U75">
+        <v>999</v>
+      </c>
+      <c r="V75">
+        <v>0</v>
+      </c>
+      <c r="W75" t="s">
+        <v>339</v>
+      </c>
+      <c r="X75" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y75" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z75" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA75">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB75">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="AC75" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="AD75" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AE75" s="38">
+        <v>123</v>
+      </c>
+      <c r="AF75" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG75" t="s">
+        <v>131</v>
+      </c>
+      <c r="AH75" s="23"/>
+      <c r="AI75" s="23"/>
+      <c r="AJ75" s="44">
+        <v>81825573157</v>
+      </c>
+      <c r="AK75" s="44">
+        <v>81825573157</v>
+      </c>
+      <c r="AL75" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="AM75" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN75" t="b">
+        <v>1</v>
+      </c>
+      <c r="AO75" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP75">
+        <v>0</v>
+      </c>
+      <c r="AQ75" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR75" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS75" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:45">
+      <c r="AH76" s="23"/>
+      <c r="AI76" s="23"/>
+    </row>
+    <row r="77" spans="1:45">
+      <c r="A77" t="s">
+        <v>428</v>
+      </c>
+      <c r="B77" t="s">
+        <v>136</v>
+      </c>
+      <c r="C77" t="b">
+        <v>0</v>
+      </c>
+      <c r="D77" t="b">
+        <v>0</v>
+      </c>
+      <c r="E77" t="s">
+        <v>408</v>
+      </c>
+      <c r="F77" t="b">
+        <v>0</v>
+      </c>
+      <c r="G77" t="s">
+        <v>424</v>
+      </c>
+      <c r="H77" t="b">
+        <v>1</v>
+      </c>
+      <c r="I77" t="b">
+        <v>1</v>
+      </c>
+      <c r="J77" t="b">
+        <v>1</v>
+      </c>
+      <c r="K77" t="b">
+        <v>1</v>
+      </c>
+      <c r="L77">
+        <v>0.02</v>
+      </c>
+      <c r="M77">
+        <v>0</v>
+      </c>
+      <c r="P77" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>35</v>
+      </c>
+      <c r="R77">
+        <v>20</v>
+      </c>
+      <c r="S77">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="T77">
+        <v>5</v>
+      </c>
+      <c r="U77">
+        <v>999</v>
+      </c>
+      <c r="V77">
+        <v>0</v>
+      </c>
+      <c r="W77" t="s">
+        <v>339</v>
+      </c>
+      <c r="X77" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y77" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z77" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA77">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB77">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="AC77" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="AD77" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AE77" s="38">
+        <v>123</v>
+      </c>
+      <c r="AF77" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG77" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH77" s="23">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="AI77" s="23">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="AL77" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="AM77" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN77" t="b">
+        <v>1</v>
+      </c>
+      <c r="AO77" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP77">
+        <v>0</v>
+      </c>
+      <c r="AQ77" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR77" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS77" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:45">
+      <c r="A78" t="s">
+        <v>429</v>
+      </c>
+      <c r="B78" t="s">
+        <v>168</v>
+      </c>
+      <c r="C78" t="b">
+        <v>0</v>
+      </c>
+      <c r="D78" t="b">
+        <v>0</v>
+      </c>
+      <c r="E78" t="s">
+        <v>408</v>
+      </c>
+      <c r="F78" t="b">
+        <v>0</v>
+      </c>
+      <c r="G78" t="s">
+        <v>424</v>
+      </c>
+      <c r="H78" t="b">
+        <v>1</v>
+      </c>
+      <c r="I78" t="b">
+        <v>0</v>
+      </c>
+      <c r="J78" t="b">
+        <v>1</v>
+      </c>
+      <c r="K78" t="b">
+        <v>1</v>
+      </c>
+      <c r="L78">
+        <v>0.02</v>
+      </c>
+      <c r="M78">
+        <v>0</v>
+      </c>
+      <c r="P78" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>35</v>
+      </c>
+      <c r="R78">
+        <v>20</v>
+      </c>
+      <c r="S78">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="T78">
+        <v>5</v>
+      </c>
+      <c r="U78">
+        <v>999</v>
+      </c>
+      <c r="V78">
+        <v>0</v>
+      </c>
+      <c r="W78" t="s">
+        <v>339</v>
+      </c>
+      <c r="X78" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y78" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z78" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA78">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB78">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="AC78" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="AD78" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AE78" s="38">
+        <v>123</v>
+      </c>
+      <c r="AF78" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG78" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH78" s="23">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="AI78" s="23">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="AL78" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="AM78" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN78" t="b">
+        <v>1</v>
+      </c>
+      <c r="AO78" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP78">
+        <v>0</v>
+      </c>
+      <c r="AQ78" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR78" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS78" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:45">
+      <c r="A80" t="s">
+        <v>430</v>
+      </c>
+      <c r="B80" t="s">
+        <v>145</v>
+      </c>
+      <c r="C80" t="b">
+        <v>0</v>
+      </c>
+      <c r="D80" t="b">
+        <v>0</v>
+      </c>
+      <c r="E80" t="s">
+        <v>412</v>
+      </c>
+      <c r="F80" t="b">
+        <v>0</v>
+      </c>
+      <c r="G80" t="s">
+        <v>424</v>
+      </c>
+      <c r="H80" t="b">
+        <v>1</v>
+      </c>
+      <c r="I80" t="b">
+        <v>1</v>
+      </c>
+      <c r="J80" t="b">
+        <v>1</v>
+      </c>
+      <c r="K80" t="b">
+        <v>1</v>
+      </c>
+      <c r="L80">
+        <v>0.02</v>
+      </c>
+      <c r="M80">
+        <v>0</v>
+      </c>
+      <c r="P80" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>35</v>
+      </c>
+      <c r="R80">
+        <v>20</v>
+      </c>
+      <c r="S80">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="T80">
+        <v>5</v>
+      </c>
+      <c r="U80">
+        <v>999</v>
+      </c>
+      <c r="V80">
+        <v>0</v>
+      </c>
+      <c r="W80" t="s">
+        <v>339</v>
+      </c>
+      <c r="X80" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y80" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z80" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA80">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB80">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="AC80" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="AD80" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AE80" s="38">
+        <v>123</v>
+      </c>
+      <c r="AF80" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG80" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH80" s="23">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="AI80" s="23">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="AL80" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="AM80" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN80" t="b">
+        <v>1</v>
+      </c>
+      <c r="AO80" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP80">
+        <v>0</v>
+      </c>
+      <c r="AQ80" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR80" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS80" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:45">
+      <c r="A81" t="s">
+        <v>431</v>
+      </c>
+      <c r="B81" t="s">
         <v>146</v>
       </c>
-      <c r="C72" t="b">
-        <v>0</v>
-      </c>
-      <c r="D72" t="b">
-        <v>0</v>
-      </c>
-      <c r="E72" t="s">
-        <v>143</v>
-      </c>
-      <c r="F72" t="b">
-        <v>0</v>
-      </c>
-      <c r="G72" t="s">
-        <v>139</v>
-      </c>
-      <c r="H72" t="b">
-        <v>1</v>
-      </c>
-      <c r="J72" t="b">
-        <v>1</v>
-      </c>
-      <c r="K72" t="b">
-        <v>1</v>
-      </c>
-      <c r="L72">
+      <c r="C81" t="b">
+        <v>0</v>
+      </c>
+      <c r="D81" t="b">
+        <v>0</v>
+      </c>
+      <c r="E81" t="s">
+        <v>412</v>
+      </c>
+      <c r="F81" t="b">
+        <v>0</v>
+      </c>
+      <c r="G81" t="s">
+        <v>424</v>
+      </c>
+      <c r="H81" t="b">
+        <v>1</v>
+      </c>
+      <c r="I81" t="b">
+        <v>0</v>
+      </c>
+      <c r="J81" t="b">
+        <v>1</v>
+      </c>
+      <c r="K81" t="b">
+        <v>1</v>
+      </c>
+      <c r="L81">
         <v>0.02</v>
       </c>
-      <c r="M72">
-        <v>0</v>
-      </c>
-      <c r="P72" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q72" t="s">
+      <c r="M81">
+        <v>0</v>
+      </c>
+      <c r="P81" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q81" t="s">
         <v>35</v>
       </c>
-      <c r="R72">
+      <c r="R81">
         <v>20</v>
       </c>
-      <c r="S72">
-        <v>2.75E-2</v>
-      </c>
-      <c r="T72">
+      <c r="S81">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="T81">
         <v>5</v>
       </c>
-      <c r="U72">
+      <c r="U81">
         <v>999</v>
       </c>
-      <c r="V72">
-        <v>0</v>
-      </c>
-      <c r="W72" t="s">
+      <c r="V81">
+        <v>0</v>
+      </c>
+      <c r="W81" t="s">
         <v>339</v>
       </c>
-      <c r="X72" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y72" t="s">
+      <c r="X81" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y81" t="s">
         <v>119</v>
       </c>
-      <c r="Z72" t="s">
+      <c r="Z81" t="s">
         <v>20</v>
       </c>
-      <c r="AA72">
+      <c r="AA81">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AB72">
+      <c r="AB81">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AC72" s="3">
+      <c r="AC81" s="3">
         <v>0.12</v>
       </c>
-      <c r="AD72" s="5">
+      <c r="AD81" s="5">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AE72" s="38">
+      <c r="AE81" s="38">
         <v>123</v>
       </c>
-      <c r="AF72" t="s">
+      <c r="AF81" t="s">
         <v>31</v>
       </c>
-      <c r="AG72" t="s">
+      <c r="AG81" t="s">
         <v>31</v>
       </c>
-      <c r="AH72" s="23">
-        <v>0.6976</v>
-      </c>
-      <c r="AI72" s="23">
-        <v>0.6976</v>
-      </c>
-      <c r="AL72" s="43">
+      <c r="AH81" s="23">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="AI81" s="23">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="AL81" s="43">
         <v>0.1</v>
       </c>
-      <c r="AM72" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN72" t="b">
-        <v>1</v>
-      </c>
-      <c r="AO72" t="b">
-        <v>0</v>
-      </c>
-      <c r="AP72">
-        <v>0</v>
-      </c>
-      <c r="AQ72" t="s">
+      <c r="AM81" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN81" t="b">
+        <v>1</v>
+      </c>
+      <c r="AO81" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP81">
+        <v>0</v>
+      </c>
+      <c r="AQ81" t="s">
         <v>3</v>
       </c>
-      <c r="AR72" t="b">
-        <v>1</v>
-      </c>
-      <c r="AS72" s="22" t="b">
+      <c r="AR81" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS81" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:45">
+      <c r="AC82" s="3"/>
+      <c r="AD82" s="5"/>
+      <c r="AE82" s="38"/>
+      <c r="AH82" s="23"/>
+      <c r="AI82" s="23"/>
+      <c r="AL82" s="43"/>
+      <c r="AS82" s="22"/>
+    </row>
+    <row r="83" spans="1:45">
+      <c r="B83" s="56" t="s">
+        <v>237</v>
+      </c>
+      <c r="AC83" s="3"/>
+      <c r="AD83" s="5"/>
+      <c r="AE83" s="38"/>
+      <c r="AH83" s="23"/>
+      <c r="AI83" s="23"/>
+      <c r="AL83" s="43"/>
+      <c r="AS83" s="22"/>
+    </row>
+    <row r="84" spans="1:45">
+      <c r="A84" t="s">
+        <v>432</v>
+      </c>
+      <c r="B84" t="s">
+        <v>138</v>
+      </c>
+      <c r="C84" t="b">
+        <v>0</v>
+      </c>
+      <c r="D84" t="b">
+        <v>0</v>
+      </c>
+      <c r="E84" t="s">
+        <v>404</v>
+      </c>
+      <c r="F84" t="b">
+        <v>0</v>
+      </c>
+      <c r="G84" t="s">
+        <v>424</v>
+      </c>
+      <c r="H84" t="b">
+        <v>1</v>
+      </c>
+      <c r="I84" t="b">
+        <v>1</v>
+      </c>
+      <c r="J84" t="b">
+        <v>1</v>
+      </c>
+      <c r="K84" t="b">
+        <v>0</v>
+      </c>
+      <c r="L84">
+        <v>0.02</v>
+      </c>
+      <c r="M84">
+        <v>0</v>
+      </c>
+      <c r="P84" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>35</v>
+      </c>
+      <c r="R84">
+        <v>20</v>
+      </c>
+      <c r="S84">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="T84">
+        <v>5</v>
+      </c>
+      <c r="U84">
+        <v>999</v>
+      </c>
+      <c r="V84">
+        <v>0</v>
+      </c>
+      <c r="W84" t="s">
+        <v>339</v>
+      </c>
+      <c r="X84" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y84" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z84" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA84">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB84">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="AC84" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="AD84" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AE84" s="38">
+        <v>123</v>
+      </c>
+      <c r="AF84" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG84" t="s">
+        <v>131</v>
+      </c>
+      <c r="AH84" s="23"/>
+      <c r="AI84" s="23"/>
+      <c r="AJ84" s="44">
+        <v>81825573157</v>
+      </c>
+      <c r="AK84" s="44">
+        <v>81825573157</v>
+      </c>
+      <c r="AL84" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="AM84" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN84" t="b">
+        <v>1</v>
+      </c>
+      <c r="AO84" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP84">
+        <v>0</v>
+      </c>
+      <c r="AQ84" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR84" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS84" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:45">
+      <c r="A85" t="s">
+        <v>433</v>
+      </c>
+      <c r="B85" t="s">
+        <v>196</v>
+      </c>
+      <c r="C85" t="b">
+        <v>0</v>
+      </c>
+      <c r="D85" t="b">
+        <v>0</v>
+      </c>
+      <c r="E85" t="s">
+        <v>404</v>
+      </c>
+      <c r="F85" t="b">
+        <v>0</v>
+      </c>
+      <c r="G85" t="s">
+        <v>424</v>
+      </c>
+      <c r="H85" t="b">
+        <v>1</v>
+      </c>
+      <c r="I85" t="b">
+        <v>0</v>
+      </c>
+      <c r="J85" t="b">
+        <v>1</v>
+      </c>
+      <c r="K85" t="b">
+        <v>0</v>
+      </c>
+      <c r="L85">
+        <v>0.02</v>
+      </c>
+      <c r="M85">
+        <v>0</v>
+      </c>
+      <c r="P85" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>35</v>
+      </c>
+      <c r="R85">
+        <v>20</v>
+      </c>
+      <c r="S85">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="T85">
+        <v>5</v>
+      </c>
+      <c r="U85">
+        <v>999</v>
+      </c>
+      <c r="V85">
+        <v>0</v>
+      </c>
+      <c r="W85" t="s">
+        <v>339</v>
+      </c>
+      <c r="X85" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y85" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z85" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA85">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB85">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="AC85" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="AD85" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AE85" s="38">
+        <v>123</v>
+      </c>
+      <c r="AF85" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG85" t="s">
+        <v>131</v>
+      </c>
+      <c r="AH85" s="23"/>
+      <c r="AI85" s="23"/>
+      <c r="AJ85" s="44">
+        <v>81825573157</v>
+      </c>
+      <c r="AK85" s="44">
+        <v>81825573157</v>
+      </c>
+      <c r="AL85" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="AM85" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN85" t="b">
+        <v>1</v>
+      </c>
+      <c r="AO85" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP85">
+        <v>0</v>
+      </c>
+      <c r="AQ85" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR85" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS85" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:45">
+      <c r="AH86" s="23"/>
+      <c r="AI86" s="23"/>
+    </row>
+    <row r="87" spans="1:45">
+      <c r="A87" t="s">
+        <v>434</v>
+      </c>
+      <c r="B87" t="s">
+        <v>136</v>
+      </c>
+      <c r="C87" t="b">
+        <v>0</v>
+      </c>
+      <c r="D87" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" t="s">
+        <v>414</v>
+      </c>
+      <c r="F87" t="b">
+        <v>0</v>
+      </c>
+      <c r="G87" t="s">
+        <v>424</v>
+      </c>
+      <c r="H87" t="b">
+        <v>1</v>
+      </c>
+      <c r="I87" t="b">
+        <v>1</v>
+      </c>
+      <c r="J87" t="b">
+        <v>1</v>
+      </c>
+      <c r="K87" t="b">
+        <v>1</v>
+      </c>
+      <c r="L87">
+        <v>0.02</v>
+      </c>
+      <c r="M87">
+        <v>0.01</v>
+      </c>
+      <c r="P87" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q87" t="s">
+        <v>35</v>
+      </c>
+      <c r="R87">
+        <v>20</v>
+      </c>
+      <c r="S87">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="T87">
+        <v>5</v>
+      </c>
+      <c r="U87">
+        <v>999</v>
+      </c>
+      <c r="V87">
+        <v>0</v>
+      </c>
+      <c r="W87" t="s">
+        <v>339</v>
+      </c>
+      <c r="X87" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y87" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z87" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA87">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB87">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="AC87" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="AD87" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AE87" s="38">
+        <v>123</v>
+      </c>
+      <c r="AF87" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG87" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH87" s="23">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="AI87" s="23">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="AL87" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="AM87" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN87" t="b">
+        <v>1</v>
+      </c>
+      <c r="AO87" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP87">
+        <v>0</v>
+      </c>
+      <c r="AQ87" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR87" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS87" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:45">
+      <c r="A88" t="s">
+        <v>435</v>
+      </c>
+      <c r="B88" t="s">
+        <v>168</v>
+      </c>
+      <c r="C88" t="b">
+        <v>0</v>
+      </c>
+      <c r="D88" t="b">
+        <v>0</v>
+      </c>
+      <c r="E88" t="s">
+        <v>414</v>
+      </c>
+      <c r="F88" t="b">
+        <v>0</v>
+      </c>
+      <c r="G88" t="s">
+        <v>424</v>
+      </c>
+      <c r="H88" t="b">
+        <v>1</v>
+      </c>
+      <c r="I88" t="b">
+        <v>0</v>
+      </c>
+      <c r="J88" t="b">
+        <v>1</v>
+      </c>
+      <c r="K88" t="b">
+        <v>1</v>
+      </c>
+      <c r="L88">
+        <v>0.02</v>
+      </c>
+      <c r="M88">
+        <v>0.01</v>
+      </c>
+      <c r="P88" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>35</v>
+      </c>
+      <c r="R88">
+        <v>20</v>
+      </c>
+      <c r="S88">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="T88">
+        <v>5</v>
+      </c>
+      <c r="U88">
+        <v>999</v>
+      </c>
+      <c r="V88">
+        <v>0</v>
+      </c>
+      <c r="W88" t="s">
+        <v>339</v>
+      </c>
+      <c r="X88" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y88" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z88" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA88">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB88">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="AC88" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="AD88" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AE88" s="38">
+        <v>123</v>
+      </c>
+      <c r="AF88" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG88" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH88" s="23">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="AI88" s="23">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="AL88" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="AM88" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN88" t="b">
+        <v>1</v>
+      </c>
+      <c r="AO88" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP88">
+        <v>0</v>
+      </c>
+      <c r="AQ88" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR88" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS88" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:45">
+      <c r="A90" t="s">
+        <v>436</v>
+      </c>
+      <c r="B90" t="s">
+        <v>145</v>
+      </c>
+      <c r="C90" t="b">
+        <v>0</v>
+      </c>
+      <c r="D90" t="b">
+        <v>0</v>
+      </c>
+      <c r="E90" t="s">
+        <v>416</v>
+      </c>
+      <c r="F90" t="b">
+        <v>0</v>
+      </c>
+      <c r="G90" t="s">
+        <v>424</v>
+      </c>
+      <c r="H90" t="b">
+        <v>1</v>
+      </c>
+      <c r="I90" t="b">
+        <v>1</v>
+      </c>
+      <c r="J90" t="b">
+        <v>1</v>
+      </c>
+      <c r="K90" t="b">
+        <v>1</v>
+      </c>
+      <c r="L90">
+        <v>0.02</v>
+      </c>
+      <c r="M90">
+        <v>0.01</v>
+      </c>
+      <c r="P90" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>35</v>
+      </c>
+      <c r="R90">
+        <v>20</v>
+      </c>
+      <c r="S90">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="T90">
+        <v>5</v>
+      </c>
+      <c r="U90">
+        <v>999</v>
+      </c>
+      <c r="V90">
+        <v>0</v>
+      </c>
+      <c r="W90" t="s">
+        <v>339</v>
+      </c>
+      <c r="X90" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y90" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z90" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA90">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB90">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="AC90" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="AD90" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AE90" s="38">
+        <v>123</v>
+      </c>
+      <c r="AF90" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG90" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH90" s="23">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="AI90" s="23">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="AL90" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="AM90" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN90" t="b">
+        <v>1</v>
+      </c>
+      <c r="AO90" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP90">
+        <v>0</v>
+      </c>
+      <c r="AQ90" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR90" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS90" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:45">
+      <c r="A91" t="s">
+        <v>437</v>
+      </c>
+      <c r="B91" t="s">
+        <v>146</v>
+      </c>
+      <c r="C91" t="b">
+        <v>0</v>
+      </c>
+      <c r="D91" t="b">
+        <v>0</v>
+      </c>
+      <c r="E91" t="s">
+        <v>416</v>
+      </c>
+      <c r="F91" t="b">
+        <v>0</v>
+      </c>
+      <c r="G91" t="s">
+        <v>424</v>
+      </c>
+      <c r="H91" t="b">
+        <v>1</v>
+      </c>
+      <c r="I91" t="b">
+        <v>0</v>
+      </c>
+      <c r="J91" t="b">
+        <v>1</v>
+      </c>
+      <c r="K91" t="b">
+        <v>1</v>
+      </c>
+      <c r="L91">
+        <v>0.02</v>
+      </c>
+      <c r="M91">
+        <v>0.01</v>
+      </c>
+      <c r="P91" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>35</v>
+      </c>
+      <c r="R91">
+        <v>20</v>
+      </c>
+      <c r="S91">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="T91">
+        <v>5</v>
+      </c>
+      <c r="U91">
+        <v>999</v>
+      </c>
+      <c r="V91">
+        <v>0</v>
+      </c>
+      <c r="W91" t="s">
+        <v>339</v>
+      </c>
+      <c r="X91" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y91" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z91" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA91">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AB91">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="AC91" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="AD91" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AE91" s="38">
+        <v>123</v>
+      </c>
+      <c r="AF91" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG91" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH91" s="23">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="AI91" s="23">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="AL91" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="AM91" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN91" t="b">
+        <v>1</v>
+      </c>
+      <c r="AO91" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP91">
+        <v>0</v>
+      </c>
+      <c r="AQ91" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR91" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS91" s="22" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN5:AO6 C5:C6 AN48:AO49 AN51:AO53 AN13:AO14 AN41:AO46 AN16:AO18 AN71:AO72 C71:C72 AN20:AO21 AN23:AO24 AN38:AO39 AN26:AO27 C32:C33 AN32:AO36 AN8:AO11 C35:C53 C8:C27 AN56:AO69 C56:C69" xr:uid="{1240F49A-5091-456D-B77A-0673AD56E758}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN5:AO6 C5:C6 AN48:AO49 AN51:AO53 AN13:AO14 AN41:AO46 AN16:AO18 AN20:AO21 AN23:AO24 AN38:AO39 AN26:AO27 C32:C33 AN32:AO36 AN8:AO11 C8:C27 C56:C69 AN56:AO69 C35:C53 AN87:AO88 AN90:AO91 AN80:AO85 AN77:AO78 C71:C72 AN71:AO75 C74:C91" xr:uid="{1240F49A-5091-456D-B77A-0673AD56E758}">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y5:Y6 Y48:Y49 Y26:Y27 Y51:Y53 Y13:Y14 Y16:Y18 Y71:Y72 Y20:Y21 Y23:Y24 Y32:Y36 Y41:Y46 Y38:Y39 Y8:Y11 Y56:Y69" xr:uid="{8909875A-86FC-4594-BBAF-A364A5851F3C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y5:Y6 Y48:Y49 Y26:Y27 Y51:Y53 Y13:Y14 Y16:Y18 Y20:Y21 Y23:Y24 Y32:Y36 Y41:Y46 Y38:Y39 Y8:Y11 Y56:Y69 Y87:Y88 Y90:Y91 Y71:Y75 Y80:Y85 Y77:Y78" xr:uid="{8909875A-86FC-4594-BBAF-A364A5851F3C}">
       <formula1>"simple, internal"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D6 D48:D49 D26:D27 D51:D53 D13:D14 D16:D18 D71:D72 D20:D21 D23:D24 D32:D36 D41:D46 D38:D39 D8:D11 D56:D69" xr:uid="{EC327A6A-3FD9-4228-86E6-BF4DFCBDFAEB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D6 D48:D49 D26:D27 D51:D53 D13:D14 D16:D18 D20:D21 D23:D24 D32:D36 D41:D46 D38:D39 D8:D11 D56:D69 D87:D88 D90:D91 D71:D75 D80:D85 D77:D78" xr:uid="{EC327A6A-3FD9-4228-86E6-BF4DFCBDFAEB}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7875,7 +9439,7 @@
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7939,19 +9503,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19F07677-8B44-417E-B263-203C3A91094A}">
-  <dimension ref="A3:R76"/>
+  <dimension ref="A3:R92"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D41" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="D34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E67" sqref="E67"/>
+      <selection pane="bottomRight" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="56.28515625" customWidth="1"/>
+    <col min="2" max="2" width="53.140625" customWidth="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
     <col min="5" max="5" width="29.140625" customWidth="1"/>
@@ -9339,7 +10903,7 @@
         <v>316</v>
       </c>
       <c r="C42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42" t="s">
         <v>70</v>
@@ -9899,7 +11463,7 @@
     <row r="56" spans="1:18">
       <c r="A56" s="59"/>
     </row>
-    <row r="57" spans="1:18">
+    <row r="57" spans="1:18" ht="13.5" customHeight="1">
       <c r="A57" s="59" t="s">
         <v>353</v>
       </c>
@@ -9907,7 +11471,7 @@
         <v>354</v>
       </c>
       <c r="C57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D57" t="s">
         <v>70</v>
@@ -9940,10 +11504,10 @@
         <v>1</v>
       </c>
       <c r="O57" s="43">
-        <v>0.11</v>
+        <v>0.04</v>
       </c>
       <c r="P57">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="Q57">
         <v>0.05</v>
@@ -9993,10 +11557,10 @@
         <v>1</v>
       </c>
       <c r="O58" s="43">
-        <v>0.11</v>
+        <v>0.04</v>
       </c>
       <c r="P58">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="Q58">
         <v>0.05</v>
@@ -10046,10 +11610,10 @@
         <v>1</v>
       </c>
       <c r="O59" s="43">
-        <v>0.11</v>
+        <v>0.04</v>
       </c>
       <c r="P59">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="Q59">
         <v>0.05</v>
@@ -10106,10 +11670,10 @@
         <v>1</v>
       </c>
       <c r="O61" s="43">
-        <v>0.11</v>
+        <v>0.04</v>
       </c>
       <c r="P61">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="Q61">
         <v>0.05</v>
@@ -10162,10 +11726,10 @@
         <v>1</v>
       </c>
       <c r="O62" s="43">
-        <v>0.11</v>
+        <v>0.04</v>
       </c>
       <c r="P62">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="Q62">
         <v>0.05</v>
@@ -10218,10 +11782,10 @@
         <v>1</v>
       </c>
       <c r="O63" s="43">
-        <v>0.11</v>
+        <v>0.04</v>
       </c>
       <c r="P63">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="Q63">
         <v>0.05</v>
@@ -10232,6 +11796,7 @@
     </row>
     <row r="64" spans="1:18">
       <c r="A64" s="59"/>
+      <c r="O64" s="43"/>
     </row>
     <row r="65" spans="1:18">
       <c r="A65" s="59" t="s">
@@ -10277,10 +11842,10 @@
         <v>1</v>
       </c>
       <c r="O65" s="43">
-        <v>0.11</v>
+        <v>0.04</v>
       </c>
       <c r="P65">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="Q65">
         <v>0.05</v>
@@ -10333,10 +11898,10 @@
         <v>1</v>
       </c>
       <c r="O66" s="43">
-        <v>0.11</v>
+        <v>0.04</v>
       </c>
       <c r="P66">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="Q66">
         <v>0.05</v>
@@ -10389,10 +11954,10 @@
         <v>1</v>
       </c>
       <c r="O67" s="43">
-        <v>0.11</v>
+        <v>0.04</v>
       </c>
       <c r="P67">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="Q67">
         <v>0.05</v>
@@ -10403,6 +11968,7 @@
     </row>
     <row r="68" spans="1:18">
       <c r="A68" s="59"/>
+      <c r="O68" s="43"/>
     </row>
     <row r="69" spans="1:18">
       <c r="A69" s="59" t="s">
@@ -10448,10 +12014,10 @@
         <v>1</v>
       </c>
       <c r="O69" s="43">
-        <v>0.11</v>
+        <v>0.04</v>
       </c>
       <c r="P69">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="Q69">
         <v>0.05</v>
@@ -10554,10 +12120,10 @@
         <v>1</v>
       </c>
       <c r="O73" s="43">
-        <v>0.11</v>
+        <v>0.04</v>
       </c>
       <c r="P73">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="Q73">
         <v>0.05</v>
@@ -10666,10 +12232,10 @@
         <v>1</v>
       </c>
       <c r="O76" s="43">
-        <v>0.11</v>
+        <v>0.04</v>
       </c>
       <c r="P76">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="Q76">
         <v>0.05</v>
@@ -10678,12 +12244,575 @@
         <v>0</v>
       </c>
     </row>
+    <row r="80" spans="1:18">
+      <c r="A80" s="59" t="s">
+        <v>402</v>
+      </c>
+      <c r="B80" t="s">
+        <v>403</v>
+      </c>
+      <c r="C80" t="b">
+        <v>0</v>
+      </c>
+      <c r="D80" t="s">
+        <v>70</v>
+      </c>
+      <c r="E80" t="s">
+        <v>422</v>
+      </c>
+      <c r="F80" t="s">
+        <v>68</v>
+      </c>
+      <c r="G80">
+        <v>2.75E-2</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+      <c r="I80" t="b">
+        <v>1</v>
+      </c>
+      <c r="J80">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K80">
+        <v>0</v>
+      </c>
+      <c r="L80">
+        <v>2018</v>
+      </c>
+      <c r="N80" t="b">
+        <v>1</v>
+      </c>
+      <c r="O80" s="43">
+        <v>0.04</v>
+      </c>
+      <c r="P80">
+        <v>0</v>
+      </c>
+      <c r="Q80">
+        <v>0.05</v>
+      </c>
+      <c r="R80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18">
+      <c r="A81" s="59" t="s">
+        <v>404</v>
+      </c>
+      <c r="B81" t="s">
+        <v>405</v>
+      </c>
+      <c r="C81" t="b">
+        <v>0</v>
+      </c>
+      <c r="D81" t="s">
+        <v>70</v>
+      </c>
+      <c r="E81" t="s">
+        <v>422</v>
+      </c>
+      <c r="F81" t="s">
+        <v>68</v>
+      </c>
+      <c r="G81">
+        <v>2.75E-2</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81" t="b">
+        <v>1</v>
+      </c>
+      <c r="J81">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K81">
+        <v>0.25</v>
+      </c>
+      <c r="L81">
+        <v>2018</v>
+      </c>
+      <c r="N81" t="b">
+        <v>1</v>
+      </c>
+      <c r="O81" s="43">
+        <v>0.04</v>
+      </c>
+      <c r="P81">
+        <v>0</v>
+      </c>
+      <c r="Q81">
+        <v>0.05</v>
+      </c>
+      <c r="R81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18">
+      <c r="A82" s="59" t="s">
+        <v>406</v>
+      </c>
+      <c r="B82" t="s">
+        <v>407</v>
+      </c>
+      <c r="C82" t="b">
+        <v>0</v>
+      </c>
+      <c r="D82" t="s">
+        <v>70</v>
+      </c>
+      <c r="E82" t="s">
+        <v>422</v>
+      </c>
+      <c r="F82" t="s">
+        <v>68</v>
+      </c>
+      <c r="G82">
+        <v>2.75E-2</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82" t="b">
+        <v>1</v>
+      </c>
+      <c r="J82">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K82">
+        <v>0.5</v>
+      </c>
+      <c r="L82">
+        <v>2018</v>
+      </c>
+      <c r="N82" t="b">
+        <v>1</v>
+      </c>
+      <c r="O82" s="43">
+        <v>0.04</v>
+      </c>
+      <c r="P82">
+        <v>0</v>
+      </c>
+      <c r="Q82">
+        <v>0.05</v>
+      </c>
+      <c r="R82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18">
+      <c r="A83" s="59"/>
+      <c r="O83" s="43"/>
+    </row>
+    <row r="84" spans="1:18">
+      <c r="A84" s="59" t="s">
+        <v>408</v>
+      </c>
+      <c r="B84" t="s">
+        <v>409</v>
+      </c>
+      <c r="C84" t="b">
+        <v>0</v>
+      </c>
+      <c r="D84" t="s">
+        <v>70</v>
+      </c>
+      <c r="E84" t="s">
+        <v>422</v>
+      </c>
+      <c r="F84" t="s">
+        <v>68</v>
+      </c>
+      <c r="G84">
+        <v>2.75E-2</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
+      </c>
+      <c r="I84" t="b">
+        <v>1</v>
+      </c>
+      <c r="J84">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K84">
+        <v>0</v>
+      </c>
+      <c r="L84">
+        <v>2018</v>
+      </c>
+      <c r="M84">
+        <v>0.01</v>
+      </c>
+      <c r="N84" t="b">
+        <v>1</v>
+      </c>
+      <c r="O84" s="43">
+        <v>0.04</v>
+      </c>
+      <c r="P84">
+        <v>0</v>
+      </c>
+      <c r="Q84">
+        <v>0.05</v>
+      </c>
+      <c r="R84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18">
+      <c r="A85" s="59" t="s">
+        <v>410</v>
+      </c>
+      <c r="B85" t="s">
+        <v>411</v>
+      </c>
+      <c r="C85" t="b">
+        <v>0</v>
+      </c>
+      <c r="D85" t="s">
+        <v>70</v>
+      </c>
+      <c r="E85" t="s">
+        <v>422</v>
+      </c>
+      <c r="F85" t="s">
+        <v>68</v>
+      </c>
+      <c r="G85">
+        <v>2.75E-2</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+      <c r="I85" t="b">
+        <v>1</v>
+      </c>
+      <c r="J85">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K85">
+        <v>0.25</v>
+      </c>
+      <c r="L85">
+        <v>2018</v>
+      </c>
+      <c r="M85">
+        <v>0.01</v>
+      </c>
+      <c r="N85" t="b">
+        <v>1</v>
+      </c>
+      <c r="O85" s="43">
+        <v>0.04</v>
+      </c>
+      <c r="P85">
+        <v>0</v>
+      </c>
+      <c r="Q85">
+        <v>0.05</v>
+      </c>
+      <c r="R85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18">
+      <c r="A86" s="59" t="s">
+        <v>412</v>
+      </c>
+      <c r="B86" t="s">
+        <v>413</v>
+      </c>
+      <c r="C86" t="b">
+        <v>0</v>
+      </c>
+      <c r="D86" t="s">
+        <v>70</v>
+      </c>
+      <c r="E86" t="s">
+        <v>422</v>
+      </c>
+      <c r="F86" t="s">
+        <v>68</v>
+      </c>
+      <c r="G86">
+        <v>2.75E-2</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+      <c r="I86" t="b">
+        <v>1</v>
+      </c>
+      <c r="J86">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K86">
+        <v>0.5</v>
+      </c>
+      <c r="L86">
+        <v>2018</v>
+      </c>
+      <c r="M86">
+        <v>0.01</v>
+      </c>
+      <c r="N86" t="b">
+        <v>1</v>
+      </c>
+      <c r="O86" s="43">
+        <v>0.04</v>
+      </c>
+      <c r="P86">
+        <v>0</v>
+      </c>
+      <c r="Q86">
+        <v>0.05</v>
+      </c>
+      <c r="R86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18">
+      <c r="A87" s="59"/>
+      <c r="O87" s="43"/>
+    </row>
+    <row r="88" spans="1:18">
+      <c r="A88" s="59" t="s">
+        <v>414</v>
+      </c>
+      <c r="B88" t="s">
+        <v>415</v>
+      </c>
+      <c r="C88" t="b">
+        <v>0</v>
+      </c>
+      <c r="D88" t="s">
+        <v>70</v>
+      </c>
+      <c r="E88" t="s">
+        <v>422</v>
+      </c>
+      <c r="F88" t="s">
+        <v>68</v>
+      </c>
+      <c r="G88">
+        <v>2.75E-2</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88" t="b">
+        <v>1</v>
+      </c>
+      <c r="J88">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K88">
+        <v>0</v>
+      </c>
+      <c r="L88">
+        <v>2018</v>
+      </c>
+      <c r="M88">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="N88" t="b">
+        <v>1</v>
+      </c>
+      <c r="O88" s="43">
+        <v>0.04</v>
+      </c>
+      <c r="P88">
+        <v>0</v>
+      </c>
+      <c r="Q88">
+        <v>0.05</v>
+      </c>
+      <c r="R88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18">
+      <c r="A89" s="59" t="s">
+        <v>416</v>
+      </c>
+      <c r="B89" t="s">
+        <v>417</v>
+      </c>
+      <c r="C89" t="b">
+        <v>0</v>
+      </c>
+      <c r="D89" t="s">
+        <v>70</v>
+      </c>
+      <c r="E89" t="s">
+        <v>422</v>
+      </c>
+      <c r="F89" t="s">
+        <v>68</v>
+      </c>
+      <c r="G89">
+        <v>2.75E-2</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+      <c r="I89" t="b">
+        <v>1</v>
+      </c>
+      <c r="J89">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K89">
+        <v>0.25</v>
+      </c>
+      <c r="L89">
+        <v>2018</v>
+      </c>
+      <c r="M89">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="N89" t="b">
+        <v>1</v>
+      </c>
+      <c r="O89" s="43">
+        <v>0.04</v>
+      </c>
+      <c r="P89">
+        <v>0</v>
+      </c>
+      <c r="Q89">
+        <v>0.05</v>
+      </c>
+      <c r="R89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18">
+      <c r="A90" s="59" t="s">
+        <v>418</v>
+      </c>
+      <c r="B90" t="s">
+        <v>419</v>
+      </c>
+      <c r="C90" t="b">
+        <v>0</v>
+      </c>
+      <c r="D90" t="s">
+        <v>70</v>
+      </c>
+      <c r="E90" t="s">
+        <v>422</v>
+      </c>
+      <c r="F90" t="s">
+        <v>68</v>
+      </c>
+      <c r="G90">
+        <v>2.75E-2</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+      <c r="I90" t="b">
+        <v>1</v>
+      </c>
+      <c r="J90">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K90">
+        <v>0.5</v>
+      </c>
+      <c r="L90">
+        <v>2018</v>
+      </c>
+      <c r="M90">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="N90" t="b">
+        <v>1</v>
+      </c>
+      <c r="O90" s="43">
+        <v>0.04</v>
+      </c>
+      <c r="P90">
+        <v>0</v>
+      </c>
+      <c r="Q90">
+        <v>0.05</v>
+      </c>
+      <c r="R90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18">
+      <c r="A91" s="59"/>
+      <c r="O91" s="43"/>
+    </row>
+    <row r="92" spans="1:18">
+      <c r="A92" s="59" t="s">
+        <v>420</v>
+      </c>
+      <c r="B92" t="s">
+        <v>421</v>
+      </c>
+      <c r="C92" t="b">
+        <v>0</v>
+      </c>
+      <c r="D92" t="s">
+        <v>70</v>
+      </c>
+      <c r="E92" t="s">
+        <v>422</v>
+      </c>
+      <c r="F92" t="s">
+        <v>68</v>
+      </c>
+      <c r="G92">
+        <v>2.75E-2</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+      <c r="I92" t="b">
+        <v>1</v>
+      </c>
+      <c r="J92">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K92">
+        <v>0</v>
+      </c>
+      <c r="L92">
+        <v>2018</v>
+      </c>
+      <c r="M92">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N92" t="b">
+        <v>1</v>
+      </c>
+      <c r="O92" s="43">
+        <v>0.04</v>
+      </c>
+      <c r="P92">
+        <v>0</v>
+      </c>
+      <c r="Q92">
+        <v>0.05</v>
+      </c>
+      <c r="R92">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C33:C37 C5:C31 C42:C52 C54:C55 C72:C76 C57:C69" xr:uid="{CE4DB086-8939-4E0F-A217-D1528E507A37}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C33:C37 C5:C31 C42:C92" xr:uid="{CE4DB086-8939-4E0F-A217-D1528E507A37}">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D24:D26 D5:D9 D11:D13 D28:D31 D20:D22 D15:D17 D33:D34 D36:D37 D42:D44 D46:D48 D50:D52 D61:D63 D65:D67 D57:D59 D72:D73 D75:D76 D54:D55 D69" xr:uid="{B6635BCF-58EB-45FF-9851-3E5464D67D97}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D24:D26 D5:D9 D11:D13 D28:D31 D20:D22 D15:D17 D33:D34 D36:D37 D42:D44 D46:D48 D50:D52 D61:D63 D65:D67 D57:D59 D72:D73 D75:D76 D54:D55 D69 D84:D86 D88:D90 D80:D82 D92" xr:uid="{B6635BCF-58EB-45FF-9851-3E5464D67D97}">
       <formula1>"singleTier,multiTier"</formula1>
     </dataValidation>
   </dataValidations>
@@ -10698,7 +12827,7 @@
   <dimension ref="A2:AR74"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="AG35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="B67" sqref="B67:B68"/>
@@ -15927,7 +18056,7 @@
   <dimension ref="A3:R41"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="K5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="C46" sqref="C46"/>
@@ -17442,7 +19571,7 @@
   <dimension ref="A3:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17833,13 +19962,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD963C7-C30C-4F41-9ED1-A3A9BFD95FFA}">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M22" sqref="M22"/>
+      <selection pane="bottomRight" activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -18440,358 +20569,397 @@
         <v>4442513264</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="25.5">
-      <c r="A27" s="33" t="s">
+    <row r="26" spans="1:11" ht="15" customHeight="1">
+      <c r="A26" s="33" t="s">
+        <v>438</v>
+      </c>
+      <c r="B26" s="27">
+        <f>B24+B25</f>
+        <v>4006671712</v>
+      </c>
+      <c r="C26" s="27">
+        <f t="shared" ref="C26:K26" si="6">C24+C25</f>
+        <v>153724045</v>
+      </c>
+      <c r="D26" s="27">
+        <f t="shared" si="6"/>
+        <v>4160395757</v>
+      </c>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27">
+        <f t="shared" si="6"/>
+        <v>526375464</v>
+      </c>
+      <c r="G26" s="27">
+        <f t="shared" si="6"/>
+        <v>1755305847</v>
+      </c>
+      <c r="H26" s="27">
+        <f t="shared" si="6"/>
+        <v>532103328</v>
+      </c>
+      <c r="I26" s="27">
+        <f t="shared" si="6"/>
+        <v>2813784639</v>
+      </c>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27">
+        <f t="shared" si="6"/>
+        <v>6974180396</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="25.5">
+      <c r="A28" s="33" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="30" t="s">
+    <row r="29" spans="1:11">
+      <c r="A29" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="B28" s="34">
+      <c r="B29" s="34">
         <v>0.16813</v>
       </c>
-      <c r="C28" s="37">
+      <c r="C29" s="37">
         <v>0.18260999999999999</v>
       </c>
-      <c r="D28" s="36">
+      <c r="D29" s="36">
         <f>D22/$D$12</f>
         <v>0.16890904798938361</v>
       </c>
-      <c r="F28" s="53">
+      <c r="F29" s="53">
         <v>0.23186000000000001</v>
       </c>
-      <c r="G28" s="53">
+      <c r="G29" s="53">
         <v>0.29893999999999998</v>
       </c>
-      <c r="H28" s="53">
+      <c r="H29" s="53">
         <v>0.29848000000000002</v>
       </c>
-      <c r="I28" s="36">
+      <c r="I29" s="36">
         <f>I22/$I$12</f>
         <v>0.27572819053794789</v>
       </c>
-      <c r="K28" s="36">
+      <c r="K29" s="36">
         <f>K22/$K$12</f>
         <v>0.20536748675571453</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
-      <c r="A29" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="B29" s="34">
-        <v>6.905E-2</v>
-      </c>
-      <c r="C29" s="37">
-        <v>7.9689999999999997E-2</v>
-      </c>
-      <c r="D29" s="36">
-        <f t="shared" ref="D29:D31" si="6">D23/$D$12</f>
-        <v>6.9626262709777217E-2</v>
-      </c>
-      <c r="F29" s="53">
-        <v>0.10485</v>
-      </c>
-      <c r="G29" s="53">
-        <v>0.11456</v>
-      </c>
-      <c r="H29" s="53">
-        <v>0.10523</v>
-      </c>
-      <c r="I29" s="36">
-        <f t="shared" ref="I29:I31" si="7">I23/$I$12</f>
-        <v>0.10999646669803917</v>
-      </c>
-      <c r="K29" s="36">
-        <f t="shared" ref="K29:K31" si="8">K23/$K$12</f>
-        <v>8.3405015983528522E-2</v>
-      </c>
-    </row>
     <row r="30" spans="1:11">
       <c r="A30" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" s="34">
+        <v>6.905E-2</v>
+      </c>
+      <c r="C30" s="37">
+        <v>7.9689999999999997E-2</v>
+      </c>
+      <c r="D30" s="36">
+        <f t="shared" ref="D30:D32" si="7">D23/$D$12</f>
+        <v>6.9626262709777217E-2</v>
+      </c>
+      <c r="F30" s="53">
+        <v>0.10485</v>
+      </c>
+      <c r="G30" s="53">
+        <v>0.11456</v>
+      </c>
+      <c r="H30" s="53">
+        <v>0.10523</v>
+      </c>
+      <c r="I30" s="36">
+        <f t="shared" ref="I30:I32" si="8">I23/$I$12</f>
+        <v>0.10999646669803917</v>
+      </c>
+      <c r="K30" s="36">
+        <f t="shared" ref="K30:K32" si="9">K23/$K$12</f>
+        <v>8.3405015983528522E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="B30" s="34">
+      <c r="B31" s="34">
         <v>9.9080000000000001E-2</v>
       </c>
-      <c r="C30" s="37">
+      <c r="C31" s="37">
         <v>0.10292</v>
       </c>
-      <c r="D30" s="36">
-        <f t="shared" si="6"/>
+      <c r="D31" s="36">
+        <f t="shared" si="7"/>
         <v>9.9282785279606378E-2</v>
       </c>
-      <c r="F30" s="53">
+      <c r="F31" s="53">
         <v>0.12701000000000001</v>
       </c>
-      <c r="G30" s="53">
+      <c r="G31" s="53">
         <v>0.18437999999999999</v>
       </c>
-      <c r="H30" s="53">
+      <c r="H31" s="53">
         <v>0.19325000000000001</v>
       </c>
-      <c r="I30" s="36">
+      <c r="I31" s="36">
+        <f t="shared" si="8"/>
+        <v>0.1657317238399087</v>
+      </c>
+      <c r="K31" s="36">
+        <f t="shared" si="9"/>
+        <v>0.12196247077218601</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="15" customHeight="1">
+      <c r="A32" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32" s="34">
+        <v>0.21068999999999999</v>
+      </c>
+      <c r="C32" s="37">
+        <v>0.10531</v>
+      </c>
+      <c r="D32" s="36">
         <f t="shared" si="7"/>
-        <v>0.1657317238399087</v>
-      </c>
-      <c r="K30" s="36">
+        <v>0.20499704691565238</v>
+      </c>
+      <c r="F32" s="53">
+        <v>8.8249999999999995E-2</v>
+      </c>
+      <c r="G32" s="53">
+        <v>0.28760000000000002</v>
+      </c>
+      <c r="H32" s="53">
+        <v>0.38479999999999998</v>
+      </c>
+      <c r="I32" s="36">
         <f t="shared" si="8"/>
-        <v>0.12196247077218601</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="15" customHeight="1">
-      <c r="A31" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="B31" s="34">
-        <v>0.21068999999999999</v>
-      </c>
-      <c r="C31" s="37">
-        <v>0.10531</v>
-      </c>
-      <c r="D31" s="36">
-        <f t="shared" si="6"/>
-        <v>0.20499704691565238</v>
-      </c>
-      <c r="F31" s="53">
-        <v>8.8249999999999995E-2</v>
-      </c>
-      <c r="G31" s="53">
-        <v>0.28760000000000002</v>
-      </c>
-      <c r="H31" s="53">
-        <v>0.38479999999999998</v>
-      </c>
-      <c r="I31" s="36">
-        <f t="shared" si="7"/>
         <v>0.23142460290287567</v>
       </c>
-      <c r="K31" s="36">
-        <f t="shared" si="8"/>
+      <c r="K32" s="36">
+        <f t="shared" si="9"/>
         <v>0.21401703536262867</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
-      <c r="A32" s="30" t="s">
+    <row r="33" spans="1:11">
+      <c r="A33" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="B32" s="35">
+      <c r="B33" s="35">
         <v>0.30976999999999999</v>
       </c>
-      <c r="C32" s="37">
+      <c r="C33" s="37">
         <v>0.20823</v>
       </c>
-      <c r="D32" s="36">
+      <c r="D33" s="36">
         <f>SUM(D24:D25)/D12</f>
         <v>0.30427983219525878</v>
       </c>
-      <c r="F32" s="54">
+      <c r="F33" s="54">
         <v>0.21526000000000001</v>
       </c>
-      <c r="G32" s="54">
+      <c r="G33" s="54">
         <v>0.47198000000000001</v>
       </c>
-      <c r="H32" s="54">
+      <c r="H33" s="54">
         <v>0.57811000000000001</v>
       </c>
-      <c r="I32" s="36">
+      <c r="I33" s="36">
         <f>SUM(I24:I25)/$I$12</f>
         <v>0.39715632674278439</v>
       </c>
-      <c r="K32" s="36">
+      <c r="K33" s="36">
         <f>SUM(K24:K25)/$K$12</f>
         <v>0.3359795061348147</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="25.5">
-      <c r="A34" s="33" t="s">
+    <row r="35" spans="1:11" ht="25.5">
+      <c r="A35" s="33" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
-      <c r="A35" s="30" t="s">
+    <row r="36" spans="1:11">
+      <c r="A36" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="B35" s="36">
+      <c r="B36" s="36">
         <f>B22/B$11</f>
         <v>0.17750120825953289</v>
       </c>
-      <c r="C35" s="36">
+      <c r="C36" s="36">
         <f>C22/C$11</f>
         <v>0.19279164833323059</v>
       </c>
-      <c r="D35" s="36">
+      <c r="D36" s="36">
         <f>D22/D$11</f>
         <v>0.1783267830917612</v>
       </c>
-      <c r="F35" s="36">
+      <c r="F36" s="36">
         <f>F22/F$11</f>
         <v>0.24478764414551246</v>
       </c>
-      <c r="G35" s="36">
+      <c r="G36" s="36">
         <f>G22/G$11</f>
         <v>0.31560777337278823</v>
       </c>
-      <c r="H35" s="36">
+      <c r="H36" s="36">
         <f>H22/H$11</f>
         <v>0.31512212579521937</v>
       </c>
-      <c r="I35" s="36">
+      <c r="I36" s="36">
         <f>I22/I$11</f>
         <v>0.29110176047618991</v>
       </c>
-      <c r="K35" s="36">
+      <c r="K36" s="36">
         <f>K22/K$11</f>
         <v>0.21681800768917101</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
-      <c r="A36" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="B36" s="36">
-        <f t="shared" ref="B36:C38" si="9">B23/B$11</f>
-        <v>7.2901953892441071E-2</v>
-      </c>
-      <c r="C36" s="36">
-        <f t="shared" si="9"/>
-        <v>8.4133215728005153E-2</v>
-      </c>
-      <c r="D36" s="36">
-        <f t="shared" ref="D36:F36" si="10">D23/D$11</f>
-        <v>7.3508362018101112E-2</v>
-      </c>
-      <c r="F36" s="36">
-        <f t="shared" si="10"/>
-        <v>0.110696043016053</v>
-      </c>
-      <c r="G36" s="36">
-        <f t="shared" ref="G36:H36" si="11">G23/G$11</f>
-        <v>0.12094743606951874</v>
-      </c>
-      <c r="H36" s="36">
-        <f t="shared" si="11"/>
-        <v>0.11109723023670871</v>
-      </c>
-      <c r="I36" s="36">
-        <f t="shared" ref="I36:K36" si="12">I23/I$11</f>
-        <v>0.11612945720018038</v>
-      </c>
-      <c r="K36" s="36">
-        <f t="shared" si="12"/>
-        <v>8.8055366905973612E-2</v>
-      </c>
-    </row>
     <row r="37" spans="1:11">
       <c r="A37" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B37" s="36">
-        <f t="shared" si="9"/>
-        <v>0.1045992543670918</v>
+        <f t="shared" ref="B37:C39" si="10">B23/B$11</f>
+        <v>7.2901953892441071E-2</v>
       </c>
       <c r="C37" s="36">
-        <f t="shared" si="9"/>
-        <v>0.10865843260522542</v>
+        <f t="shared" si="10"/>
+        <v>8.4133215728005153E-2</v>
       </c>
       <c r="D37" s="36">
-        <f t="shared" ref="D37:F37" si="13">D24/D$11</f>
-        <v>0.10481842107366009</v>
+        <f t="shared" ref="D37:F37" si="11">D23/D$11</f>
+        <v>7.3508362018101112E-2</v>
       </c>
       <c r="F37" s="36">
+        <f t="shared" si="11"/>
+        <v>0.110696043016053</v>
+      </c>
+      <c r="G37" s="36">
+        <f t="shared" ref="G37:H37" si="12">G23/G$11</f>
+        <v>0.12094743606951874</v>
+      </c>
+      <c r="H37" s="36">
+        <f t="shared" si="12"/>
+        <v>0.11109723023670871</v>
+      </c>
+      <c r="I37" s="36">
+        <f t="shared" ref="I37:K37" si="13">I23/I$11</f>
+        <v>0.11612945720018038</v>
+      </c>
+      <c r="K37" s="36">
         <f t="shared" si="13"/>
-        <v>0.13409160112945948</v>
-      </c>
-      <c r="G37" s="36">
-        <f t="shared" ref="G37:H37" si="14">G24/G$11</f>
-        <v>0.19466033730326945</v>
-      </c>
-      <c r="H37" s="36">
-        <f t="shared" si="14"/>
-        <v>0.20402489555851064</v>
-      </c>
-      <c r="I37" s="36">
-        <f t="shared" ref="I37:K37" si="15">I24/I$11</f>
-        <v>0.17497230327600952</v>
-      </c>
-      <c r="K37" s="36">
-        <f t="shared" si="15"/>
-        <v>0.12876264078319741</v>
+        <v>8.8055366905973612E-2</v>
       </c>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B38" s="36">
-        <f t="shared" si="9"/>
-        <v>0.222433714666711</v>
+        <f t="shared" si="10"/>
+        <v>0.1045992543670918</v>
       </c>
       <c r="C38" s="36">
-        <f t="shared" si="9"/>
-        <v>0.11118197881078788</v>
+        <f t="shared" si="10"/>
+        <v>0.10865843260522542</v>
       </c>
       <c r="D38" s="36">
-        <f t="shared" ref="D38:F38" si="16">D25/D$11</f>
-        <v>0.21642691350718413</v>
+        <f t="shared" ref="D38:F38" si="14">D24/D$11</f>
+        <v>0.10481842107366009</v>
       </c>
       <c r="F38" s="36">
+        <f t="shared" si="14"/>
+        <v>0.13409160112945948</v>
+      </c>
+      <c r="G38" s="36">
+        <f t="shared" ref="G38:H38" si="15">G24/G$11</f>
+        <v>0.19466033730326945</v>
+      </c>
+      <c r="H38" s="36">
+        <f t="shared" si="15"/>
+        <v>0.20402489555851064</v>
+      </c>
+      <c r="I38" s="36">
+        <f t="shared" ref="I38:K38" si="16">I24/I$11</f>
+        <v>0.17497230327600952</v>
+      </c>
+      <c r="K38" s="36">
         <f t="shared" si="16"/>
-        <v>9.3173975543692972E-2</v>
-      </c>
-      <c r="G38" s="36">
-        <f t="shared" ref="G38:H38" si="17">G25/G$11</f>
-        <v>0.30363134916273504</v>
-      </c>
-      <c r="H38" s="36">
-        <f t="shared" si="17"/>
-        <v>0.40625874427848757</v>
-      </c>
-      <c r="I38" s="36">
-        <f t="shared" ref="I38:K38" si="18">I25/I$11</f>
-        <v>0.24432797093070013</v>
-      </c>
-      <c r="K38" s="36">
-        <f t="shared" si="18"/>
-        <v>0.22594982269060079</v>
+        <v>0.12876264078319741</v>
       </c>
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="B39" s="36">
+        <f t="shared" si="10"/>
+        <v>0.222433714666711</v>
+      </c>
+      <c r="C39" s="36">
+        <f t="shared" si="10"/>
+        <v>0.11118197881078788</v>
+      </c>
+      <c r="D39" s="36">
+        <f t="shared" ref="D39:F39" si="17">D25/D$11</f>
+        <v>0.21642691350718413</v>
+      </c>
+      <c r="F39" s="36">
+        <f t="shared" si="17"/>
+        <v>9.3173975543692972E-2</v>
+      </c>
+      <c r="G39" s="36">
+        <f t="shared" ref="G39:H39" si="18">G25/G$11</f>
+        <v>0.30363134916273504</v>
+      </c>
+      <c r="H39" s="36">
+        <f t="shared" si="18"/>
+        <v>0.40625874427848757</v>
+      </c>
+      <c r="I39" s="36">
+        <f t="shared" ref="I39:K39" si="19">I25/I$11</f>
+        <v>0.24432797093070013</v>
+      </c>
+      <c r="K39" s="36">
+        <f t="shared" si="19"/>
+        <v>0.22594982269060079</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="B39" s="36">
+      <c r="B40" s="36">
         <f>SUM(B24:B25)/B$11</f>
         <v>0.3270329690338028</v>
       </c>
-      <c r="C39" s="36">
-        <f t="shared" ref="C39:D39" si="19">SUM(C24:C25)/C$11</f>
+      <c r="C40" s="36">
+        <f t="shared" ref="C40:D40" si="20">SUM(C24:C25)/C$11</f>
         <v>0.21984041141601332</v>
       </c>
-      <c r="D39" s="36">
-        <f t="shared" si="19"/>
+      <c r="D40" s="36">
+        <f t="shared" si="20"/>
         <v>0.3212453345808442</v>
       </c>
-      <c r="F39" s="36">
-        <f t="shared" ref="F39:G39" si="20">SUM(F24:F25)/F$11</f>
+      <c r="F40" s="36">
+        <f t="shared" ref="F40:G40" si="21">SUM(F24:F25)/F$11</f>
         <v>0.22726557667315242</v>
       </c>
-      <c r="G39" s="36">
-        <f t="shared" si="20"/>
+      <c r="G40" s="36">
+        <f t="shared" si="21"/>
         <v>0.49829168646600452</v>
       </c>
-      <c r="H39" s="36">
-        <f t="shared" ref="H39:I39" si="21">SUM(H24:H25)/H$11</f>
+      <c r="H40" s="36">
+        <f t="shared" ref="H40:I40" si="22">SUM(H24:H25)/H$11</f>
         <v>0.61028363983699829</v>
       </c>
-      <c r="I39" s="36">
-        <f t="shared" si="21"/>
+      <c r="I40" s="36">
+        <f t="shared" si="22"/>
         <v>0.41930027420670968</v>
       </c>
-      <c r="K39" s="36">
-        <f t="shared" ref="K39" si="22">SUM(K24:K25)/K$11</f>
+      <c r="K40" s="36">
+        <f t="shared" ref="K40" si="23">SUM(K24:K25)/K$11</f>
         <v>0.3547124634737982</v>
       </c>
     </row>

</xml_diff>

<commit_message>
clean up and modify gitignore
</commit_message>
<xml_diff>
--- a/model/RunControl.xlsx
+++ b/model/RunControl.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89335A70-8DC4-4AF0-BC9D-8DF14CAA4CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EF91F8-3E64-4100-B1F1-373789A30DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,6 +82,57 @@
     the DR used in determining COLA. Leave blank (NA when loaded) if the DR for regular valuation is used.</t>
       </text>
     </comment>
+    <comment ref="P4" authorId="0" shapeId="0" xr:uid="{7507BEC7-0732-453E-A152-9197089D86E4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+cd: constant dollar
+cp: constant percent
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q4" authorId="0" shapeId="0" xr:uid="{7C262F51-2478-4278-9CDC-7FF127FA8A2A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+closed or open
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="S4" authorId="3" shapeId="0" xr:uid="{8515E407-C037-4E97-A4C6-62FC0108B1A6}">
       <text>
         <t>[Threaded comment]
@@ -110,8 +161,59 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
+method1: Use asset smoothing
 method2 = No smoothing
 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y4" authorId="0" shapeId="0" xr:uid="{70C751E0-23F2-4E85-8FBA-B7495846EA2F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+simple: use parameters in the "params_sim" tab
+internal: use parameters in the "returns" tab</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AF4" authorId="0" shapeId="0" xr:uid="{59FEBCFF-A785-436D-9457-5FEF996127AD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+MA_pct: percentage of initial AL, percentage given by MA_0_pct
+AA0: dollar value given by MA_0</t>
         </r>
       </text>
     </comment>
@@ -135,7 +237,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-AL_pct; AA0, noSmoothing</t>
+AL_pct: percentage of initial AL, percentage given by AA_0_pct
+AA0: dollar value given by AA_0</t>
         </r>
       </text>
     </comment>
@@ -1232,7 +1335,7 @@
     <numFmt numFmtId="168" formatCode="0.000%"/>
     <numFmt numFmtId="169" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1340,6 +1443,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1911,10 +2027,10 @@
   <dimension ref="A2:AS91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="X5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C94" sqref="C94"/>
+      <selection pane="bottomRight" activeCell="AI14" sqref="AI14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -8474,10 +8590,10 @@
   <dimension ref="A3:R51"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="F14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
+      <selection pane="bottomRight" activeCell="O58" sqref="O58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -10310,7 +10426,7 @@
   <dimension ref="A3:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -10394,7 +10510,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>